<commit_message>
Redraw vaccine uptake figure
</commit_message>
<xml_diff>
--- a/docs/tabs/Tab_ProgrammeProfile.xlsx
+++ b/docs/tabs/Tab_ProgrammeProfile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\HPRU\Shingrix\HPRU_RZV\docs\tabs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HPRU_Shingrix\docs\tabs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D22B84E1-58AE-43FA-B63F-E397D47F0B42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BAAE397-564B-46FE-9CE8-AB5062D85D50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="34605" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="51">
   <si>
     <t>Eligibility</t>
   </si>
@@ -222,6 +222,9 @@
   </si>
   <si>
     <t>Saved medical cost</t>
+  </si>
+  <si>
+    <t>Marginal threshold price per administration</t>
   </si>
 </sst>
 </file>
@@ -295,12 +298,6 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -310,8 +307,14 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -596,10 +599,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AD26"/>
+  <dimension ref="A1:AD29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:L1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -632,24 +635,27 @@
       <c r="D1" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="17"/>
-      <c r="G1" s="16" t="s">
+      <c r="F1" s="16"/>
+      <c r="G1" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16" t="s">
+      <c r="H1" s="14"/>
+      <c r="I1" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="J1" s="16"/>
-      <c r="K1" s="15" t="s">
+      <c r="J1" s="14"/>
+      <c r="K1" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="L1" s="15"/>
+      <c r="L1" s="13"/>
       <c r="M1" s="6" t="s">
         <v>41</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:30" s="1" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -686,6 +692,9 @@
       <c r="M2" s="6" t="s">
         <v>42</v>
       </c>
+      <c r="N2" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="Q2" s="1" t="s">
         <v>0</v>
       </c>
@@ -743,43 +752,47 @@
       </c>
       <c r="D3" s="9">
         <f t="shared" ref="D3:E3" si="0">U3 / 1000</f>
-        <v>2965.5050000000001</v>
+        <v>640.87300000000005</v>
       </c>
       <c r="E3" s="3">
         <f t="shared" si="0"/>
-        <v>624.54221633449197</v>
+        <v>308.98772385586199</v>
       </c>
       <c r="F3" s="5">
         <f>AA3</f>
-        <v>0.67144604554687604</v>
+        <v>0.50275377571315005</v>
       </c>
       <c r="G3" s="9">
         <f>W3 / 1000</f>
-        <v>1249.0844326689801</v>
+        <v>617.97544771172397</v>
       </c>
       <c r="H3" s="5">
         <f>AB3</f>
-        <v>0.67144604554687604</v>
+        <v>0.50275377571315005</v>
       </c>
       <c r="I3" s="9">
         <f>Y3</f>
-        <v>4065.0961132832399</v>
+        <v>1959.7805499829601</v>
       </c>
       <c r="J3" s="5">
         <f>AC3</f>
-        <v>0.65520802147552304</v>
+        <v>0.47811564488677299</v>
       </c>
       <c r="K3" s="7">
         <f>-X3/1000000</f>
-        <v>6.6142491241228996</v>
+        <v>3.10664610742537</v>
       </c>
       <c r="L3" s="5">
         <f>AD3</f>
-        <v>0.62021428993287597</v>
+        <v>0.43407980180762201</v>
       </c>
       <c r="M3" s="7">
         <f>Z3</f>
-        <v>70.384490503922706</v>
+        <v>68.452973760889407</v>
+      </c>
+      <c r="N3" s="7">
+        <f>(I3 * 20 + K3 * 1000) /G3</f>
+        <v>68.452973760889478</v>
       </c>
       <c r="Q3" t="s">
         <v>14</v>
@@ -794,34 +807,34 @@
         <v>2965505</v>
       </c>
       <c r="U3">
-        <v>2965505</v>
+        <v>640873</v>
       </c>
       <c r="V3">
-        <v>624542.21633449197</v>
+        <v>308987.72385586199</v>
       </c>
       <c r="W3">
-        <v>1249084.43266898</v>
+        <v>617975.44771172397</v>
       </c>
       <c r="X3">
-        <v>-6614249.1241229</v>
+        <v>-3106646.1074253698</v>
       </c>
       <c r="Y3">
-        <v>4065.0961132832399</v>
+        <v>1959.7805499829601</v>
       </c>
       <c r="Z3">
-        <v>70.384490503922706</v>
+        <v>68.452973760889407</v>
       </c>
       <c r="AA3">
-        <v>0.67144604554687604</v>
+        <v>0.50275377571315005</v>
       </c>
       <c r="AB3">
-        <v>0.67144604554687604</v>
+        <v>0.50275377571315005</v>
       </c>
       <c r="AC3">
-        <v>0.65520802147552304</v>
+        <v>0.47811564488677299</v>
       </c>
       <c r="AD3">
-        <v>0.62021428993287597</v>
+        <v>0.43407980180762201</v>
       </c>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.25">
@@ -846,7 +859,7 @@
       </c>
       <c r="F4" s="5">
         <f t="shared" ref="F4:F5" si="5">AA4</f>
-        <v>0.93078670524280505</v>
+        <v>0.89524993072826198</v>
       </c>
       <c r="G4" s="9">
         <f t="shared" ref="G4:G5" si="6">W4 / 1000</f>
@@ -854,7 +867,7 @@
       </c>
       <c r="H4" s="5">
         <f t="shared" ref="H4:H5" si="7">AB4</f>
-        <v>0.93078670524280505</v>
+        <v>0.89524993072826198</v>
       </c>
       <c r="I4" s="9">
         <f t="shared" ref="I4:I5" si="8">Y4</f>
@@ -862,7 +875,7 @@
       </c>
       <c r="J4" s="5">
         <f t="shared" ref="J4:J5" si="9">AC4</f>
-        <v>0.92775538100938104</v>
+        <v>0.89064903263216899</v>
       </c>
       <c r="K4" s="7">
         <f t="shared" ref="K4:K5" si="10">-X4/1000000</f>
@@ -870,11 +883,15 @@
       </c>
       <c r="L4" s="5">
         <f t="shared" ref="L4:L5" si="11">AD4</f>
-        <v>0.90858015982727502</v>
+        <v>0.86377493228978997</v>
       </c>
       <c r="M4" s="7">
         <f t="shared" ref="M4:M5" si="12">Z4</f>
-        <v>72.081003249813506</v>
+        <v>71.9692777218591</v>
+      </c>
+      <c r="N4" s="7">
+        <f t="shared" ref="N4:N26" si="13">(I4 * 20 + K4 * 1000) /G4</f>
+        <v>76.473360297813258</v>
       </c>
       <c r="Q4" t="s">
         <v>17</v>
@@ -904,19 +921,19 @@
         <v>1690.96100110564</v>
       </c>
       <c r="Z4">
-        <v>72.081003249813506</v>
+        <v>71.9692777218591</v>
       </c>
       <c r="AA4">
-        <v>0.93078670524280505</v>
+        <v>0.89524993072826198</v>
       </c>
       <c r="AB4">
-        <v>0.93078670524280505</v>
+        <v>0.89524993072826198</v>
       </c>
       <c r="AC4">
-        <v>0.92775538100938104</v>
+        <v>0.89064903263216899</v>
       </c>
       <c r="AD4">
-        <v>0.90858015982727502</v>
+        <v>0.86377493228978997</v>
       </c>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.25">
@@ -967,7 +984,11 @@
       </c>
       <c r="M5" s="7">
         <f t="shared" si="12"/>
-        <v>72.435004323883405</v>
+        <v>72.516739855052194</v>
+      </c>
+      <c r="N5" s="7">
+        <f t="shared" si="13"/>
+        <v>77.195643078934864</v>
       </c>
       <c r="Q5" t="s">
         <v>17</v>
@@ -997,7 +1018,7 @@
         <v>448.22607513721198</v>
       </c>
       <c r="Z5">
-        <v>72.435004323883405</v>
+        <v>72.516739855052194</v>
       </c>
       <c r="AA5">
         <v>1</v>
@@ -1015,33 +1036,35 @@
     <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B6" s="10"/>
       <c r="C6" s="11"/>
+      <c r="N6" s="7"/>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="14"/>
-      <c r="M7" s="14"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="12"/>
+      <c r="N7" s="7"/>
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="12" t="str">
+      <c r="B8" s="15" t="str">
         <f>R8</f>
         <v>[80,85)</v>
       </c>
-      <c r="C8" s="13">
+      <c r="C8" s="17">
         <f>T8/1000</f>
         <v>1508.4970000000001</v>
       </c>
@@ -1055,7 +1078,7 @@
       </c>
       <c r="F8" s="5">
         <f>AA8</f>
-        <v>1.15694237769202</v>
+        <v>1.23752264637281</v>
       </c>
       <c r="G8" s="9">
         <f>W8 / 1000</f>
@@ -1063,7 +1086,7 @@
       </c>
       <c r="H8" s="5">
         <f>AB8</f>
-        <v>1.0784711888460099</v>
+        <v>1.1187613231864</v>
       </c>
       <c r="I8" s="9">
         <f>Y8</f>
@@ -1071,7 +1094,7 @@
       </c>
       <c r="J8" s="5">
         <f>AC8</f>
-        <v>1.0892882836790301</v>
+        <v>1.1351486149602901</v>
       </c>
       <c r="K8" s="7">
         <f>-X8/1000000</f>
@@ -1079,11 +1102,15 @@
       </c>
       <c r="L8" s="5">
         <f>AD8</f>
-        <v>1.13417061199852</v>
+        <v>1.19992816296426</v>
       </c>
       <c r="M8" s="7">
         <f>Z8</f>
-        <v>73.400104353916802</v>
+        <v>73.916081346127996</v>
+      </c>
+      <c r="N8" s="7">
+        <f t="shared" si="13"/>
+        <v>85.698886164489963</v>
       </c>
       <c r="Q8" t="s">
         <v>20</v>
@@ -1113,38 +1140,38 @@
         <v>553.96979745149702</v>
       </c>
       <c r="Z8">
-        <v>73.400104353916802</v>
+        <v>73.916081346127996</v>
       </c>
       <c r="AA8">
-        <v>1.15694237769202</v>
+        <v>1.23752264637281</v>
       </c>
       <c r="AB8">
-        <v>1.0784711888460099</v>
+        <v>1.1187613231864</v>
       </c>
       <c r="AC8">
-        <v>1.0892882836790301</v>
+        <v>1.1351486149602901</v>
       </c>
       <c r="AD8">
-        <v>1.13417061199852</v>
+        <v>1.19992816296426</v>
       </c>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="12"/>
-      <c r="C9" s="13"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="17"/>
       <c r="D9" s="9">
-        <f t="shared" ref="D9:E12" si="13">U9/1000</f>
+        <f t="shared" ref="D9:E12" si="14">U9/1000</f>
         <v>433.09521756606995</v>
       </c>
       <c r="E9" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>58.790011311030398</v>
       </c>
       <c r="F9" s="5">
         <f>AA9</f>
-        <v>1.22014758557072</v>
+        <v>1.3331798452802599</v>
       </c>
       <c r="G9" s="9">
         <f>W9 / 1000</f>
@@ -1152,7 +1179,7 @@
       </c>
       <c r="H9" s="5">
         <f>AB9</f>
-        <v>1.1100737927853599</v>
+        <v>1.16658992264013</v>
       </c>
       <c r="I9" s="9">
         <f>Y9</f>
@@ -1160,7 +1187,7 @@
       </c>
       <c r="J9" s="5">
         <f>AC9</f>
-        <v>1.13728469403735</v>
+        <v>1.20779698623271</v>
       </c>
       <c r="K9" s="7">
         <f>-X9/1000000</f>
@@ -1168,11 +1195,15 @@
       </c>
       <c r="L9" s="5">
         <f>AD9</f>
-        <v>1.20778920057239</v>
+        <v>1.30962751481456</v>
       </c>
       <c r="M9" s="7">
         <f>Z9</f>
-        <v>74.574683610568698</v>
+        <v>75.5864610688146</v>
+      </c>
+      <c r="N9" s="7">
+        <f t="shared" si="13"/>
+        <v>114.65840233660472</v>
       </c>
       <c r="Q9" t="s">
         <v>23</v>
@@ -1202,44 +1233,44 @@
         <v>297.783321943685</v>
       </c>
       <c r="Z9">
-        <v>74.574683610568698</v>
+        <v>75.5864610688146</v>
       </c>
       <c r="AA9">
-        <v>1.22014758557072</v>
+        <v>1.3331798452802599</v>
       </c>
       <c r="AB9">
-        <v>1.1100737927853599</v>
+        <v>1.16658992264013</v>
       </c>
       <c r="AC9">
-        <v>1.13728469403735</v>
+        <v>1.20779698623271</v>
       </c>
       <c r="AD9">
-        <v>1.20778920057239</v>
+        <v>1.30962751481456</v>
       </c>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="12" t="str">
+      <c r="B10" s="15" t="str">
         <f>R10</f>
         <v>[85,90)</v>
       </c>
-      <c r="C10" s="13">
+      <c r="C10" s="17">
         <f>T10/1000</f>
         <v>940.56899999999996</v>
       </c>
       <c r="D10" s="9">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>344.41771727378898</v>
       </c>
       <c r="E10" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>46.752586205033197</v>
       </c>
       <c r="F10" s="5">
         <f>AA10</f>
-        <v>1.27041134405722</v>
+        <v>1.4092509556325299</v>
       </c>
       <c r="G10" s="9">
         <f>W10 / 1000</f>
@@ -1247,7 +1278,7 @@
       </c>
       <c r="H10" s="5">
         <f>AB10</f>
-        <v>1.1352056720286099</v>
+        <v>1.2046254778162599</v>
       </c>
       <c r="I10" s="9">
         <f>Y10</f>
@@ -1255,7 +1286,7 @@
       </c>
       <c r="J10" s="5">
         <f>AC10</f>
-        <v>1.16182208019065</v>
+        <v>1.24493728747632</v>
       </c>
       <c r="K10" s="7">
         <f>-X10/1000000</f>
@@ -1263,11 +1294,15 @@
       </c>
       <c r="L10" s="5">
         <f>AD10</f>
-        <v>1.2508900726826</v>
+        <v>1.3738522958958601</v>
       </c>
       <c r="M10" s="7">
         <f>Z10</f>
-        <v>74.583124682626604</v>
+        <v>75.566553458173203</v>
+      </c>
+      <c r="N10" s="7">
+        <f t="shared" si="13"/>
+        <v>74.955966394291565</v>
       </c>
       <c r="Q10" t="s">
         <v>25</v>
@@ -1297,38 +1332,38 @@
         <v>152.236892425848</v>
       </c>
       <c r="Z10">
-        <v>74.583124682626604</v>
+        <v>75.566553458173203</v>
       </c>
       <c r="AA10">
-        <v>1.27041134405722</v>
+        <v>1.4092509556325299</v>
       </c>
       <c r="AB10">
-        <v>1.1352056720286099</v>
+        <v>1.2046254778162599</v>
       </c>
       <c r="AC10">
-        <v>1.16182208019065</v>
+        <v>1.24493728747632</v>
       </c>
       <c r="AD10">
-        <v>1.2508900726826</v>
+        <v>1.3738522958958601</v>
       </c>
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="12"/>
-      <c r="C11" s="13"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="17"/>
       <c r="D11" s="9">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>596.15128272620996</v>
       </c>
       <c r="E11" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>80.923869008580112</v>
       </c>
       <c r="F11" s="5">
         <f>AA11</f>
-        <v>1.3574126874653101</v>
+        <v>1.54092214367092</v>
       </c>
       <c r="G11" s="9">
         <f>W11 / 1000</f>
@@ -1336,7 +1371,7 @@
       </c>
       <c r="H11" s="5">
         <f>AB11</f>
-        <v>1.1787063437326499</v>
+        <v>1.2704610718354601</v>
       </c>
       <c r="I11" s="9">
         <f>Y11</f>
@@ -1344,7 +1379,7 @@
       </c>
       <c r="J11" s="5">
         <f>AC11</f>
-        <v>1.2168338165371699</v>
+        <v>1.32820420299369</v>
       </c>
       <c r="K11" s="7">
         <f>-X11/1000000</f>
@@ -1352,11 +1387,15 @@
       </c>
       <c r="L11" s="5">
         <f>AD11</f>
-        <v>1.34989531853752</v>
+        <v>1.52138040680452</v>
       </c>
       <c r="M11" s="7">
         <f>Z11</f>
-        <v>75.425200650990803</v>
+        <v>76.697980800319897</v>
+      </c>
+      <c r="N11" s="7">
+        <f t="shared" si="13"/>
+        <v>97.400250187460955</v>
       </c>
       <c r="Q11" t="s">
         <v>27</v>
@@ -1386,19 +1425,19 @@
         <v>341.30839104135401</v>
       </c>
       <c r="Z11">
-        <v>75.425200650990803</v>
+        <v>76.697980800319897</v>
       </c>
       <c r="AA11">
-        <v>1.3574126874653101</v>
+        <v>1.54092214367092</v>
       </c>
       <c r="AB11">
-        <v>1.1787063437326499</v>
+        <v>1.2704610718354601</v>
       </c>
       <c r="AC11">
-        <v>1.2168338165371699</v>
+        <v>1.32820420299369</v>
       </c>
       <c r="AD11">
-        <v>1.34989531853752</v>
+        <v>1.52138040680452</v>
       </c>
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.25">
@@ -1414,16 +1453,16 @@
         <v>417.13799999999998</v>
       </c>
       <c r="D12" s="9">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>417.13799999999998</v>
       </c>
       <c r="E12" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>56.6239171978836</v>
       </c>
       <c r="F12" s="5">
         <f>AA12</f>
-        <v>1.41828912510476</v>
+        <v>1.63305489189682</v>
       </c>
       <c r="G12" s="9">
         <f>W12 / 1000</f>
@@ -1431,7 +1470,7 @@
       </c>
       <c r="H12" s="5">
         <f>AB12</f>
-        <v>1.20914456255238</v>
+        <v>1.31652744594841</v>
       </c>
       <c r="I12" s="9">
         <f>Y12</f>
@@ -1439,7 +1478,7 @@
       </c>
       <c r="J12" s="5">
         <f>AC12</f>
-        <v>1.24595690501515</v>
+        <v>1.37228551925366</v>
       </c>
       <c r="K12" s="7">
         <f>-X12/1000000</f>
@@ -1447,11 +1486,15 @@
       </c>
       <c r="L12" s="5">
         <f>AD12</f>
-        <v>1.4089340664699599</v>
+        <v>1.6093542800844001</v>
       </c>
       <c r="M12" s="7">
         <f>Z12</f>
-        <v>75.412976587741099</v>
+        <v>76.636453798361202</v>
+      </c>
+      <c r="N12" s="7">
+        <f t="shared" si="13"/>
+        <v>74.939605232342714</v>
       </c>
       <c r="Q12" t="s">
         <v>27</v>
@@ -1481,59 +1524,63 @@
         <v>180.68788827103401</v>
       </c>
       <c r="Z12">
-        <v>75.412976587741099</v>
+        <v>76.636453798361202</v>
       </c>
       <c r="AA12">
-        <v>1.41828912510476</v>
+        <v>1.63305489189682</v>
       </c>
       <c r="AB12">
-        <v>1.20914456255238</v>
+        <v>1.31652744594841</v>
       </c>
       <c r="AC12">
-        <v>1.24595690501515</v>
+        <v>1.37228551925366</v>
       </c>
       <c r="AD12">
-        <v>1.4089340664699599</v>
-      </c>
+        <v>1.6093542800844001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="N13" s="7"/>
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="14"/>
-      <c r="M14" s="14"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="12"/>
+      <c r="M14" s="12"/>
+      <c r="N14" s="7"/>
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="13">
+      <c r="C15" s="17">
         <v>1508.4970000000001</v>
       </c>
       <c r="D15" s="9">
-        <f t="shared" ref="D15:E19" si="14">U15/1000</f>
+        <f t="shared" ref="D15:E19" si="15">U15/1000</f>
         <v>1075.4017824339201</v>
       </c>
       <c r="E15" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>154.05686067103699</v>
       </c>
       <c r="F15" s="5">
         <f>AA15</f>
-        <v>1.16562670573983</v>
+        <v>1.2506658433233</v>
       </c>
       <c r="G15" s="9">
         <f>W15 / 1000</f>
@@ -1541,7 +1588,7 @@
       </c>
       <c r="H15" s="5">
         <f>AB15</f>
-        <v>1.08281335286991</v>
+        <v>1.1253329216616501</v>
       </c>
       <c r="I15" s="9">
         <f>Y15</f>
@@ -1549,7 +1596,7 @@
       </c>
       <c r="J15" s="5">
         <f>AC15</f>
-        <v>1.1007912647114</v>
+        <v>1.15255976780568</v>
       </c>
       <c r="K15" s="7">
         <f>-X15/1000000</f>
@@ -1557,11 +1604,15 @@
       </c>
       <c r="L15" s="5">
         <f>AD15</f>
-        <v>1.1431697263516101</v>
+        <v>1.2133377790800199</v>
       </c>
       <c r="M15" s="7">
         <f>Z15</f>
-        <v>73.862002341414396</v>
+        <v>74.585709366457493</v>
+      </c>
+      <c r="N15" s="7">
+        <f t="shared" si="13"/>
+        <v>91.093499051523196</v>
       </c>
       <c r="Q15" t="s">
         <v>20</v>
@@ -1591,38 +1642,38 @@
         <v>625.33754930004795</v>
       </c>
       <c r="Z15">
-        <v>73.862002341414396</v>
+        <v>74.585709366457493</v>
       </c>
       <c r="AA15">
-        <v>1.16562670573983</v>
+        <v>1.2506658433233</v>
       </c>
       <c r="AB15">
-        <v>1.08281335286991</v>
+        <v>1.1253329216616501</v>
       </c>
       <c r="AC15">
-        <v>1.1007912647114</v>
+        <v>1.15255976780568</v>
       </c>
       <c r="AD15">
-        <v>1.1431697263516101</v>
+        <v>1.2133377790800199</v>
       </c>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="12"/>
-      <c r="C16" s="13"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="17"/>
       <c r="D16" s="9">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>433.09521756606995</v>
       </c>
       <c r="E16" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>24.936483516051698</v>
       </c>
       <c r="F16" s="5">
         <f>AA16</f>
-        <v>1.1924359474672599</v>
+        <v>1.2912399835650401</v>
       </c>
       <c r="G16" s="9">
         <f>W16 / 1000</f>
@@ -1630,7 +1681,7 @@
       </c>
       <c r="H16" s="5">
         <f>AB16</f>
-        <v>1.0962179737336299</v>
+        <v>1.1456199917825201</v>
       </c>
       <c r="I16" s="9">
         <f>Y16</f>
@@ -1638,7 +1689,7 @@
       </c>
       <c r="J16" s="5">
         <f>AC16</f>
-        <v>1.1223759122795001</v>
+        <v>1.18523074212658</v>
       </c>
       <c r="K16" s="7">
         <f>-X16/1000000</f>
@@ -1646,11 +1697,15 @@
       </c>
       <c r="L16" s="5">
         <f>AD16</f>
-        <v>1.17379168061221</v>
+        <v>1.25896767500512</v>
       </c>
       <c r="M16" s="7">
         <f>Z16</f>
-        <v>74.432326814197495</v>
+        <v>75.398823493638503</v>
+      </c>
+      <c r="N16" s="7">
+        <f t="shared" si="13"/>
+        <v>120.5026305457756</v>
       </c>
       <c r="Q16" t="s">
         <v>23</v>
@@ -1680,43 +1735,43 @@
         <v>133.917266058618</v>
       </c>
       <c r="Z16">
-        <v>74.432326814197495</v>
+        <v>75.398823493638503</v>
       </c>
       <c r="AA16">
-        <v>1.1924359474672599</v>
+        <v>1.2912399835650401</v>
       </c>
       <c r="AB16">
-        <v>1.0962179737336299</v>
+        <v>1.1456199917825201</v>
       </c>
       <c r="AC16">
-        <v>1.1223759122795001</v>
+        <v>1.18523074212658</v>
       </c>
       <c r="AD16">
-        <v>1.17379168061221</v>
+        <v>1.25896767500512</v>
       </c>
     </row>
     <row r="17" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="12" t="str">
-        <f t="shared" ref="B17" si="15">R15</f>
+      <c r="B17" s="15" t="str">
+        <f t="shared" ref="B17" si="16">R15</f>
         <v>[80,85)</v>
       </c>
-      <c r="C17" s="13">
+      <c r="C17" s="17">
         <v>940.56899999999996</v>
       </c>
       <c r="D17" s="9">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>344.41771727378898</v>
       </c>
       <c r="E17" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="F17" s="5">
         <f>AA17</f>
-        <v>1.1924359474672599</v>
+        <v>1.2912399835650401</v>
       </c>
       <c r="G17" s="9">
         <f>W17 / 1000</f>
@@ -1724,7 +1779,7 @@
       </c>
       <c r="H17" s="5">
         <f>AB17</f>
-        <v>1.0962179737336299</v>
+        <v>1.1456199917825201</v>
       </c>
       <c r="I17" s="9">
         <f>Y17</f>
@@ -1732,7 +1787,7 @@
       </c>
       <c r="J17" s="5">
         <f>AC17</f>
-        <v>1.1223759122795001</v>
+        <v>1.18523074212658</v>
       </c>
       <c r="K17" s="7">
         <f>-X17/1000000</f>
@@ -1740,12 +1795,13 @@
       </c>
       <c r="L17" s="5">
         <f>AD17</f>
-        <v>1.17379168061221</v>
+        <v>1.25896767500512</v>
       </c>
       <c r="M17" s="7">
         <f>Z17</f>
-        <v>74.432326814197495</v>
-      </c>
+        <v>75.398823493638503</v>
+      </c>
+      <c r="N17" s="7"/>
       <c r="Q17" t="s">
         <v>25</v>
       </c>
@@ -1774,38 +1830,38 @@
         <v>0</v>
       </c>
       <c r="Z17">
-        <v>74.432326814197495</v>
+        <v>75.398823493638503</v>
       </c>
       <c r="AA17">
-        <v>1.1924359474672599</v>
+        <v>1.2912399835650401</v>
       </c>
       <c r="AB17">
-        <v>1.0962179737336299</v>
+        <v>1.1456199917825201</v>
       </c>
       <c r="AC17">
-        <v>1.1223759122795001</v>
+        <v>1.18523074212658</v>
       </c>
       <c r="AD17">
-        <v>1.17379168061221</v>
+        <v>1.25896767500512</v>
       </c>
     </row>
     <row r="18" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="12"/>
-      <c r="C18" s="13"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="17"/>
       <c r="D18" s="9">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>596.15128272620996</v>
       </c>
       <c r="E18" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="F18" s="5">
         <f>AA18</f>
-        <v>1.1924359474672599</v>
+        <v>1.2912399835650401</v>
       </c>
       <c r="G18" s="9">
         <f>W18 / 1000</f>
@@ -1813,7 +1869,7 @@
       </c>
       <c r="H18" s="5">
         <f>AB18</f>
-        <v>1.0962179737336299</v>
+        <v>1.1456199917825201</v>
       </c>
       <c r="I18" s="9">
         <f>Y18</f>
@@ -1821,7 +1877,7 @@
       </c>
       <c r="J18" s="5">
         <f>AC18</f>
-        <v>1.1223759122795001</v>
+        <v>1.18523074212658</v>
       </c>
       <c r="K18" s="7">
         <f>-X18/1000000</f>
@@ -1829,12 +1885,13 @@
       </c>
       <c r="L18" s="5">
         <f>AD18</f>
-        <v>1.17379168061221</v>
+        <v>1.25896767500512</v>
       </c>
       <c r="M18" s="7">
         <f>Z18</f>
-        <v>74.432326814197495</v>
-      </c>
+        <v>75.398823493638503</v>
+      </c>
+      <c r="N18" s="7"/>
       <c r="Q18" t="s">
         <v>27</v>
       </c>
@@ -1863,19 +1920,19 @@
         <v>0</v>
       </c>
       <c r="Z18">
-        <v>74.432326814197495</v>
+        <v>75.398823493638503</v>
       </c>
       <c r="AA18">
-        <v>1.1924359474672599</v>
+        <v>1.2912399835650401</v>
       </c>
       <c r="AB18">
-        <v>1.0962179737336299</v>
+        <v>1.1456199917825201</v>
       </c>
       <c r="AC18">
-        <v>1.1223759122795001</v>
+        <v>1.18523074212658</v>
       </c>
       <c r="AD18">
-        <v>1.17379168061221</v>
+        <v>1.25896767500512</v>
       </c>
     </row>
     <row r="19" spans="1:30" x14ac:dyDescent="0.25">
@@ -1883,23 +1940,23 @@
         <v>34</v>
       </c>
       <c r="B19" s="10" t="str">
-        <f t="shared" ref="B19" si="16">R17</f>
+        <f t="shared" ref="B19" si="17">R17</f>
         <v>[85,90)</v>
       </c>
       <c r="C19" s="11">
         <v>417.13799999999998</v>
       </c>
       <c r="D19" s="9">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>417.13799999999998</v>
       </c>
       <c r="E19" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="F19" s="5">
         <f>AA19</f>
-        <v>1.1924359474672599</v>
+        <v>1.2912399835650401</v>
       </c>
       <c r="G19" s="9">
         <f>W19 / 1000</f>
@@ -1907,7 +1964,7 @@
       </c>
       <c r="H19" s="5">
         <f>AB19</f>
-        <v>1.0962179737336299</v>
+        <v>1.1456199917825201</v>
       </c>
       <c r="I19" s="9">
         <f>Y19</f>
@@ -1915,7 +1972,7 @@
       </c>
       <c r="J19" s="5">
         <f>AC19</f>
-        <v>1.1223759122795001</v>
+        <v>1.18523074212658</v>
       </c>
       <c r="K19" s="7">
         <f>-X19/1000000</f>
@@ -1923,12 +1980,13 @@
       </c>
       <c r="L19" s="5">
         <f>AD19</f>
-        <v>1.17379168061221</v>
+        <v>1.25896767500512</v>
       </c>
       <c r="M19" s="7">
         <f>Z19</f>
-        <v>74.432326814197495</v>
-      </c>
+        <v>75.398823493638503</v>
+      </c>
+      <c r="N19" s="7"/>
       <c r="Q19" t="s">
         <v>27</v>
       </c>
@@ -1957,59 +2015,63 @@
         <v>0</v>
       </c>
       <c r="Z19">
-        <v>74.432326814197495</v>
+        <v>75.398823493638503</v>
       </c>
       <c r="AA19">
-        <v>1.1924359474672599</v>
+        <v>1.2912399835650401</v>
       </c>
       <c r="AB19">
-        <v>1.0962179737336299</v>
+        <v>1.1456199917825201</v>
       </c>
       <c r="AC19">
-        <v>1.1223759122795001</v>
+        <v>1.18523074212658</v>
       </c>
       <c r="AD19">
-        <v>1.17379168061221</v>
-      </c>
+        <v>1.25896767500512</v>
+      </c>
+    </row>
+    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="N20" s="7"/>
     </row>
     <row r="21" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A21" s="14" t="s">
+      <c r="A21" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="B21" s="14"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="14"/>
-      <c r="K21" s="14"/>
-      <c r="L21" s="14"/>
-      <c r="M21" s="14"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="12"/>
+      <c r="K21" s="12"/>
+      <c r="L21" s="12"/>
+      <c r="M21" s="12"/>
+      <c r="N21" s="7"/>
     </row>
     <row r="22" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>33</v>
       </c>
-      <c r="B22" s="12" t="s">
+      <c r="B22" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="13">
+      <c r="C22" s="17">
         <v>1508.4970000000001</v>
       </c>
       <c r="D22" s="9">
-        <f t="shared" ref="D22:E26" si="17">U22/1000</f>
+        <f t="shared" ref="D22:E26" si="18">U22/1000</f>
         <v>1075.4017824339201</v>
       </c>
       <c r="E22" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>256.661789483196</v>
       </c>
       <c r="F22" s="5">
         <f>AA22</f>
-        <v>1.27593738114763</v>
+        <v>1.4176142732588399</v>
       </c>
       <c r="G22" s="9">
         <f>W22 / 1000</f>
@@ -2017,7 +2079,7 @@
       </c>
       <c r="H22" s="5">
         <f>AB22</f>
-        <v>1.13796869057381</v>
+        <v>1.20880713662942</v>
       </c>
       <c r="I22" s="9">
         <f>Y22</f>
@@ -2025,7 +2087,7 @@
       </c>
       <c r="J22" s="5">
         <f>AC22</f>
-        <v>1.16170207008537</v>
+        <v>1.24475563766918</v>
       </c>
       <c r="K22" s="7">
         <f>-X22/1000000</f>
@@ -2033,11 +2095,15 @@
       </c>
       <c r="L22" s="5">
         <f>AD22</f>
-        <v>1.2370313312638701</v>
+        <v>1.35320133014732</v>
       </c>
       <c r="M22" s="7">
         <f>Z22</f>
-        <v>74.325184973719004</v>
+        <v>75.195652340758002</v>
+      </c>
+      <c r="N22" s="7">
+        <f t="shared" si="13"/>
+        <v>88.025254474808591</v>
       </c>
       <c r="Q22" t="s">
         <v>20</v>
@@ -2067,38 +2133,38 @@
         <v>1003.24543514224</v>
       </c>
       <c r="Z22">
-        <v>74.325184973719004</v>
+        <v>75.195652340758002</v>
       </c>
       <c r="AA22">
-        <v>1.27593738114763</v>
+        <v>1.4176142732588399</v>
       </c>
       <c r="AB22">
-        <v>1.13796869057381</v>
+        <v>1.20880713662942</v>
       </c>
       <c r="AC22">
-        <v>1.16170207008537</v>
+        <v>1.24475563766918</v>
       </c>
       <c r="AD22">
-        <v>1.2370313312638701</v>
+        <v>1.35320133014732</v>
       </c>
     </row>
     <row r="23" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>34</v>
       </c>
-      <c r="B23" s="12"/>
-      <c r="C23" s="13"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="17"/>
       <c r="D23" s="9">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>433.09521756606995</v>
       </c>
       <c r="E23" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>76.705702678003306</v>
       </c>
       <c r="F23" s="5">
         <f>AA23</f>
-        <v>1.3584037691466999</v>
+        <v>1.54242208490538</v>
       </c>
       <c r="G23" s="9">
         <f>W23 / 1000</f>
@@ -2106,7 +2172,7 @@
       </c>
       <c r="H23" s="5">
         <f>AB23</f>
-        <v>1.1792018845733501</v>
+        <v>1.2712110424526899</v>
       </c>
       <c r="I23" s="9">
         <f>Y23</f>
@@ -2114,7 +2180,7 @@
       </c>
       <c r="J23" s="5">
         <f>AC23</f>
-        <v>1.2252060352216501</v>
+        <v>1.3408765684231601</v>
       </c>
       <c r="K23" s="7">
         <f>-X23/1000000</f>
@@ -2122,11 +2188,15 @@
       </c>
       <c r="L23" s="5">
         <f>AD23</f>
-        <v>1.3326503547119399</v>
+        <v>1.4956836175696899</v>
       </c>
       <c r="M23" s="7">
         <f>Z23</f>
-        <v>75.783248062612401</v>
+        <v>77.199891657303397</v>
+      </c>
+      <c r="N23" s="7">
+        <f t="shared" si="13"/>
+        <v>116.02340370179897</v>
       </c>
       <c r="Q23" t="s">
         <v>23</v>
@@ -2156,43 +2226,43 @@
         <v>393.99658336326797</v>
       </c>
       <c r="Z23">
-        <v>75.783248062612401</v>
+        <v>77.199891657303397</v>
       </c>
       <c r="AA23">
-        <v>1.3584037691466999</v>
+        <v>1.54242208490538</v>
       </c>
       <c r="AB23">
-        <v>1.1792018845733501</v>
+        <v>1.2712110424526899</v>
       </c>
       <c r="AC23">
-        <v>1.2252060352216501</v>
+        <v>1.3408765684231601</v>
       </c>
       <c r="AD23">
-        <v>1.3326503547119399</v>
+        <v>1.4956836175696899</v>
       </c>
     </row>
     <row r="24" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>33</v>
       </c>
-      <c r="B24" s="12" t="str">
-        <f t="shared" ref="B24" si="18">R22</f>
+      <c r="B24" s="15" t="str">
+        <f t="shared" ref="B24" si="19">R22</f>
         <v>[80,85)</v>
       </c>
-      <c r="C24" s="13">
+      <c r="C24" s="17">
         <v>940.56899999999996</v>
       </c>
       <c r="D24" s="9">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>344.41771727378898</v>
       </c>
       <c r="E24" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>46.752586205033197</v>
       </c>
       <c r="F24" s="5">
         <f>AA24</f>
-        <v>1.4086675276331999</v>
+        <v>1.61849319525765</v>
       </c>
       <c r="G24" s="9">
         <f>W24 / 1000</f>
@@ -2200,7 +2270,7 @@
       </c>
       <c r="H24" s="5">
         <f>AB24</f>
-        <v>1.2043337638166001</v>
+        <v>1.3092465976288199</v>
       </c>
       <c r="I24" s="9">
         <f>Y24</f>
@@ -2208,7 +2278,7 @@
       </c>
       <c r="J24" s="5">
         <f>AC24</f>
-        <v>1.2497434213749501</v>
+        <v>1.3780168696667801</v>
       </c>
       <c r="K24" s="7">
         <f>-X24/1000000</f>
@@ -2216,11 +2286,15 @@
       </c>
       <c r="L24" s="5">
         <f>AD24</f>
-        <v>1.3757512268221399</v>
+        <v>1.5599083986510001</v>
       </c>
       <c r="M24" s="7">
         <f>Z24</f>
-        <v>75.765984457112793</v>
+        <v>77.134702300839194</v>
+      </c>
+      <c r="N24" s="7">
+        <f t="shared" si="13"/>
+        <v>74.955966394291565</v>
       </c>
       <c r="Q24" t="s">
         <v>25</v>
@@ -2250,38 +2324,38 @@
         <v>152.236892425848</v>
       </c>
       <c r="Z24">
-        <v>75.765984457112793</v>
+        <v>77.134702300839194</v>
       </c>
       <c r="AA24">
-        <v>1.4086675276331999</v>
+        <v>1.61849319525765</v>
       </c>
       <c r="AB24">
-        <v>1.2043337638166001</v>
+        <v>1.3092465976288199</v>
       </c>
       <c r="AC24">
-        <v>1.2497434213749501</v>
+        <v>1.3780168696667801</v>
       </c>
       <c r="AD24">
-        <v>1.3757512268221399</v>
+        <v>1.5599083986510001</v>
       </c>
     </row>
     <row r="25" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>34</v>
       </c>
-      <c r="B25" s="12"/>
-      <c r="C25" s="13"/>
+      <c r="B25" s="15"/>
+      <c r="C25" s="17"/>
       <c r="D25" s="9">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>596.15128272620996</v>
       </c>
       <c r="E25" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>80.923869008580112</v>
       </c>
       <c r="F25" s="5">
         <f>AA25</f>
-        <v>1.49566887104128</v>
+        <v>1.7501643832960401</v>
       </c>
       <c r="G25" s="9">
         <f>W25 / 1000</f>
@@ -2289,7 +2363,7 @@
       </c>
       <c r="H25" s="5">
         <f>AB25</f>
-        <v>1.2478344355206401</v>
+        <v>1.37508219164802</v>
       </c>
       <c r="I25" s="9">
         <f>Y25</f>
@@ -2297,7 +2371,7 @@
       </c>
       <c r="J25" s="5">
         <f>AC25</f>
-        <v>1.30475515772147</v>
+        <v>1.46128378518414</v>
       </c>
       <c r="K25" s="7">
         <f>-X25/1000000</f>
@@ -2305,11 +2379,15 @@
       </c>
       <c r="L25" s="5">
         <f>AD25</f>
-        <v>1.4747564726770701</v>
+        <v>1.70743650955965</v>
       </c>
       <c r="M25" s="7">
         <f>Z25</f>
-        <v>76.520175128811402</v>
+        <v>78.104967490326601</v>
+      </c>
+      <c r="N25" s="7">
+        <f t="shared" si="13"/>
+        <v>97.400250187460955</v>
       </c>
       <c r="Q25" t="s">
         <v>27</v>
@@ -2339,19 +2417,19 @@
         <v>341.30839104135401</v>
       </c>
       <c r="Z25">
-        <v>76.520175128811402</v>
+        <v>78.104967490326601</v>
       </c>
       <c r="AA25">
-        <v>1.49566887104128</v>
+        <v>1.7501643832960401</v>
       </c>
       <c r="AB25">
-        <v>1.2478344355206401</v>
+        <v>1.37508219164802</v>
       </c>
       <c r="AC25">
-        <v>1.30475515772147</v>
+        <v>1.46128378518414</v>
       </c>
       <c r="AD25">
-        <v>1.4747564726770701</v>
+        <v>1.70743650955965</v>
       </c>
     </row>
     <row r="26" spans="1:30" x14ac:dyDescent="0.25">
@@ -2359,23 +2437,23 @@
         <v>34</v>
       </c>
       <c r="B26" s="10" t="str">
-        <f t="shared" ref="B26" si="19">R24</f>
+        <f t="shared" ref="B26" si="20">R24</f>
         <v>[85,90)</v>
       </c>
       <c r="C26" s="11">
         <v>417.13799999999998</v>
       </c>
       <c r="D26" s="9">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>417.13799999999998</v>
       </c>
       <c r="E26" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>56.6239171978836</v>
       </c>
       <c r="F26" s="5">
         <f>AA26</f>
-        <v>1.5565453086807399</v>
+        <v>1.8422971315219401</v>
       </c>
       <c r="G26" s="9">
         <f>W26 / 1000</f>
@@ -2383,7 +2461,7 @@
       </c>
       <c r="H26" s="5">
         <f>AB26</f>
-        <v>1.27827265434037</v>
+        <v>1.4211485657609699</v>
       </c>
       <c r="I26" s="9">
         <f>Y26</f>
@@ -2391,7 +2469,7 @@
       </c>
       <c r="J26" s="5">
         <f>AC26</f>
-        <v>1.3338782461994501</v>
+        <v>1.5053651014441101</v>
       </c>
       <c r="K26" s="7">
         <f>-X26/1000000</f>
@@ -2399,11 +2477,15 @@
       </c>
       <c r="L26" s="5">
         <f>AD26</f>
-        <v>1.53379522060951</v>
+        <v>1.79541038283954</v>
       </c>
       <c r="M26" s="7">
         <f>Z26</f>
-        <v>76.482538610338395</v>
+        <v>78.002362621636394</v>
+      </c>
+      <c r="N26" s="7">
+        <f t="shared" si="13"/>
+        <v>74.939605232342714</v>
       </c>
       <c r="Q26" t="s">
         <v>27</v>
@@ -2433,23 +2515,51 @@
         <v>180.68788827103401</v>
       </c>
       <c r="Z26">
-        <v>76.482538610338395</v>
+        <v>78.002362621636394</v>
       </c>
       <c r="AA26">
-        <v>1.5565453086807399</v>
+        <v>1.8422971315219401</v>
       </c>
       <c r="AB26">
-        <v>1.27827265434037</v>
+        <v>1.4211485657609699</v>
       </c>
       <c r="AC26">
-        <v>1.3338782461994501</v>
+        <v>1.5053651014441101</v>
       </c>
       <c r="AD26">
-        <v>1.53379522060951</v>
+        <v>1.79541038283954</v>
+      </c>
+    </row>
+    <row r="29" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="D29" s="9">
+        <f>SUM(D3:D5)</f>
+        <v>2168.6131270308952</v>
+      </c>
+      <c r="E29" s="9">
+        <f>SUM(E3:E5)</f>
+        <v>614.59055860409251</v>
+      </c>
+      <c r="G29" s="9">
+        <f>SUM(G3:G5)</f>
+        <v>1229.1811172081859</v>
+      </c>
+      <c r="I29" s="9">
+        <f>SUM(I3:I5)</f>
+        <v>4098.9676262258126</v>
+      </c>
+      <c r="K29" s="9">
+        <f>SUM(K3:K5)</f>
+        <v>7.1568547868121879</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="C24:C25"/>
     <mergeCell ref="A14:M14"/>
     <mergeCell ref="A21:M21"/>
     <mergeCell ref="K1:L1"/>
@@ -2464,12 +2574,6 @@
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="A7:M7"/>
     <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="C24:C25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Apply fixed QALY loss
</commit_message>
<xml_diff>
--- a/docs/tabs/Tab_ProgrammeProfile.xlsx
+++ b/docs/tabs/Tab_ProgrammeProfile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HPRU_Shingrix\docs\tabs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\HPRU\Shingrix\HPRU_RZV\docs\tabs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BAAE397-564B-46FE-9CE8-AB5062D85D50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F076679E-D6A1-41D6-A331-7AA0743CE33B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="34605" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="56">
   <si>
     <t>Eligibility</t>
   </si>
@@ -225,6 +225,21 @@
   </si>
   <si>
     <t>Marginal threshold price per administration</t>
+  </si>
+  <si>
+    <t>HZ prevention</t>
+  </si>
+  <si>
+    <t>Cases</t>
+  </si>
+  <si>
+    <t>dRisk_HZ</t>
+  </si>
+  <si>
+    <t>Prop_Case</t>
+  </si>
+  <si>
+    <t>NNV</t>
   </si>
 </sst>
 </file>
@@ -298,6 +313,12 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -307,14 +328,8 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -599,10 +614,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AD29"/>
+  <dimension ref="A1:AH29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+      <selection activeCell="Q22" sqref="Q22:Q23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -614,15 +629,15 @@
     <col min="5" max="5" width="9.140625" style="3"/>
     <col min="6" max="6" width="13.42578125" style="5" customWidth="1"/>
     <col min="7" max="7" width="9.140625" style="9"/>
-    <col min="8" max="8" width="12.5703125" style="5" customWidth="1"/>
-    <col min="9" max="9" width="11.85546875" style="9" customWidth="1"/>
-    <col min="10" max="10" width="12.5703125" style="5" customWidth="1"/>
-    <col min="11" max="11" width="14.140625" style="7" customWidth="1"/>
-    <col min="12" max="12" width="13.7109375" style="5" customWidth="1"/>
+    <col min="8" max="10" width="12.5703125" style="5" customWidth="1"/>
+    <col min="11" max="11" width="11.85546875" style="9" customWidth="1"/>
+    <col min="12" max="12" width="12.5703125" style="5" customWidth="1"/>
     <col min="13" max="13" width="14.140625" style="7" customWidth="1"/>
+    <col min="14" max="14" width="13.7109375" style="5" customWidth="1"/>
+    <col min="15" max="15" width="14.140625" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="1" customFormat="1" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" s="1" customFormat="1" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>30</v>
       </c>
@@ -635,30 +650,37 @@
       <c r="D1" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="16"/>
-      <c r="G1" s="14" t="s">
+      <c r="F1" s="17"/>
+      <c r="G1" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14" t="s">
+      <c r="H1" s="16"/>
+      <c r="I1" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="J1" s="14"/>
-      <c r="K1" s="13" t="s">
+      <c r="L1" s="16"/>
+      <c r="M1" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="L1" s="13"/>
-      <c r="M1" s="6" t="s">
+      <c r="N1" s="15"/>
+      <c r="O1" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>50</v>
       </c>
+      <c r="Q1" s="1" t="s">
+        <v>55</v>
+      </c>
     </row>
-    <row r="2" spans="1:30" s="1" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" s="1" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" s="1" t="s">
         <v>38</v>
       </c>
@@ -677,81 +699,93 @@
       <c r="H2" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="I2" s="8" t="s">
-        <v>44</v>
+      <c r="I2" s="4" t="s">
+        <v>52</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="K2" s="6" t="s">
-        <v>40</v>
+      <c r="K2" s="8" t="s">
+        <v>44</v>
       </c>
       <c r="L2" s="4" t="s">
         <v>36</v>
       </c>
       <c r="M2" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="O2" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="Q2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="R2" s="1" t="s">
+      <c r="S2" t="s">
+        <v>0</v>
+      </c>
+      <c r="T2" t="s">
         <v>1</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="U2" t="s">
         <v>2</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="V2" t="s">
         <v>3</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="W2" t="s">
         <v>4</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="X2" t="s">
         <v>5</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="Y2" t="s">
         <v>6</v>
       </c>
-      <c r="X2" s="1" t="s">
+      <c r="Z2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AA2" t="s">
         <v>7</v>
       </c>
-      <c r="Y2" s="1" t="s">
+      <c r="AB2" t="s">
         <v>8</v>
       </c>
-      <c r="Z2" s="1" t="s">
+      <c r="AC2" t="s">
         <v>9</v>
       </c>
-      <c r="AA2" s="1" t="s">
+      <c r="AD2" t="s">
         <v>10</v>
       </c>
-      <c r="AB2" s="1" t="s">
+      <c r="AE2" t="s">
         <v>11</v>
       </c>
-      <c r="AC2" s="1" t="s">
+      <c r="AF2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG2" t="s">
         <v>12</v>
       </c>
-      <c r="AD2" s="1" t="s">
+      <c r="AH2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>35</v>
       </c>
       <c r="B3" s="10" t="str">
-        <f>R3</f>
+        <f>T3</f>
         <v>[65,70)</v>
       </c>
       <c r="C3" s="11">
-        <f>T3 / 1000</f>
+        <f>V3 / 1000</f>
         <v>2965.5050000000001</v>
       </c>
       <c r="D3" s="9">
-        <f t="shared" ref="D3:E3" si="0">U3 / 1000</f>
+        <f t="shared" ref="D3:E3" si="0">W3 / 1000</f>
         <v>640.87300000000005</v>
       </c>
       <c r="E3" s="3">
@@ -759,184 +793,220 @@
         <v>308.98772385586199</v>
       </c>
       <c r="F3" s="5">
-        <f>AA3</f>
+        <f>AD3</f>
         <v>0.50275377571315005</v>
       </c>
       <c r="G3" s="9">
-        <f>W3 / 1000</f>
+        <f>Y3 / 1000</f>
         <v>617.97544771172397</v>
       </c>
       <c r="H3" s="5">
+        <f>AE3</f>
+        <v>0.50275377571315005</v>
+      </c>
+      <c r="I3" s="9">
+        <f>-Z3</f>
+        <v>23162.658977379899</v>
+      </c>
+      <c r="J3" s="5">
+        <f>AF3</f>
+        <v>0.51078717450861</v>
+      </c>
+      <c r="K3" s="9">
         <f>AB3</f>
+        <v>1959.7805499829601</v>
+      </c>
+      <c r="L3" s="5">
+        <f>AG3</f>
+        <v>0.47811564488677299</v>
+      </c>
+      <c r="M3" s="7">
+        <f>-AA3/1000000</f>
+        <v>3.10664610742537</v>
+      </c>
+      <c r="N3" s="5">
+        <f>AH3</f>
+        <v>0.43407980180762201</v>
+      </c>
+      <c r="O3" s="7">
+        <f>AC3</f>
+        <v>68.452973760889407</v>
+      </c>
+      <c r="P3" s="7">
+        <f>(K3 * 20 + M3 * 1000) /G3</f>
+        <v>68.452973760889478</v>
+      </c>
+      <c r="Q3" s="3">
+        <f>E3/I3*1000</f>
+        <v>13.339907311920106</v>
+      </c>
+      <c r="S3" t="s">
+        <v>14</v>
+      </c>
+      <c r="T3" t="s">
+        <v>15</v>
+      </c>
+      <c r="U3" t="s">
+        <v>16</v>
+      </c>
+      <c r="V3">
+        <v>2965505</v>
+      </c>
+      <c r="W3">
+        <v>640873</v>
+      </c>
+      <c r="X3">
+        <v>308987.72385586199</v>
+      </c>
+      <c r="Y3">
+        <v>617975.44771172397</v>
+      </c>
+      <c r="Z3">
+        <v>-23162.658977379899</v>
+      </c>
+      <c r="AA3">
+        <v>-3106646.1074253698</v>
+      </c>
+      <c r="AB3">
+        <v>1959.7805499829601</v>
+      </c>
+      <c r="AC3">
+        <v>68.452973760889407</v>
+      </c>
+      <c r="AD3">
         <v>0.50275377571315005</v>
       </c>
-      <c r="I3" s="9">
-        <f>Y3</f>
-        <v>1959.7805499829601</v>
-      </c>
-      <c r="J3" s="5">
-        <f>AC3</f>
+      <c r="AE3">
+        <v>0.50275377571315005</v>
+      </c>
+      <c r="AF3">
+        <v>0.51078717450861</v>
+      </c>
+      <c r="AG3">
         <v>0.47811564488677299</v>
       </c>
-      <c r="K3" s="7">
-        <f>-X3/1000000</f>
-        <v>3.10664610742537</v>
-      </c>
-      <c r="L3" s="5">
-        <f>AD3</f>
+      <c r="AH3">
         <v>0.43407980180762201</v>
       </c>
-      <c r="M3" s="7">
-        <f>Z3</f>
-        <v>68.452973760889407</v>
-      </c>
-      <c r="N3" s="7">
-        <f>(I3 * 20 + K3 * 1000) /G3</f>
-        <v>68.452973760889478</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>14</v>
-      </c>
-      <c r="R3" t="s">
-        <v>15</v>
-      </c>
-      <c r="S3" t="s">
-        <v>16</v>
-      </c>
-      <c r="T3">
-        <v>2965505</v>
-      </c>
-      <c r="U3">
-        <v>640873</v>
-      </c>
-      <c r="V3">
-        <v>308987.72385586199</v>
-      </c>
-      <c r="W3">
-        <v>617975.44771172397</v>
-      </c>
-      <c r="X3">
-        <v>-3106646.1074253698</v>
-      </c>
-      <c r="Y3">
-        <v>1959.7805499829601</v>
-      </c>
-      <c r="Z3">
-        <v>68.452973760889407</v>
-      </c>
-      <c r="AA3">
-        <v>0.50275377571315005</v>
-      </c>
-      <c r="AB3">
-        <v>0.50275377571315005</v>
-      </c>
-      <c r="AC3">
-        <v>0.47811564488677299</v>
-      </c>
-      <c r="AD3">
-        <v>0.43407980180762201</v>
-      </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>48</v>
       </c>
       <c r="B4" s="10" t="str">
-        <f t="shared" ref="B4:B5" si="1">R4</f>
+        <f t="shared" ref="B4:B5" si="1">T4</f>
         <v>[70,75)</v>
       </c>
       <c r="C4" s="11">
-        <f t="shared" ref="C4:C5" si="2">T4 / 1000</f>
+        <f t="shared" ref="C4:C5" si="2">V4 / 1000</f>
         <v>2662.3220000000001</v>
       </c>
       <c r="D4" s="9">
-        <f t="shared" ref="D4:D5" si="3">U4 / 1000</f>
+        <f t="shared" ref="D4:D5" si="3">W4 / 1000</f>
         <v>1053.4762497747899</v>
       </c>
       <c r="E4" s="3">
-        <f t="shared" ref="E4:E5" si="4">V4 / 1000</f>
+        <f t="shared" ref="E4:E5" si="4">X4 / 1000</f>
         <v>241.22443116069599</v>
       </c>
       <c r="F4" s="5">
-        <f t="shared" ref="F4:F5" si="5">AA4</f>
+        <f t="shared" ref="F4:F5" si="5">AD4</f>
         <v>0.89524993072826198</v>
       </c>
       <c r="G4" s="9">
-        <f t="shared" ref="G4:G5" si="6">W4 / 1000</f>
+        <f t="shared" ref="G4:G5" si="6">Y4 / 1000</f>
         <v>482.44886232139299</v>
       </c>
       <c r="H4" s="5">
-        <f t="shared" ref="H4:H5" si="7">AB4</f>
+        <f t="shared" ref="H4:H5" si="7">AE4</f>
         <v>0.89524993072826198</v>
       </c>
       <c r="I4" s="9">
-        <f t="shared" ref="I4:I5" si="8">Y4</f>
+        <f t="shared" ref="I4:I5" si="8">-Z4</f>
+        <v>17879.289898334198</v>
+      </c>
+      <c r="J4" s="5">
+        <f t="shared" ref="J4:J5" si="9">AF4</f>
+        <v>0.90506453179773005</v>
+      </c>
+      <c r="K4" s="9">
+        <f t="shared" ref="K4:K5" si="10">AB4</f>
         <v>1690.96100110564</v>
       </c>
-      <c r="J4" s="5">
-        <f t="shared" ref="J4:J5" si="9">AC4</f>
+      <c r="L4" s="5">
+        <f t="shared" ref="L4:L5" si="11">AG4</f>
         <v>0.89064903263216899</v>
       </c>
-      <c r="K4" s="7">
-        <f t="shared" ref="K4:K5" si="10">-X4/1000000</f>
+      <c r="M4" s="7">
+        <f t="shared" ref="M4:M5" si="12">-AA4/1000000</f>
         <v>3.0752656514611902</v>
       </c>
-      <c r="L4" s="5">
-        <f t="shared" ref="L4:L5" si="11">AD4</f>
+      <c r="N4" s="5">
+        <f t="shared" ref="N4:N5" si="13">AH4</f>
         <v>0.86377493228978997</v>
       </c>
-      <c r="M4" s="7">
-        <f t="shared" ref="M4:M5" si="12">Z4</f>
+      <c r="O4" s="7">
+        <f t="shared" ref="O4:O5" si="14">AC4</f>
         <v>71.9692777218591</v>
       </c>
-      <c r="N4" s="7">
-        <f t="shared" ref="N4:N26" si="13">(I4 * 20 + K4 * 1000) /G4</f>
+      <c r="P4" s="7">
+        <f>(K4 * 20 + M4 * 1000) /G4</f>
         <v>76.473360297813258</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="Q4" s="3">
+        <f t="shared" ref="Q4:Q5" si="15">E4/I4*1000</f>
+        <v>13.491835108237195</v>
+      </c>
+      <c r="S4" t="s">
         <v>17</v>
       </c>
-      <c r="R4" t="s">
+      <c r="T4" t="s">
         <v>18</v>
       </c>
-      <c r="S4" t="s">
+      <c r="U4" t="s">
         <v>16</v>
       </c>
-      <c r="T4">
+      <c r="V4">
         <v>2662322</v>
       </c>
-      <c r="U4">
+      <c r="W4">
         <v>1053476.2497747899</v>
       </c>
-      <c r="V4">
+      <c r="X4">
         <v>241224.431160696</v>
       </c>
-      <c r="W4">
+      <c r="Y4">
         <v>482448.86232139298</v>
       </c>
-      <c r="X4">
+      <c r="Z4">
+        <v>-17879.289898334198</v>
+      </c>
+      <c r="AA4">
         <v>-3075265.6514611901</v>
       </c>
-      <c r="Y4">
+      <c r="AB4">
         <v>1690.96100110564</v>
       </c>
-      <c r="Z4">
+      <c r="AC4">
         <v>71.9692777218591</v>
       </c>
-      <c r="AA4">
+      <c r="AD4">
         <v>0.89524993072826198</v>
       </c>
-      <c r="AB4">
+      <c r="AE4">
         <v>0.89524993072826198</v>
       </c>
-      <c r="AC4">
+      <c r="AF4">
+        <v>0.90506453179773005</v>
+      </c>
+      <c r="AG4">
         <v>0.89064903263216899</v>
       </c>
-      <c r="AD4">
+      <c r="AH4">
         <v>0.86377493228978997</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5" s="18"/>
       <c r="B5" s="10" t="str">
         <f t="shared" si="1"/>
@@ -968,15 +1038,15 @@
       </c>
       <c r="I5" s="9">
         <f t="shared" si="8"/>
-        <v>448.22607513721198</v>
+        <v>4305.03737088253</v>
       </c>
       <c r="J5" s="5">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-      <c r="K5" s="7">
+      <c r="K5" s="9">
         <f t="shared" si="10"/>
-        <v>0.97494302792562804</v>
+        <v>448.22607513721198</v>
       </c>
       <c r="L5" s="5">
         <f t="shared" si="11"/>
@@ -984,845 +1054,1006 @@
       </c>
       <c r="M5" s="7">
         <f t="shared" si="12"/>
+        <v>0.97494302792562804</v>
+      </c>
+      <c r="N5" s="5">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="O5" s="7">
+        <f t="shared" si="14"/>
         <v>72.516739855052194</v>
       </c>
-      <c r="N5" s="7">
-        <f t="shared" si="13"/>
+      <c r="P5" s="7">
+        <f>(K5 * 20 + M5 * 1000) /G5</f>
         <v>77.195643078934864</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="Q5" s="3">
+        <f t="shared" si="15"/>
+        <v>14.954203190653597</v>
+      </c>
+      <c r="S5" t="s">
         <v>17</v>
       </c>
-      <c r="R5" t="s">
+      <c r="T5" t="s">
         <v>19</v>
       </c>
-      <c r="S5" t="s">
+      <c r="U5" t="s">
         <v>16</v>
       </c>
-      <c r="T5">
+      <c r="V5">
         <v>2423598</v>
       </c>
-      <c r="U5">
+      <c r="W5">
         <v>474263.87725610501</v>
       </c>
-      <c r="V5">
+      <c r="X5">
         <v>64378.4035875345</v>
       </c>
-      <c r="W5">
+      <c r="Y5">
         <v>128756.807175069</v>
       </c>
-      <c r="X5">
+      <c r="Z5">
+        <v>-4305.03737088253</v>
+      </c>
+      <c r="AA5">
         <v>-974943.027925628</v>
       </c>
-      <c r="Y5">
+      <c r="AB5">
         <v>448.22607513721198</v>
       </c>
-      <c r="Z5">
+      <c r="AC5">
         <v>72.516739855052194</v>
-      </c>
-      <c r="AA5">
-        <v>1</v>
-      </c>
-      <c r="AB5">
-        <v>1</v>
-      </c>
-      <c r="AC5">
-        <v>1</v>
       </c>
       <c r="AD5">
         <v>1</v>
       </c>
+      <c r="AE5">
+        <v>1</v>
+      </c>
+      <c r="AF5">
+        <v>1</v>
+      </c>
+      <c r="AG5">
+        <v>1</v>
+      </c>
+      <c r="AH5">
+        <v>1</v>
+      </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="B6" s="10"/>
       <c r="C6" s="11"/>
-      <c r="N6" s="7"/>
+      <c r="P6" s="7"/>
+      <c r="Q6" s="3"/>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="12"/>
-      <c r="M7" s="12"/>
-      <c r="N7" s="7"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="14"/>
+      <c r="N7" s="14"/>
+      <c r="O7" s="14"/>
+      <c r="P7" s="7"/>
+      <c r="Q7" s="3"/>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="15" t="str">
-        <f>R8</f>
+      <c r="B8" s="12" t="str">
+        <f>T8</f>
         <v>[80,85)</v>
       </c>
-      <c r="C8" s="17">
-        <f>T8/1000</f>
+      <c r="C8" s="13">
+        <f>V8/1000</f>
         <v>1508.4970000000001</v>
       </c>
       <c r="D8" s="9">
-        <f>U8/1000</f>
+        <f>W8/1000</f>
         <v>1075.4017824339201</v>
       </c>
       <c r="E8" s="3">
-        <f>V8/1000</f>
+        <f t="shared" ref="E8" si="16">X8 / 1000</f>
         <v>145.979175915393</v>
       </c>
       <c r="F8" s="5">
-        <f>AA8</f>
+        <f t="shared" ref="F8" si="17">AD8</f>
         <v>1.23752264637281</v>
       </c>
       <c r="G8" s="9">
-        <f>W8 / 1000</f>
+        <f t="shared" ref="G8" si="18">Y8 / 1000</f>
         <v>145.979175915393</v>
       </c>
       <c r="H8" s="5">
-        <f>AB8</f>
+        <f t="shared" ref="H8" si="19">AE8</f>
         <v>1.1187613231864</v>
       </c>
       <c r="I8" s="9">
-        <f>Y8</f>
+        <f t="shared" ref="I8" si="20">-Z8</f>
+        <v>6288.9277062869696</v>
+      </c>
+      <c r="J8" s="5">
+        <f t="shared" ref="J8" si="21">AF8</f>
+        <v>1.1386845792152001</v>
+      </c>
+      <c r="K8" s="9">
+        <f t="shared" ref="K8" si="22">AB8</f>
         <v>553.96979745149702</v>
       </c>
-      <c r="J8" s="5">
-        <f>AC8</f>
+      <c r="L8" s="5">
+        <f t="shared" ref="L8" si="23">AG8</f>
         <v>1.1351486149602901</v>
       </c>
-      <c r="K8" s="7">
-        <f>-X8/1000000</f>
+      <c r="M8" s="7">
+        <f t="shared" ref="M8" si="24">-AA8/1000000</f>
         <v>1.43085683012938</v>
       </c>
-      <c r="L8" s="5">
-        <f>AD8</f>
+      <c r="N8" s="5">
+        <f t="shared" ref="N8" si="25">AH8</f>
         <v>1.19992816296426</v>
       </c>
-      <c r="M8" s="7">
-        <f>Z8</f>
+      <c r="O8" s="7">
+        <f t="shared" ref="O8" si="26">AC8</f>
         <v>73.916081346127996</v>
       </c>
-      <c r="N8" s="7">
-        <f t="shared" si="13"/>
+      <c r="P8" s="7">
+        <f>(K8 * 20 + M8 * 1000) /G8</f>
         <v>85.698886164489963</v>
       </c>
-      <c r="Q8" t="s">
+      <c r="Q8" s="3">
+        <f t="shared" ref="Q8:Q12" si="27">E8/I8*1000</f>
+        <v>23.212093179169361</v>
+      </c>
+      <c r="S8" t="s">
         <v>20</v>
       </c>
-      <c r="R8" t="s">
+      <c r="T8" t="s">
         <v>21</v>
       </c>
-      <c r="S8" t="s">
+      <c r="U8" t="s">
         <v>22</v>
       </c>
-      <c r="T8">
+      <c r="V8">
         <v>1508497</v>
       </c>
-      <c r="U8">
+      <c r="W8">
         <v>1075401.7824339201</v>
       </c>
-      <c r="V8">
+      <c r="X8">
         <v>145979.17591539299</v>
       </c>
-      <c r="W8">
+      <c r="Y8">
         <v>145979.17591539299</v>
       </c>
-      <c r="X8">
+      <c r="Z8">
+        <v>-6288.9277062869696</v>
+      </c>
+      <c r="AA8">
         <v>-1430856.8301293801</v>
       </c>
-      <c r="Y8">
+      <c r="AB8">
         <v>553.96979745149702</v>
       </c>
-      <c r="Z8">
+      <c r="AC8">
         <v>73.916081346127996</v>
       </c>
-      <c r="AA8">
+      <c r="AD8">
         <v>1.23752264637281</v>
       </c>
-      <c r="AB8">
+      <c r="AE8">
         <v>1.1187613231864</v>
       </c>
-      <c r="AC8">
+      <c r="AF8">
+        <v>1.1386845792152001</v>
+      </c>
+      <c r="AG8">
         <v>1.1351486149602901</v>
       </c>
-      <c r="AD8">
+      <c r="AH8">
         <v>1.19992816296426</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="15"/>
-      <c r="C9" s="17"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="13"/>
       <c r="D9" s="9">
-        <f t="shared" ref="D9:E12" si="14">U9/1000</f>
+        <f t="shared" ref="D9:E12" si="28">W9/1000</f>
         <v>433.09521756606995</v>
       </c>
       <c r="E9" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" ref="E9:E12" si="29">X9 / 1000</f>
         <v>58.790011311030398</v>
       </c>
       <c r="F9" s="5">
-        <f>AA9</f>
+        <f t="shared" ref="F9:F12" si="30">AD9</f>
         <v>1.3331798452802599</v>
       </c>
       <c r="G9" s="9">
-        <f>W9 / 1000</f>
+        <f t="shared" ref="G9:G12" si="31">Y9 / 1000</f>
         <v>58.790011311030398</v>
       </c>
       <c r="H9" s="5">
-        <f>AB9</f>
+        <f t="shared" ref="H9:H12" si="32">AE9</f>
         <v>1.16658992264013</v>
       </c>
       <c r="I9" s="9">
-        <f>Y9</f>
+        <f t="shared" ref="I9:I12" si="33">-Z9</f>
+        <v>2562.3213034586302</v>
+      </c>
+      <c r="J9" s="5">
+        <f t="shared" ref="J9:J12" si="34">AF9</f>
+        <v>1.1951893552884101</v>
+      </c>
+      <c r="K9" s="9">
+        <f t="shared" ref="K9:K12" si="35">AB9</f>
         <v>297.783321943685</v>
       </c>
-      <c r="J9" s="5">
-        <f>AC9</f>
+      <c r="L9" s="5">
+        <f t="shared" ref="L9:L12" si="36">AG9</f>
         <v>1.20779698623271</v>
       </c>
-      <c r="K9" s="7">
-        <f>-X9/1000000</f>
+      <c r="M9" s="7">
+        <f t="shared" ref="M9:M12" si="37">-AA9/1000000</f>
         <v>0.78510233139996599</v>
       </c>
-      <c r="L9" s="5">
-        <f>AD9</f>
+      <c r="N9" s="5">
+        <f t="shared" ref="N9:N12" si="38">AH9</f>
         <v>1.30962751481456</v>
       </c>
-      <c r="M9" s="7">
-        <f>Z9</f>
+      <c r="O9" s="7">
+        <f t="shared" ref="O9:O12" si="39">AC9</f>
         <v>75.5864610688146</v>
       </c>
-      <c r="N9" s="7">
-        <f t="shared" si="13"/>
+      <c r="P9" s="7">
+        <f t="shared" ref="P9:P12" si="40">(K9 * 20 + M9 * 1000) /G9</f>
         <v>114.65840233660472</v>
       </c>
-      <c r="Q9" t="s">
+      <c r="Q9" s="3">
+        <f t="shared" si="27"/>
+        <v>22.944043446727559</v>
+      </c>
+      <c r="S9" t="s">
         <v>23</v>
       </c>
-      <c r="R9" t="s">
+      <c r="T9" t="s">
         <v>21</v>
       </c>
-      <c r="S9" t="s">
+      <c r="U9" t="s">
         <v>24</v>
       </c>
-      <c r="T9">
+      <c r="V9">
         <v>1508497</v>
       </c>
-      <c r="U9">
+      <c r="W9">
         <v>433095.21756606997</v>
       </c>
-      <c r="V9">
+      <c r="X9">
         <v>58790.011311030401</v>
       </c>
-      <c r="W9">
+      <c r="Y9">
         <v>58790.011311030401</v>
       </c>
-      <c r="X9">
+      <c r="Z9">
+        <v>-2562.3213034586302</v>
+      </c>
+      <c r="AA9">
         <v>-785102.33139996603</v>
       </c>
-      <c r="Y9">
+      <c r="AB9">
         <v>297.783321943685</v>
       </c>
-      <c r="Z9">
+      <c r="AC9">
         <v>75.5864610688146</v>
       </c>
-      <c r="AA9">
+      <c r="AD9">
         <v>1.3331798452802599</v>
       </c>
-      <c r="AB9">
+      <c r="AE9">
         <v>1.16658992264013</v>
       </c>
-      <c r="AC9">
+      <c r="AF9">
+        <v>1.1951893552884101</v>
+      </c>
+      <c r="AG9">
         <v>1.20779698623271</v>
       </c>
-      <c r="AD9">
+      <c r="AH9">
         <v>1.30962751481456</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="15" t="str">
-        <f>R10</f>
+      <c r="B10" s="12" t="str">
+        <f>T10</f>
         <v>[85,90)</v>
       </c>
-      <c r="C10" s="17">
-        <f>T10/1000</f>
+      <c r="C10" s="13">
+        <f>V10/1000</f>
         <v>940.56899999999996</v>
       </c>
       <c r="D10" s="9">
-        <f t="shared" si="14"/>
+        <f t="shared" si="28"/>
         <v>344.41771727378898</v>
       </c>
       <c r="E10" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="29"/>
         <v>46.752586205033197</v>
       </c>
       <c r="F10" s="5">
-        <f>AA10</f>
+        <f t="shared" si="30"/>
         <v>1.4092509556325299</v>
       </c>
       <c r="G10" s="9">
-        <f>W10 / 1000</f>
+        <f t="shared" si="31"/>
         <v>46.752586205033197</v>
       </c>
       <c r="H10" s="5">
-        <f>AB10</f>
+        <f t="shared" si="32"/>
         <v>1.2046254778162599</v>
       </c>
       <c r="I10" s="9">
-        <f>Y10</f>
+        <f t="shared" si="33"/>
+        <v>2006.1488139017399</v>
+      </c>
+      <c r="J10" s="5">
+        <f t="shared" si="34"/>
+        <v>1.23942931432322</v>
+      </c>
+      <c r="K10" s="9">
+        <f t="shared" si="35"/>
         <v>152.236892425848</v>
       </c>
-      <c r="J10" s="5">
-        <f>AC10</f>
+      <c r="L10" s="5">
+        <f t="shared" si="36"/>
         <v>1.24493728747632</v>
       </c>
-      <c r="K10" s="7">
-        <f>-X10/1000000</f>
+      <c r="M10" s="7">
+        <f t="shared" si="37"/>
         <v>0.45964743191372803</v>
       </c>
-      <c r="L10" s="5">
-        <f>AD10</f>
+      <c r="N10" s="5">
+        <f t="shared" si="38"/>
         <v>1.3738522958958601</v>
       </c>
-      <c r="M10" s="7">
-        <f>Z10</f>
+      <c r="O10" s="7">
+        <f t="shared" si="39"/>
         <v>75.566553458173203</v>
       </c>
-      <c r="N10" s="7">
-        <f t="shared" si="13"/>
+      <c r="P10" s="7">
+        <f t="shared" si="40"/>
         <v>74.955966394291565</v>
       </c>
-      <c r="Q10" t="s">
+      <c r="Q10" s="3">
+        <f t="shared" si="27"/>
+        <v>23.304645139512122</v>
+      </c>
+      <c r="S10" t="s">
         <v>25</v>
       </c>
-      <c r="R10" t="s">
+      <c r="T10" t="s">
         <v>26</v>
       </c>
-      <c r="S10" t="s">
+      <c r="U10" t="s">
         <v>22</v>
       </c>
-      <c r="T10">
+      <c r="V10">
         <v>940569</v>
       </c>
-      <c r="U10">
+      <c r="W10">
         <v>344417.71727378899</v>
       </c>
-      <c r="V10">
+      <c r="X10">
         <v>46752.5862050332</v>
       </c>
-      <c r="W10">
+      <c r="Y10">
         <v>46752.5862050332</v>
       </c>
-      <c r="X10">
+      <c r="Z10">
+        <v>-2006.1488139017399</v>
+      </c>
+      <c r="AA10">
         <v>-459647.43191372801</v>
       </c>
-      <c r="Y10">
+      <c r="AB10">
         <v>152.236892425848</v>
       </c>
-      <c r="Z10">
+      <c r="AC10">
         <v>75.566553458173203</v>
       </c>
-      <c r="AA10">
+      <c r="AD10">
         <v>1.4092509556325299</v>
       </c>
-      <c r="AB10">
+      <c r="AE10">
         <v>1.2046254778162599</v>
       </c>
-      <c r="AC10">
+      <c r="AF10">
+        <v>1.23942931432322</v>
+      </c>
+      <c r="AG10">
         <v>1.24493728747632</v>
       </c>
-      <c r="AD10">
+      <c r="AH10">
         <v>1.3738522958958601</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="15"/>
-      <c r="C11" s="17"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="13"/>
       <c r="D11" s="9">
-        <f t="shared" si="14"/>
+        <f t="shared" si="28"/>
         <v>596.15128272620996</v>
       </c>
       <c r="E11" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="29"/>
         <v>80.923869008580112</v>
       </c>
       <c r="F11" s="5">
-        <f>AA11</f>
+        <f t="shared" si="30"/>
         <v>1.54092214367092</v>
       </c>
       <c r="G11" s="9">
-        <f>W11 / 1000</f>
+        <f t="shared" si="31"/>
         <v>80.923869008580112</v>
       </c>
       <c r="H11" s="5">
-        <f>AB11</f>
+        <f t="shared" si="32"/>
         <v>1.2704610718354601</v>
       </c>
       <c r="I11" s="9">
-        <f>Y11</f>
+        <f t="shared" si="33"/>
+        <v>2717.22961367896</v>
+      </c>
+      <c r="J11" s="5">
+        <f t="shared" si="34"/>
+        <v>1.2993501566676899</v>
+      </c>
+      <c r="K11" s="9">
+        <f t="shared" si="35"/>
         <v>341.30839104135401</v>
       </c>
-      <c r="J11" s="5">
-        <f>AC11</f>
+      <c r="L11" s="5">
+        <f t="shared" si="36"/>
         <v>1.32820420299369</v>
       </c>
-      <c r="K11" s="7">
-        <f>-X11/1000000</f>
+      <c r="M11" s="7">
+        <f t="shared" si="37"/>
         <v>1.0558372667459401</v>
       </c>
-      <c r="L11" s="5">
-        <f>AD11</f>
+      <c r="N11" s="5">
+        <f t="shared" si="38"/>
         <v>1.52138040680452</v>
       </c>
-      <c r="M11" s="7">
-        <f>Z11</f>
+      <c r="O11" s="7">
+        <f t="shared" si="39"/>
         <v>76.697980800319897</v>
       </c>
-      <c r="N11" s="7">
-        <f t="shared" si="13"/>
+      <c r="P11" s="7">
+        <f t="shared" si="40"/>
         <v>97.400250187460955</v>
       </c>
-      <c r="Q11" t="s">
+      <c r="Q11" s="3">
+        <f t="shared" si="27"/>
+        <v>29.781755874143524</v>
+      </c>
+      <c r="S11" t="s">
         <v>27</v>
       </c>
-      <c r="R11" t="s">
+      <c r="T11" t="s">
         <v>26</v>
       </c>
-      <c r="S11" t="s">
+      <c r="U11" t="s">
         <v>24</v>
       </c>
-      <c r="T11">
+      <c r="V11">
         <v>940569</v>
       </c>
-      <c r="U11">
+      <c r="W11">
         <v>596151.28272620996</v>
       </c>
-      <c r="V11">
+      <c r="X11">
         <v>80923.869008580106</v>
       </c>
-      <c r="W11">
+      <c r="Y11">
         <v>80923.869008580106</v>
       </c>
-      <c r="X11">
+      <c r="Z11">
+        <v>-2717.22961367896</v>
+      </c>
+      <c r="AA11">
         <v>-1055837.2667459401</v>
       </c>
-      <c r="Y11">
+      <c r="AB11">
         <v>341.30839104135401</v>
       </c>
-      <c r="Z11">
+      <c r="AC11">
         <v>76.697980800319897</v>
       </c>
-      <c r="AA11">
+      <c r="AD11">
         <v>1.54092214367092</v>
       </c>
-      <c r="AB11">
+      <c r="AE11">
         <v>1.2704610718354601</v>
       </c>
-      <c r="AC11">
+      <c r="AF11">
+        <v>1.2993501566676899</v>
+      </c>
+      <c r="AG11">
         <v>1.32820420299369</v>
       </c>
-      <c r="AD11">
+      <c r="AH11">
         <v>1.52138040680452</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>34</v>
       </c>
       <c r="B12" s="10" t="str">
-        <f>R12</f>
+        <f>T12</f>
         <v>[90,95)</v>
       </c>
       <c r="C12" s="11">
-        <f>T12/1000</f>
+        <f>V12/1000</f>
         <v>417.13799999999998</v>
       </c>
       <c r="D12" s="9">
-        <f t="shared" si="14"/>
+        <f t="shared" si="28"/>
         <v>417.13799999999998</v>
       </c>
       <c r="E12" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="29"/>
         <v>56.6239171978836</v>
       </c>
       <c r="F12" s="5">
-        <f>AA12</f>
+        <f t="shared" si="30"/>
         <v>1.63305489189682</v>
       </c>
       <c r="G12" s="9">
-        <f>W12 / 1000</f>
+        <f t="shared" si="31"/>
         <v>56.6239171978836</v>
       </c>
       <c r="H12" s="5">
-        <f>AB12</f>
+        <f t="shared" si="32"/>
         <v>1.31652744594841</v>
       </c>
       <c r="I12" s="9">
-        <f>Y12</f>
+        <f t="shared" si="33"/>
+        <v>1389.8661793003801</v>
+      </c>
+      <c r="J12" s="5">
+        <f t="shared" si="34"/>
+        <v>1.3299997387974101</v>
+      </c>
+      <c r="K12" s="9">
+        <f t="shared" si="35"/>
         <v>180.68788827103401</v>
       </c>
-      <c r="J12" s="5">
-        <f>AC12</f>
+      <c r="L12" s="5">
+        <f t="shared" si="36"/>
         <v>1.37228551925366</v>
       </c>
-      <c r="K12" s="7">
-        <f>-X12/1000000</f>
+      <c r="M12" s="7">
+        <f t="shared" si="37"/>
         <v>0.629616236097578</v>
       </c>
-      <c r="L12" s="5">
-        <f>AD12</f>
+      <c r="N12" s="5">
+        <f t="shared" si="38"/>
         <v>1.6093542800844001</v>
       </c>
-      <c r="M12" s="7">
-        <f>Z12</f>
+      <c r="O12" s="7">
+        <f t="shared" si="39"/>
         <v>76.636453798361202</v>
       </c>
-      <c r="N12" s="7">
-        <f t="shared" si="13"/>
+      <c r="P12" s="7">
+        <f t="shared" si="40"/>
         <v>74.939605232342714</v>
       </c>
-      <c r="Q12" t="s">
+      <c r="Q12" s="3">
+        <f t="shared" si="27"/>
+        <v>40.740553328944593</v>
+      </c>
+      <c r="S12" t="s">
         <v>27</v>
       </c>
-      <c r="R12" t="s">
+      <c r="T12" t="s">
         <v>28</v>
       </c>
-      <c r="S12" t="s">
+      <c r="U12" t="s">
         <v>24</v>
       </c>
-      <c r="T12">
+      <c r="V12">
         <v>417138</v>
       </c>
-      <c r="U12">
+      <c r="W12">
         <v>417138</v>
       </c>
-      <c r="V12">
+      <c r="X12">
         <v>56623.917197883602</v>
       </c>
-      <c r="W12">
+      <c r="Y12">
         <v>56623.917197883602</v>
       </c>
-      <c r="X12">
+      <c r="Z12">
+        <v>-1389.8661793003801</v>
+      </c>
+      <c r="AA12">
         <v>-629616.23609757796</v>
       </c>
-      <c r="Y12">
+      <c r="AB12">
         <v>180.68788827103401</v>
       </c>
-      <c r="Z12">
+      <c r="AC12">
         <v>76.636453798361202</v>
       </c>
-      <c r="AA12">
+      <c r="AD12">
         <v>1.63305489189682</v>
       </c>
-      <c r="AB12">
+      <c r="AE12">
         <v>1.31652744594841</v>
       </c>
-      <c r="AC12">
+      <c r="AF12">
+        <v>1.3299997387974101</v>
+      </c>
+      <c r="AG12">
         <v>1.37228551925366</v>
       </c>
-      <c r="AD12">
+      <c r="AH12">
         <v>1.6093542800844001</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="N13" s="7"/>
+    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="P13" s="7"/>
+      <c r="Q13" s="3"/>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A14" s="12" t="s">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="12"/>
-      <c r="L14" s="12"/>
-      <c r="M14" s="12"/>
-      <c r="N14" s="7"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="14"/>
+      <c r="N14" s="14"/>
+      <c r="O14" s="14"/>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="3"/>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="17">
+      <c r="C15" s="13">
         <v>1508.4970000000001</v>
       </c>
       <c r="D15" s="9">
-        <f t="shared" ref="D15:E19" si="15">U15/1000</f>
+        <f t="shared" ref="D15:E19" si="41">W15/1000</f>
         <v>1075.4017824339201</v>
       </c>
       <c r="E15" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" ref="E15" si="42">X15 / 1000</f>
         <v>154.05686067103699</v>
       </c>
       <c r="F15" s="5">
-        <f>AA15</f>
+        <f t="shared" ref="F15" si="43">AD15</f>
         <v>1.2506658433233</v>
       </c>
       <c r="G15" s="9">
-        <f>W15 / 1000</f>
+        <f t="shared" ref="G15" si="44">Y15 / 1000</f>
         <v>154.05686067103699</v>
       </c>
       <c r="H15" s="5">
-        <f>AB15</f>
+        <f t="shared" ref="H15" si="45">AE15</f>
         <v>1.1253329216616501</v>
       </c>
       <c r="I15" s="9">
-        <f>Y15</f>
+        <f t="shared" ref="I15" si="46">-Z15</f>
+        <v>7051.1535137497303</v>
+      </c>
+      <c r="J15" s="5">
+        <f t="shared" ref="J15" si="47">AF15</f>
+        <v>1.1554933215496499</v>
+      </c>
+      <c r="K15" s="9">
+        <f t="shared" ref="K15" si="48">AB15</f>
         <v>625.33754930004795</v>
       </c>
-      <c r="J15" s="5">
-        <f>AC15</f>
+      <c r="L15" s="5">
+        <f t="shared" ref="L15" si="49">AG15</f>
         <v>1.15255976780568</v>
       </c>
-      <c r="K15" s="7">
-        <f>-X15/1000000</f>
+      <c r="M15" s="7">
+        <f t="shared" ref="M15" si="50">-AA15/1000000</f>
         <v>1.5268275054167901</v>
       </c>
-      <c r="L15" s="5">
-        <f>AD15</f>
+      <c r="N15" s="5">
+        <f t="shared" ref="N15" si="51">AH15</f>
         <v>1.2133377790800199</v>
       </c>
-      <c r="M15" s="7">
-        <f>Z15</f>
+      <c r="O15" s="7">
+        <f t="shared" ref="O15" si="52">AC15</f>
         <v>74.585709366457493</v>
       </c>
-      <c r="N15" s="7">
-        <f t="shared" si="13"/>
+      <c r="P15" s="7">
+        <f>(K15 * 20 + M15 * 1000) /G15</f>
         <v>91.093499051523196</v>
       </c>
-      <c r="Q15" t="s">
+      <c r="Q15" s="3">
+        <f t="shared" ref="Q15:Q19" si="53">E15/I15*1000</f>
+        <v>21.848462151707025</v>
+      </c>
+      <c r="S15" t="s">
         <v>20</v>
       </c>
-      <c r="R15" t="s">
+      <c r="T15" t="s">
         <v>21</v>
       </c>
-      <c r="S15" t="s">
+      <c r="U15" t="s">
         <v>22</v>
       </c>
-      <c r="T15">
+      <c r="V15">
         <v>1508497</v>
       </c>
-      <c r="U15">
+      <c r="W15">
         <v>1075401.7824339201</v>
       </c>
-      <c r="V15">
+      <c r="X15">
         <v>154056.86067103699</v>
       </c>
-      <c r="W15">
+      <c r="Y15">
         <v>154056.86067103699</v>
       </c>
-      <c r="X15">
+      <c r="Z15">
+        <v>-7051.1535137497303</v>
+      </c>
+      <c r="AA15">
         <v>-1526827.50541679</v>
       </c>
-      <c r="Y15">
+      <c r="AB15">
         <v>625.33754930004795</v>
       </c>
-      <c r="Z15">
+      <c r="AC15">
         <v>74.585709366457493</v>
       </c>
-      <c r="AA15">
+      <c r="AD15">
         <v>1.2506658433233</v>
       </c>
-      <c r="AB15">
+      <c r="AE15">
         <v>1.1253329216616501</v>
       </c>
-      <c r="AC15">
+      <c r="AF15">
+        <v>1.1554933215496499</v>
+      </c>
+      <c r="AG15">
         <v>1.15255976780568</v>
       </c>
-      <c r="AD15">
+      <c r="AH15">
         <v>1.2133377790800199</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="15"/>
-      <c r="C16" s="17"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="13"/>
       <c r="D16" s="9">
-        <f t="shared" si="15"/>
+        <f t="shared" ref="D16:D19" si="54">W16/1000</f>
         <v>433.09521756606995</v>
       </c>
       <c r="E16" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" ref="E16:E19" si="55">X16 / 1000</f>
         <v>24.936483516051698</v>
       </c>
       <c r="F16" s="5">
-        <f>AA16</f>
+        <f t="shared" ref="F16:F19" si="56">AD16</f>
         <v>1.2912399835650401</v>
       </c>
       <c r="G16" s="9">
-        <f>W16 / 1000</f>
+        <f t="shared" ref="G16:G19" si="57">Y16 / 1000</f>
         <v>24.936483516051698</v>
       </c>
       <c r="H16" s="5">
-        <f>AB16</f>
+        <f t="shared" ref="H16:H19" si="58">AE16</f>
         <v>1.1456199917825201</v>
       </c>
       <c r="I16" s="9">
-        <f>Y16</f>
+        <f t="shared" ref="I16:I19" si="59">-Z16</f>
+        <v>1203.54318314784</v>
+      </c>
+      <c r="J16" s="5">
+        <f t="shared" ref="J16:J19" si="60">AF16</f>
+        <v>1.1820340750322</v>
+      </c>
+      <c r="K16" s="9">
+        <f t="shared" ref="K16:K19" si="61">AB16</f>
         <v>133.917266058618</v>
       </c>
-      <c r="J16" s="5">
-        <f>AC16</f>
+      <c r="L16" s="5">
+        <f t="shared" ref="L16:L19" si="62">AG16</f>
         <v>1.18523074212658</v>
       </c>
-      <c r="K16" s="7">
-        <f>-X16/1000000</f>
+      <c r="M16" s="7">
+        <f t="shared" ref="M16:M19" si="63">-AA16/1000000</f>
         <v>0.32656653907324101</v>
       </c>
-      <c r="L16" s="5">
-        <f>AD16</f>
+      <c r="N16" s="5">
+        <f t="shared" ref="N16:N19" si="64">AH16</f>
         <v>1.25896767500512</v>
       </c>
-      <c r="M16" s="7">
-        <f>Z16</f>
+      <c r="O16" s="7">
+        <f t="shared" ref="O16:O19" si="65">AC16</f>
         <v>75.398823493638503</v>
       </c>
-      <c r="N16" s="7">
-        <f t="shared" si="13"/>
+      <c r="P16" s="7">
+        <f t="shared" ref="P16:P19" si="66">(K16 * 20 + M16 * 1000) /G16</f>
         <v>120.5026305457756</v>
       </c>
-      <c r="Q16" t="s">
+      <c r="Q16" s="3">
+        <f t="shared" si="53"/>
+        <v>20.719226252298558</v>
+      </c>
+      <c r="S16" t="s">
         <v>23</v>
       </c>
-      <c r="R16" t="s">
+      <c r="T16" t="s">
         <v>21</v>
       </c>
-      <c r="S16" t="s">
+      <c r="U16" t="s">
         <v>24</v>
       </c>
-      <c r="T16">
+      <c r="V16">
         <v>1508497</v>
       </c>
-      <c r="U16">
+      <c r="W16">
         <v>433095.21756606997</v>
       </c>
-      <c r="V16">
+      <c r="X16">
         <v>24936.4835160517</v>
       </c>
-      <c r="W16">
+      <c r="Y16">
         <v>24936.4835160517</v>
       </c>
-      <c r="X16">
+      <c r="Z16">
+        <v>-1203.54318314784</v>
+      </c>
+      <c r="AA16">
         <v>-326566.539073241</v>
       </c>
-      <c r="Y16">
+      <c r="AB16">
         <v>133.917266058618</v>
       </c>
-      <c r="Z16">
+      <c r="AC16">
         <v>75.398823493638503</v>
       </c>
-      <c r="AA16">
+      <c r="AD16">
         <v>1.2912399835650401</v>
       </c>
-      <c r="AB16">
+      <c r="AE16">
         <v>1.1456199917825201</v>
       </c>
-      <c r="AC16">
+      <c r="AF16">
+        <v>1.1820340750322</v>
+      </c>
+      <c r="AG16">
         <v>1.18523074212658</v>
       </c>
-      <c r="AD16">
+      <c r="AH16">
         <v>1.25896767500512</v>
       </c>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="15" t="str">
-        <f t="shared" ref="B17" si="16">R15</f>
+      <c r="B17" s="12" t="str">
+        <f t="shared" ref="B17" si="67">T15</f>
         <v>[80,85)</v>
       </c>
-      <c r="C17" s="17">
+      <c r="C17" s="13">
         <v>940.56899999999996</v>
       </c>
       <c r="D17" s="9">
-        <f t="shared" si="15"/>
+        <f t="shared" si="54"/>
         <v>344.41771727378898</v>
       </c>
       <c r="E17" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="55"/>
         <v>0</v>
       </c>
       <c r="F17" s="5">
-        <f>AA17</f>
+        <f t="shared" si="56"/>
         <v>1.2912399835650401</v>
       </c>
       <c r="G17" s="9">
-        <f>W17 / 1000</f>
+        <f t="shared" si="57"/>
         <v>0</v>
       </c>
       <c r="H17" s="5">
-        <f>AB17</f>
+        <f t="shared" si="58"/>
         <v>1.1456199917825201</v>
       </c>
       <c r="I17" s="9">
-        <f>Y17</f>
+        <f t="shared" si="59"/>
         <v>0</v>
       </c>
       <c r="J17" s="5">
-        <f>AC17</f>
+        <f t="shared" si="60"/>
+        <v>1.1820340750322</v>
+      </c>
+      <c r="K17" s="9">
+        <f t="shared" si="61"/>
+        <v>0</v>
+      </c>
+      <c r="L17" s="5">
+        <f t="shared" si="62"/>
         <v>1.18523074212658</v>
       </c>
-      <c r="K17" s="7">
-        <f>-X17/1000000</f>
-        <v>0</v>
-      </c>
-      <c r="L17" s="5">
-        <f>AD17</f>
+      <c r="M17" s="7">
+        <f t="shared" si="63"/>
+        <v>0</v>
+      </c>
+      <c r="N17" s="5">
+        <f t="shared" si="64"/>
         <v>1.25896767500512</v>
       </c>
-      <c r="M17" s="7">
-        <f>Z17</f>
+      <c r="O17" s="7">
+        <f t="shared" si="65"/>
         <v>75.398823493638503</v>
       </c>
-      <c r="N17" s="7"/>
-      <c r="Q17" t="s">
+      <c r="P17" s="7" t="e">
+        <f t="shared" si="66"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q17" s="3" t="e">
+        <f t="shared" si="53"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S17" t="s">
         <v>25</v>
       </c>
-      <c r="R17" t="s">
+      <c r="T17" t="s">
         <v>26</v>
       </c>
-      <c r="S17" t="s">
+      <c r="U17" t="s">
         <v>22</v>
       </c>
-      <c r="T17">
+      <c r="V17">
         <v>940569</v>
       </c>
-      <c r="U17">
+      <c r="W17">
         <v>344417.71727378899</v>
       </c>
-      <c r="V17">
-        <v>0</v>
-      </c>
-      <c r="W17">
-        <v>0</v>
-      </c>
       <c r="X17">
         <v>0</v>
       </c>
@@ -1830,89 +2061,110 @@
         <v>0</v>
       </c>
       <c r="Z17">
+        <v>0</v>
+      </c>
+      <c r="AA17">
+        <v>0</v>
+      </c>
+      <c r="AB17">
+        <v>0</v>
+      </c>
+      <c r="AC17">
         <v>75.398823493638503</v>
       </c>
-      <c r="AA17">
+      <c r="AD17">
         <v>1.2912399835650401</v>
       </c>
-      <c r="AB17">
+      <c r="AE17">
         <v>1.1456199917825201</v>
       </c>
-      <c r="AC17">
+      <c r="AF17">
+        <v>1.1820340750322</v>
+      </c>
+      <c r="AG17">
         <v>1.18523074212658</v>
       </c>
-      <c r="AD17">
+      <c r="AH17">
         <v>1.25896767500512</v>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="15"/>
-      <c r="C18" s="17"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="13"/>
       <c r="D18" s="9">
-        <f t="shared" si="15"/>
+        <f t="shared" si="54"/>
         <v>596.15128272620996</v>
       </c>
       <c r="E18" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="55"/>
         <v>0</v>
       </c>
       <c r="F18" s="5">
-        <f>AA18</f>
+        <f t="shared" si="56"/>
         <v>1.2912399835650401</v>
       </c>
       <c r="G18" s="9">
-        <f>W18 / 1000</f>
+        <f t="shared" si="57"/>
         <v>0</v>
       </c>
       <c r="H18" s="5">
-        <f>AB18</f>
+        <f t="shared" si="58"/>
         <v>1.1456199917825201</v>
       </c>
       <c r="I18" s="9">
-        <f>Y18</f>
+        <f t="shared" si="59"/>
         <v>0</v>
       </c>
       <c r="J18" s="5">
-        <f>AC18</f>
+        <f t="shared" si="60"/>
+        <v>1.1820340750322</v>
+      </c>
+      <c r="K18" s="9">
+        <f t="shared" si="61"/>
+        <v>0</v>
+      </c>
+      <c r="L18" s="5">
+        <f t="shared" si="62"/>
         <v>1.18523074212658</v>
       </c>
-      <c r="K18" s="7">
-        <f>-X18/1000000</f>
-        <v>0</v>
-      </c>
-      <c r="L18" s="5">
-        <f>AD18</f>
+      <c r="M18" s="7">
+        <f t="shared" si="63"/>
+        <v>0</v>
+      </c>
+      <c r="N18" s="5">
+        <f t="shared" si="64"/>
         <v>1.25896767500512</v>
       </c>
-      <c r="M18" s="7">
-        <f>Z18</f>
+      <c r="O18" s="7">
+        <f t="shared" si="65"/>
         <v>75.398823493638503</v>
       </c>
-      <c r="N18" s="7"/>
-      <c r="Q18" t="s">
+      <c r="P18" s="7" t="e">
+        <f t="shared" si="66"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q18" s="3" t="e">
+        <f t="shared" si="53"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S18" t="s">
         <v>27</v>
       </c>
-      <c r="R18" t="s">
+      <c r="T18" t="s">
         <v>26</v>
       </c>
-      <c r="S18" t="s">
+      <c r="U18" t="s">
         <v>24</v>
       </c>
-      <c r="T18">
+      <c r="V18">
         <v>940569</v>
       </c>
-      <c r="U18">
+      <c r="W18">
         <v>596151.28272620996</v>
       </c>
-      <c r="V18">
-        <v>0</v>
-      </c>
-      <c r="W18">
-        <v>0</v>
-      </c>
       <c r="X18">
         <v>0</v>
       </c>
@@ -1920,94 +2172,115 @@
         <v>0</v>
       </c>
       <c r="Z18">
+        <v>0</v>
+      </c>
+      <c r="AA18">
+        <v>0</v>
+      </c>
+      <c r="AB18">
+        <v>0</v>
+      </c>
+      <c r="AC18">
         <v>75.398823493638503</v>
       </c>
-      <c r="AA18">
+      <c r="AD18">
         <v>1.2912399835650401</v>
       </c>
-      <c r="AB18">
+      <c r="AE18">
         <v>1.1456199917825201</v>
       </c>
-      <c r="AC18">
+      <c r="AF18">
+        <v>1.1820340750322</v>
+      </c>
+      <c r="AG18">
         <v>1.18523074212658</v>
       </c>
-      <c r="AD18">
+      <c r="AH18">
         <v>1.25896767500512</v>
       </c>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>34</v>
       </c>
       <c r="B19" s="10" t="str">
-        <f t="shared" ref="B19" si="17">R17</f>
+        <f t="shared" ref="B19" si="68">T17</f>
         <v>[85,90)</v>
       </c>
       <c r="C19" s="11">
         <v>417.13799999999998</v>
       </c>
       <c r="D19" s="9">
-        <f t="shared" si="15"/>
+        <f t="shared" si="54"/>
         <v>417.13799999999998</v>
       </c>
       <c r="E19" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="55"/>
         <v>0</v>
       </c>
       <c r="F19" s="5">
-        <f>AA19</f>
+        <f t="shared" si="56"/>
         <v>1.2912399835650401</v>
       </c>
       <c r="G19" s="9">
-        <f>W19 / 1000</f>
+        <f t="shared" si="57"/>
         <v>0</v>
       </c>
       <c r="H19" s="5">
-        <f>AB19</f>
+        <f t="shared" si="58"/>
         <v>1.1456199917825201</v>
       </c>
       <c r="I19" s="9">
-        <f>Y19</f>
+        <f t="shared" si="59"/>
         <v>0</v>
       </c>
       <c r="J19" s="5">
-        <f>AC19</f>
+        <f t="shared" si="60"/>
+        <v>1.1820340750322</v>
+      </c>
+      <c r="K19" s="9">
+        <f t="shared" si="61"/>
+        <v>0</v>
+      </c>
+      <c r="L19" s="5">
+        <f t="shared" si="62"/>
         <v>1.18523074212658</v>
       </c>
-      <c r="K19" s="7">
-        <f>-X19/1000000</f>
-        <v>0</v>
-      </c>
-      <c r="L19" s="5">
-        <f>AD19</f>
+      <c r="M19" s="7">
+        <f t="shared" si="63"/>
+        <v>0</v>
+      </c>
+      <c r="N19" s="5">
+        <f t="shared" si="64"/>
         <v>1.25896767500512</v>
       </c>
-      <c r="M19" s="7">
-        <f>Z19</f>
+      <c r="O19" s="7">
+        <f t="shared" si="65"/>
         <v>75.398823493638503</v>
       </c>
-      <c r="N19" s="7"/>
-      <c r="Q19" t="s">
+      <c r="P19" s="7" t="e">
+        <f t="shared" si="66"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q19" s="3" t="e">
+        <f t="shared" si="53"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S19" t="s">
         <v>27</v>
       </c>
-      <c r="R19" t="s">
+      <c r="T19" t="s">
         <v>28</v>
       </c>
-      <c r="S19" t="s">
+      <c r="U19" t="s">
         <v>24</v>
       </c>
-      <c r="T19">
+      <c r="V19">
         <v>417138</v>
       </c>
-      <c r="U19">
+      <c r="W19">
         <v>417138</v>
       </c>
-      <c r="V19">
-        <v>0</v>
-      </c>
-      <c r="W19">
-        <v>0</v>
-      </c>
       <c r="X19">
         <v>0</v>
       </c>
@@ -2015,522 +2288,628 @@
         <v>0</v>
       </c>
       <c r="Z19">
+        <v>0</v>
+      </c>
+      <c r="AA19">
+        <v>0</v>
+      </c>
+      <c r="AB19">
+        <v>0</v>
+      </c>
+      <c r="AC19">
         <v>75.398823493638503</v>
       </c>
-      <c r="AA19">
+      <c r="AD19">
         <v>1.2912399835650401</v>
       </c>
-      <c r="AB19">
+      <c r="AE19">
         <v>1.1456199917825201</v>
       </c>
-      <c r="AC19">
+      <c r="AF19">
+        <v>1.1820340750322</v>
+      </c>
+      <c r="AG19">
         <v>1.18523074212658</v>
       </c>
-      <c r="AD19">
+      <c r="AH19">
         <v>1.25896767500512</v>
       </c>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="N20" s="7"/>
+    <row r="20" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="P20" s="7"/>
+      <c r="Q20" s="3"/>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A21" s="12" t="s">
+    <row r="21" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A21" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="B21" s="12"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="12"/>
-      <c r="J21" s="12"/>
-      <c r="K21" s="12"/>
-      <c r="L21" s="12"/>
-      <c r="M21" s="12"/>
-      <c r="N21" s="7"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="14"/>
+      <c r="K21" s="14"/>
+      <c r="L21" s="14"/>
+      <c r="M21" s="14"/>
+      <c r="N21" s="14"/>
+      <c r="O21" s="14"/>
+      <c r="P21" s="7"/>
+      <c r="Q21" s="3"/>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>33</v>
       </c>
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="17">
+      <c r="C22" s="13">
         <v>1508.4970000000001</v>
       </c>
       <c r="D22" s="9">
-        <f t="shared" ref="D22:E26" si="18">U22/1000</f>
-        <v>1075.4017824339201</v>
+        <f t="shared" ref="D22:D26" si="69">W22/1000</f>
+        <v>1075.4017819999999</v>
       </c>
       <c r="E22" s="3">
-        <f t="shared" si="18"/>
-        <v>256.661789483196</v>
+        <f t="shared" ref="E22:E26" si="70">X22 / 1000</f>
+        <v>256.6617895</v>
       </c>
       <c r="F22" s="5">
-        <f>AA22</f>
-        <v>1.4176142732588399</v>
+        <f t="shared" ref="F22:F26" si="71">AD22</f>
+        <v>1.4176142730000001</v>
       </c>
       <c r="G22" s="9">
-        <f>W22 / 1000</f>
-        <v>256.661789483196</v>
+        <f t="shared" ref="G22:G26" si="72">Y22 / 1000</f>
+        <v>256.6617895</v>
       </c>
       <c r="H22" s="5">
-        <f>AB22</f>
-        <v>1.20880713662942</v>
+        <f t="shared" ref="H22:H26" si="73">AE22</f>
+        <v>1.208807137</v>
       </c>
       <c r="I22" s="9">
-        <f>Y22</f>
-        <v>1003.24543514224</v>
+        <f t="shared" ref="I22:I26" si="74">-Z22</f>
+        <v>11354.85009</v>
       </c>
       <c r="J22" s="5">
-        <f>AC22</f>
-        <v>1.24475563766918</v>
-      </c>
-      <c r="K22" s="7">
-        <f>-X22/1000000</f>
-        <v>2.5278106303732799</v>
+        <f t="shared" ref="J22:J26" si="75">AF22</f>
+        <v>1.250399222</v>
+      </c>
+      <c r="K22" s="9">
+        <f t="shared" ref="K22:K26" si="76">AB22</f>
+        <v>1003.245435</v>
       </c>
       <c r="L22" s="5">
-        <f>AD22</f>
-        <v>1.35320133014732</v>
+        <f t="shared" ref="L22:L26" si="77">AG22</f>
+        <v>1.244755638</v>
       </c>
       <c r="M22" s="7">
-        <f>Z22</f>
-        <v>75.195652340758002</v>
-      </c>
-      <c r="N22" s="7">
-        <f t="shared" si="13"/>
-        <v>88.025254474808591</v>
-      </c>
-      <c r="Q22" t="s">
+        <f t="shared" ref="M22:M26" si="78">-AA22/1000000</f>
+        <v>2.5278106299999998</v>
+      </c>
+      <c r="N22" s="5">
+        <f t="shared" ref="N22:N26" si="79">AH22</f>
+        <v>1.3532013300000001</v>
+      </c>
+      <c r="O22" s="7">
+        <f t="shared" ref="O22:O26" si="80">AC22</f>
+        <v>75.195652339999995</v>
+      </c>
+      <c r="P22" s="7">
+        <f>(K22 * 20 + M22 * 1000) /G22</f>
+        <v>88.025254456507241</v>
+      </c>
+      <c r="Q22" s="3">
+        <f t="shared" ref="Q22:Q26" si="81">E22/I22*1000</f>
+        <v>22.603714489021495</v>
+      </c>
+      <c r="S22" t="s">
         <v>20</v>
       </c>
-      <c r="R22" t="s">
+      <c r="T22" t="s">
         <v>21</v>
       </c>
-      <c r="S22" t="s">
+      <c r="U22" t="s">
         <v>22</v>
       </c>
-      <c r="T22">
+      <c r="V22">
         <v>1508497</v>
       </c>
-      <c r="U22">
-        <v>1075401.7824339201</v>
-      </c>
-      <c r="V22">
-        <v>256661.78948319599</v>
-      </c>
       <c r="W22">
-        <v>256661.78948319599</v>
+        <v>1075401.7819999999</v>
       </c>
       <c r="X22">
-        <v>-2527810.63037328</v>
+        <v>256661.78950000001</v>
       </c>
       <c r="Y22">
-        <v>1003.24543514224</v>
+        <v>256661.78950000001</v>
       </c>
       <c r="Z22">
-        <v>75.195652340758002</v>
+        <v>-11354.85009</v>
       </c>
       <c r="AA22">
-        <v>1.4176142732588399</v>
+        <v>-2527810.63</v>
       </c>
       <c r="AB22">
-        <v>1.20880713662942</v>
+        <v>1003.245435</v>
       </c>
       <c r="AC22">
-        <v>1.24475563766918</v>
+        <v>75.195652339999995</v>
       </c>
       <c r="AD22">
-        <v>1.35320133014732</v>
+        <v>1.4176142730000001</v>
+      </c>
+      <c r="AE22">
+        <v>1.208807137</v>
+      </c>
+      <c r="AF22">
+        <v>1.250399222</v>
+      </c>
+      <c r="AG22">
+        <v>1.244755638</v>
+      </c>
+      <c r="AH22">
+        <v>1.3532013300000001</v>
       </c>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>34</v>
       </c>
-      <c r="B23" s="15"/>
-      <c r="C23" s="17"/>
+      <c r="B23" s="12"/>
+      <c r="C23" s="13"/>
       <c r="D23" s="9">
-        <f t="shared" si="18"/>
-        <v>433.09521756606995</v>
+        <f t="shared" si="69"/>
+        <v>433.09521759999996</v>
       </c>
       <c r="E23" s="3">
-        <f t="shared" si="18"/>
-        <v>76.705702678003306</v>
+        <f t="shared" si="70"/>
+        <v>76.705702680000002</v>
       </c>
       <c r="F23" s="5">
-        <f>AA23</f>
-        <v>1.54242208490538</v>
+        <f t="shared" si="71"/>
+        <v>1.5424220850000001</v>
       </c>
       <c r="G23" s="9">
-        <f>W23 / 1000</f>
-        <v>76.705702678003306</v>
+        <f t="shared" si="72"/>
+        <v>76.705702680000002</v>
       </c>
       <c r="H23" s="5">
-        <f>AB23</f>
-        <v>1.2712110424526899</v>
+        <f t="shared" si="73"/>
+        <v>1.271211042</v>
       </c>
       <c r="I23" s="9">
-        <f>Y23</f>
-        <v>393.99658336326797</v>
+        <f t="shared" si="74"/>
+        <v>3427.0105130000002</v>
       </c>
       <c r="J23" s="5">
-        <f>AC23</f>
-        <v>1.3408765684231601</v>
-      </c>
-      <c r="K23" s="7">
-        <f>-X23/1000000</f>
-        <v>1.01972504077478</v>
+        <f t="shared" si="75"/>
+        <v>1.3259722819999999</v>
+      </c>
+      <c r="K23" s="9">
+        <f t="shared" si="76"/>
+        <v>393.99658340000002</v>
       </c>
       <c r="L23" s="5">
-        <f>AD23</f>
-        <v>1.4956836175696899</v>
+        <f t="shared" si="77"/>
+        <v>1.3408765680000001</v>
       </c>
       <c r="M23" s="7">
-        <f>Z23</f>
-        <v>77.199891657303397</v>
-      </c>
-      <c r="N23" s="7">
-        <f t="shared" si="13"/>
-        <v>116.02340370179897</v>
-      </c>
-      <c r="Q23" t="s">
+        <f t="shared" si="78"/>
+        <v>1.0197250410000001</v>
+      </c>
+      <c r="N23" s="5">
+        <f t="shared" si="79"/>
+        <v>1.4956836179999999</v>
+      </c>
+      <c r="O23" s="7">
+        <f t="shared" si="80"/>
+        <v>77.199891660000006</v>
+      </c>
+      <c r="P23" s="7">
+        <f t="shared" ref="P23:P26" si="82">(K23 * 20 + M23 * 1000) /G23</f>
+        <v>116.02340371129236</v>
+      </c>
+      <c r="Q23" s="3">
+        <f t="shared" si="81"/>
+        <v>22.382686714565089</v>
+      </c>
+      <c r="S23" t="s">
         <v>23</v>
       </c>
-      <c r="R23" t="s">
+      <c r="T23" t="s">
         <v>21</v>
       </c>
-      <c r="S23" t="s">
+      <c r="U23" t="s">
         <v>24</v>
       </c>
-      <c r="T23">
+      <c r="V23">
         <v>1508497</v>
       </c>
-      <c r="U23">
-        <v>433095.21756606997</v>
-      </c>
-      <c r="V23">
-        <v>76705.702678003305</v>
-      </c>
       <c r="W23">
-        <v>76705.702678003305</v>
+        <v>433095.21759999997</v>
       </c>
       <c r="X23">
-        <v>-1019725.04077478</v>
+        <v>76705.702680000002</v>
       </c>
       <c r="Y23">
-        <v>393.99658336326797</v>
+        <v>76705.702680000002</v>
       </c>
       <c r="Z23">
-        <v>77.199891657303397</v>
+        <v>-3427.0105130000002</v>
       </c>
       <c r="AA23">
-        <v>1.54242208490538</v>
+        <v>-1019725.041</v>
       </c>
       <c r="AB23">
-        <v>1.2712110424526899</v>
+        <v>393.99658340000002</v>
       </c>
       <c r="AC23">
-        <v>1.3408765684231601</v>
+        <v>77.199891660000006</v>
       </c>
       <c r="AD23">
-        <v>1.4956836175696899</v>
+        <v>1.5424220850000001</v>
+      </c>
+      <c r="AE23">
+        <v>1.271211042</v>
+      </c>
+      <c r="AF23">
+        <v>1.3259722819999999</v>
+      </c>
+      <c r="AG23">
+        <v>1.3408765680000001</v>
+      </c>
+      <c r="AH23">
+        <v>1.4956836179999999</v>
       </c>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>33</v>
       </c>
-      <c r="B24" s="15" t="str">
-        <f t="shared" ref="B24" si="19">R22</f>
+      <c r="B24" s="12" t="str">
+        <f t="shared" ref="B24" si="83">T22</f>
         <v>[80,85)</v>
       </c>
-      <c r="C24" s="17">
+      <c r="C24" s="13">
         <v>940.56899999999996</v>
       </c>
       <c r="D24" s="9">
-        <f t="shared" si="18"/>
-        <v>344.41771727378898</v>
+        <f t="shared" si="69"/>
+        <v>344.41771729999999</v>
       </c>
       <c r="E24" s="3">
-        <f t="shared" si="18"/>
-        <v>46.752586205033197</v>
+        <f t="shared" si="70"/>
+        <v>46.752586210000004</v>
       </c>
       <c r="F24" s="5">
-        <f>AA24</f>
-        <v>1.61849319525765</v>
+        <f t="shared" si="71"/>
+        <v>1.6184931950000001</v>
       </c>
       <c r="G24" s="9">
-        <f>W24 / 1000</f>
-        <v>46.752586205033197</v>
+        <f t="shared" si="72"/>
+        <v>46.752586210000004</v>
       </c>
       <c r="H24" s="5">
-        <f>AB24</f>
-        <v>1.3092465976288199</v>
+        <f t="shared" si="73"/>
+        <v>1.3092465980000001</v>
       </c>
       <c r="I24" s="9">
-        <f>Y24</f>
-        <v>152.236892425848</v>
+        <f t="shared" si="74"/>
+        <v>2006.1488139999999</v>
       </c>
       <c r="J24" s="5">
-        <f>AC24</f>
-        <v>1.3780168696667801</v>
-      </c>
-      <c r="K24" s="7">
-        <f>-X24/1000000</f>
-        <v>0.45964743191372803</v>
+        <f t="shared" si="75"/>
+        <v>1.3702122409999999</v>
+      </c>
+      <c r="K24" s="9">
+        <f t="shared" si="76"/>
+        <v>152.23689239999999</v>
       </c>
       <c r="L24" s="5">
-        <f>AD24</f>
-        <v>1.5599083986510001</v>
+        <f t="shared" si="77"/>
+        <v>1.3780168699999999</v>
       </c>
       <c r="M24" s="7">
-        <f>Z24</f>
-        <v>77.134702300839194</v>
-      </c>
-      <c r="N24" s="7">
-        <f t="shared" si="13"/>
-        <v>74.955966394291565</v>
-      </c>
-      <c r="Q24" t="s">
+        <f t="shared" si="78"/>
+        <v>0.45964743190000001</v>
+      </c>
+      <c r="N24" s="5">
+        <f t="shared" si="79"/>
+        <v>1.559908399</v>
+      </c>
+      <c r="O24" s="7">
+        <f t="shared" si="80"/>
+        <v>77.134702300000001</v>
+      </c>
+      <c r="P24" s="7">
+        <f t="shared" si="82"/>
+        <v>74.95596637497755</v>
+      </c>
+      <c r="Q24" s="3">
+        <f t="shared" si="81"/>
+        <v>23.304645140846468</v>
+      </c>
+      <c r="S24" t="s">
         <v>25</v>
       </c>
-      <c r="R24" t="s">
+      <c r="T24" t="s">
         <v>26</v>
       </c>
-      <c r="S24" t="s">
+      <c r="U24" t="s">
         <v>22</v>
       </c>
-      <c r="T24">
+      <c r="V24">
         <v>940569</v>
       </c>
-      <c r="U24">
-        <v>344417.71727378899</v>
-      </c>
-      <c r="V24">
-        <v>46752.5862050332</v>
-      </c>
       <c r="W24">
-        <v>46752.5862050332</v>
+        <v>344417.71730000002</v>
       </c>
       <c r="X24">
-        <v>-459647.43191372801</v>
+        <v>46752.586210000001</v>
       </c>
       <c r="Y24">
-        <v>152.236892425848</v>
+        <v>46752.586210000001</v>
       </c>
       <c r="Z24">
-        <v>77.134702300839194</v>
+        <v>-2006.1488139999999</v>
       </c>
       <c r="AA24">
-        <v>1.61849319525765</v>
+        <v>-459647.43190000003</v>
       </c>
       <c r="AB24">
-        <v>1.3092465976288199</v>
+        <v>152.23689239999999</v>
       </c>
       <c r="AC24">
-        <v>1.3780168696667801</v>
+        <v>77.134702300000001</v>
       </c>
       <c r="AD24">
-        <v>1.5599083986510001</v>
+        <v>1.6184931950000001</v>
+      </c>
+      <c r="AE24">
+        <v>1.3092465980000001</v>
+      </c>
+      <c r="AF24">
+        <v>1.3702122409999999</v>
+      </c>
+      <c r="AG24">
+        <v>1.3780168699999999</v>
+      </c>
+      <c r="AH24">
+        <v>1.559908399</v>
       </c>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>34</v>
       </c>
-      <c r="B25" s="15"/>
-      <c r="C25" s="17"/>
+      <c r="B25" s="12"/>
+      <c r="C25" s="13"/>
       <c r="D25" s="9">
-        <f t="shared" si="18"/>
-        <v>596.15128272620996</v>
+        <f t="shared" si="69"/>
+        <v>596.15128270000002</v>
       </c>
       <c r="E25" s="3">
-        <f t="shared" si="18"/>
-        <v>80.923869008580112</v>
+        <f t="shared" si="70"/>
+        <v>80.92386900999999</v>
       </c>
       <c r="F25" s="5">
-        <f>AA25</f>
-        <v>1.7501643832960401</v>
+        <f t="shared" si="71"/>
+        <v>1.750164383</v>
       </c>
       <c r="G25" s="9">
-        <f>W25 / 1000</f>
-        <v>80.923869008580112</v>
+        <f t="shared" si="72"/>
+        <v>80.92386900999999</v>
       </c>
       <c r="H25" s="5">
-        <f>AB25</f>
-        <v>1.37508219164802</v>
+        <f t="shared" si="73"/>
+        <v>1.375082192</v>
       </c>
       <c r="I25" s="9">
-        <f>Y25</f>
-        <v>341.30839104135401</v>
+        <f t="shared" si="74"/>
+        <v>2717.2296139999999</v>
       </c>
       <c r="J25" s="5">
-        <f>AC25</f>
-        <v>1.46128378518414</v>
-      </c>
-      <c r="K25" s="7">
-        <f>-X25/1000000</f>
-        <v>1.0558372667459401</v>
+        <f t="shared" si="75"/>
+        <v>1.4301330839999999</v>
+      </c>
+      <c r="K25" s="9">
+        <f t="shared" si="76"/>
+        <v>341.30839099999997</v>
       </c>
       <c r="L25" s="5">
-        <f>AD25</f>
-        <v>1.70743650955965</v>
+        <f t="shared" si="77"/>
+        <v>1.461283785</v>
       </c>
       <c r="M25" s="7">
-        <f>Z25</f>
-        <v>78.104967490326601</v>
-      </c>
-      <c r="N25" s="7">
-        <f t="shared" si="13"/>
-        <v>97.400250187460955</v>
-      </c>
-      <c r="Q25" t="s">
+        <f t="shared" si="78"/>
+        <v>1.055837267</v>
+      </c>
+      <c r="N25" s="5">
+        <f t="shared" si="79"/>
+        <v>1.70743651</v>
+      </c>
+      <c r="O25" s="7">
+        <f t="shared" si="80"/>
+        <v>78.104967490000007</v>
+      </c>
+      <c r="P25" s="7">
+        <f t="shared" si="82"/>
+        <v>97.400250178670987</v>
+      </c>
+      <c r="Q25" s="3">
+        <f t="shared" si="81"/>
+        <v>29.781755871147364</v>
+      </c>
+      <c r="S25" t="s">
         <v>27</v>
       </c>
-      <c r="R25" t="s">
+      <c r="T25" t="s">
         <v>26</v>
       </c>
-      <c r="S25" t="s">
+      <c r="U25" t="s">
         <v>24</v>
       </c>
-      <c r="T25">
+      <c r="V25">
         <v>940569</v>
       </c>
-      <c r="U25">
-        <v>596151.28272620996</v>
-      </c>
-      <c r="V25">
-        <v>80923.869008580106</v>
-      </c>
       <c r="W25">
-        <v>80923.869008580106</v>
+        <v>596151.28269999998</v>
       </c>
       <c r="X25">
-        <v>-1055837.2667459401</v>
+        <v>80923.869009999995</v>
       </c>
       <c r="Y25">
-        <v>341.30839104135401</v>
+        <v>80923.869009999995</v>
       </c>
       <c r="Z25">
-        <v>78.104967490326601</v>
+        <v>-2717.2296139999999</v>
       </c>
       <c r="AA25">
-        <v>1.7501643832960401</v>
+        <v>-1055837.267</v>
       </c>
       <c r="AB25">
-        <v>1.37508219164802</v>
+        <v>341.30839099999997</v>
       </c>
       <c r="AC25">
-        <v>1.46128378518414</v>
+        <v>78.104967490000007</v>
       </c>
       <c r="AD25">
-        <v>1.70743650955965</v>
+        <v>1.750164383</v>
+      </c>
+      <c r="AE25">
+        <v>1.375082192</v>
+      </c>
+      <c r="AF25">
+        <v>1.4301330839999999</v>
+      </c>
+      <c r="AG25">
+        <v>1.461283785</v>
+      </c>
+      <c r="AH25">
+        <v>1.70743651</v>
       </c>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>34</v>
       </c>
       <c r="B26" s="10" t="str">
-        <f t="shared" ref="B26" si="20">R24</f>
+        <f t="shared" ref="B26" si="84">T24</f>
         <v>[85,90)</v>
       </c>
       <c r="C26" s="11">
         <v>417.13799999999998</v>
       </c>
       <c r="D26" s="9">
-        <f t="shared" si="18"/>
+        <f t="shared" si="69"/>
         <v>417.13799999999998</v>
       </c>
       <c r="E26" s="3">
-        <f t="shared" si="18"/>
-        <v>56.6239171978836</v>
+        <f t="shared" si="70"/>
+        <v>56.623917200000001</v>
       </c>
       <c r="F26" s="5">
-        <f>AA26</f>
-        <v>1.8422971315219401</v>
+        <f t="shared" si="71"/>
+        <v>1.8422971319999999</v>
       </c>
       <c r="G26" s="9">
-        <f>W26 / 1000</f>
-        <v>56.6239171978836</v>
+        <f t="shared" si="72"/>
+        <v>56.623917200000001</v>
       </c>
       <c r="H26" s="5">
-        <f>AB26</f>
-        <v>1.4211485657609699</v>
+        <f t="shared" si="73"/>
+        <v>1.4211485660000001</v>
       </c>
       <c r="I26" s="9">
-        <f>Y26</f>
-        <v>180.68788827103401</v>
+        <f t="shared" si="74"/>
+        <v>1389.8661790000001</v>
       </c>
       <c r="J26" s="5">
-        <f>AC26</f>
-        <v>1.5053651014441101</v>
-      </c>
-      <c r="K26" s="7">
-        <f>-X26/1000000</f>
-        <v>0.629616236097578</v>
+        <f t="shared" si="75"/>
+        <v>1.4607826660000001</v>
+      </c>
+      <c r="K26" s="9">
+        <f t="shared" si="76"/>
+        <v>180.6878883</v>
       </c>
       <c r="L26" s="5">
-        <f>AD26</f>
-        <v>1.79541038283954</v>
+        <f t="shared" si="77"/>
+        <v>1.505365101</v>
       </c>
       <c r="M26" s="7">
-        <f>Z26</f>
-        <v>78.002362621636394</v>
-      </c>
-      <c r="N26" s="7">
-        <f t="shared" si="13"/>
-        <v>74.939605232342714</v>
-      </c>
-      <c r="Q26" t="s">
+        <f t="shared" si="78"/>
+        <v>0.62961623609999995</v>
+      </c>
+      <c r="N26" s="5">
+        <f t="shared" si="79"/>
+        <v>1.7954103830000001</v>
+      </c>
+      <c r="O26" s="7">
+        <f t="shared" si="80"/>
+        <v>78.00236262</v>
+      </c>
+      <c r="P26" s="7">
+        <f t="shared" si="82"/>
+        <v>74.939605239815506</v>
+      </c>
+      <c r="Q26" s="3">
+        <f t="shared" si="81"/>
+        <v>40.740553339272239</v>
+      </c>
+      <c r="S26" t="s">
         <v>27</v>
       </c>
-      <c r="R26" t="s">
+      <c r="T26" t="s">
         <v>28</v>
       </c>
-      <c r="S26" t="s">
+      <c r="U26" t="s">
         <v>24</v>
       </c>
-      <c r="T26">
+      <c r="V26">
         <v>417138</v>
       </c>
-      <c r="U26">
+      <c r="W26">
         <v>417138</v>
       </c>
-      <c r="V26">
-        <v>56623.917197883602</v>
-      </c>
-      <c r="W26">
-        <v>56623.917197883602</v>
-      </c>
       <c r="X26">
-        <v>-629616.23609757796</v>
+        <v>56623.917200000004</v>
       </c>
       <c r="Y26">
-        <v>180.68788827103401</v>
+        <v>56623.917200000004</v>
       </c>
       <c r="Z26">
-        <v>78.002362621636394</v>
+        <v>-1389.8661790000001</v>
       </c>
       <c r="AA26">
-        <v>1.8422971315219401</v>
+        <v>-629616.23609999998</v>
       </c>
       <c r="AB26">
-        <v>1.4211485657609699</v>
+        <v>180.6878883</v>
       </c>
       <c r="AC26">
-        <v>1.5053651014441101</v>
+        <v>78.00236262</v>
       </c>
       <c r="AD26">
-        <v>1.79541038283954</v>
+        <v>1.8422971319999999</v>
+      </c>
+      <c r="AE26">
+        <v>1.4211485660000001</v>
+      </c>
+      <c r="AF26">
+        <v>1.4607826660000001</v>
+      </c>
+      <c r="AG26">
+        <v>1.505365101</v>
+      </c>
+      <c r="AH26">
+        <v>1.7954103830000001</v>
       </c>
     </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:34" x14ac:dyDescent="0.25">
       <c r="D29" s="9">
         <f>SUM(D3:D5)</f>
         <v>2168.6131270308952</v>
@@ -2543,27 +2922,21 @@
         <f>SUM(G3:G5)</f>
         <v>1229.1811172081859</v>
       </c>
-      <c r="I29" s="9">
-        <f>SUM(I3:I5)</f>
-        <v>4098.9676262258126</v>
-      </c>
       <c r="K29" s="9">
         <f>SUM(K3:K5)</f>
+        <v>4098.9676262258126</v>
+      </c>
+      <c r="M29" s="9">
+        <f>SUM(M3:M5)</f>
         <v>7.1568547868121879</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="20">
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="A14:M14"/>
-    <mergeCell ref="A21:M21"/>
+  <mergeCells count="21">
+    <mergeCell ref="A14:O14"/>
+    <mergeCell ref="A21:O21"/>
+    <mergeCell ref="M1:N1"/>
     <mergeCell ref="K1:L1"/>
-    <mergeCell ref="I1:J1"/>
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="B17:B18"/>
     <mergeCell ref="E1:F1"/>
@@ -2572,9 +2945,17 @@
     <mergeCell ref="C10:C11"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="B8:B9"/>
-    <mergeCell ref="A7:M7"/>
+    <mergeCell ref="A7:O7"/>
     <mergeCell ref="A4:A5"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="C24:C25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add results with population norm
</commit_message>
<xml_diff>
--- a/docs/tabs/Tab_ProgrammeProfile.xlsx
+++ b/docs/tabs/Tab_ProgrammeProfile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\HPRU\Shingrix\HPRU_RZV\docs\tabs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0459337C-0DEA-422C-99FB-83027E8F584B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1718D0B-2128-42EA-A6D9-A6AC582DBEA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="5265" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -165,21 +165,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Additional eligibility 3: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Those who reach age 80 years be called in on 80th birthday, keeping eligibility for higher ages to catch-up</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">Additional eligibility 1: </t>
     </r>
     <r>
@@ -225,6 +210,21 @@
   </si>
   <si>
     <t>Needed to vaccinate </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Additional eligibility 2: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Those who reach age 80 years be called in on 80th birthday, keeping eligibility for higher ages to catch-up</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -298,8 +298,17 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -307,17 +316,8 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -602,7 +602,7 @@
   <dimension ref="A1:AH22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:Q19"/>
+      <selection activeCell="B17" sqref="B17:B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -638,34 +638,34 @@
       <c r="D1" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="16"/>
-      <c r="G1" s="14" t="s">
+      <c r="F1" s="18"/>
+      <c r="G1" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14" t="s">
+      <c r="H1" s="17"/>
+      <c r="I1" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="L1" s="14"/>
-      <c r="M1" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="N1" s="13"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="N1" s="16"/>
       <c r="O1" s="6" t="s">
         <v>38</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:34" s="1" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -688,7 +688,7 @@
         <v>33</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>33</v>
@@ -733,7 +733,7 @@
         <v>6</v>
       </c>
       <c r="Z2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AA2" t="s">
         <v>7</v>
@@ -751,7 +751,7 @@
         <v>11</v>
       </c>
       <c r="AF2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="AG2" t="s">
         <v>12</v>
@@ -835,7 +835,7 @@
         <v>15</v>
       </c>
       <c r="U3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="V3">
         <v>2965505</v>
@@ -878,8 +878,8 @@
       </c>
     </row>
     <row r="4" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
-        <v>44</v>
+      <c r="A4" s="15" t="s">
+        <v>43</v>
       </c>
       <c r="B4" s="10" t="str">
         <f t="shared" ref="B4:B5" si="1">T4</f>
@@ -952,7 +952,7 @@
         <v>17</v>
       </c>
       <c r="U4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="V4">
         <v>2662322</v>
@@ -995,7 +995,7 @@
       </c>
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A5" s="18"/>
+      <c r="A5" s="15"/>
       <c r="B5" s="10" t="str">
         <f t="shared" si="1"/>
         <v>[75,80)</v>
@@ -1067,7 +1067,7 @@
         <v>18</v>
       </c>
       <c r="U5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="V5">
         <v>2423598</v>
@@ -1116,23 +1116,23 @@
       <c r="Q6" s="3"/>
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="12"/>
-      <c r="M7" s="12"/>
-      <c r="N7" s="12"/>
-      <c r="O7" s="12"/>
+      <c r="A7" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="14"/>
+      <c r="N7" s="14"/>
+      <c r="O7" s="14"/>
       <c r="P7" s="7"/>
       <c r="Q7" s="3"/>
     </row>
@@ -1140,11 +1140,11 @@
       <c r="A8" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="15" t="str">
+      <c r="B8" s="13" t="str">
         <f>T8</f>
         <v>[80,85)</v>
       </c>
-      <c r="C8" s="17">
+      <c r="C8" s="12">
         <f>V8/1000</f>
         <v>1508.4970000000001</v>
       </c>
@@ -1162,11 +1162,11 @@
       </c>
       <c r="G8" s="9">
         <f t="shared" ref="G8" si="18">Y8 / 1000</f>
-        <v>291.958351830786</v>
+        <v>145.979175915393</v>
       </c>
       <c r="H8" s="5">
         <f t="shared" ref="H8" si="19">AE8</f>
-        <v>1.23752264637281</v>
+        <v>1.1187613231864</v>
       </c>
       <c r="I8" s="9">
         <f t="shared" ref="I8" si="20">-Z8</f>
@@ -1194,11 +1194,11 @@
       </c>
       <c r="O8" s="7">
         <f>((SUM($K$3:$K$5)+ SUM($K$8:K8)) * 20 + (SUM($M$3:$M$5) + SUM($M$8:M8)) * 1000) /(SUM($G$3:$G$5) + SUM($G$8:G8))</f>
-        <v>87.672327166819258</v>
+        <v>96.979121534279145</v>
       </c>
       <c r="P8" s="7">
         <f>(K8 * 20 + M8 * 1000) /G8</f>
-        <v>46.321940978362043</v>
+        <v>92.643881956724087</v>
       </c>
       <c r="Q8" s="3">
         <f t="shared" ref="Q8:Q12" si="26">E8/I8*1000</f>
@@ -1211,7 +1211,7 @@
         <v>20</v>
       </c>
       <c r="U8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="V8">
         <v>1508497</v>
@@ -1223,7 +1223,7 @@
         <v>145979.17591539299</v>
       </c>
       <c r="Y8">
-        <v>291958.35183078598</v>
+        <v>145979.17591539299</v>
       </c>
       <c r="Z8">
         <v>-5467.3873239638797</v>
@@ -1241,7 +1241,7 @@
         <v>1.23752264637281</v>
       </c>
       <c r="AE8">
-        <v>1.23752264637281</v>
+        <v>1.1187613231864</v>
       </c>
       <c r="AF8">
         <v>1.1202526060015501</v>
@@ -1257,8 +1257,8 @@
       <c r="A9" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="15"/>
-      <c r="C9" s="17"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="12"/>
       <c r="D9" s="9">
         <f t="shared" ref="D9:D12" si="27">W9/1000</f>
         <v>433.09521756606995</v>
@@ -1273,11 +1273,11 @@
       </c>
       <c r="G9" s="9">
         <f t="shared" ref="G9:G12" si="30">Y9 / 1000</f>
-        <v>117.58002262206</v>
+        <v>58.790011311030398</v>
       </c>
       <c r="H9" s="5">
         <f t="shared" ref="H9:H12" si="31">AE9</f>
-        <v>1.3331798452802599</v>
+        <v>1.16658992264013</v>
       </c>
       <c r="I9" s="9">
         <f t="shared" ref="I9:I12" si="32">-Z9</f>
@@ -1305,11 +1305,11 @@
       </c>
       <c r="O9" s="7">
         <f>((SUM($K$3:$K$5)+ SUM($K$8:K9)) * 20 + (SUM($M$3:$M$5) + SUM($M$8:M9)) * 1000) /(SUM($G$3:$G$5) + SUM($G$8:G9))</f>
-        <v>86.477528846796758</v>
+        <v>98.826585324238735</v>
       </c>
       <c r="P9" s="7">
         <f t="shared" ref="P9:P12" si="38">(K9 * 20 + M9 * 1000) /G9</f>
-        <v>71.020354731687263</v>
+        <v>142.04070946337356</v>
       </c>
       <c r="Q9" s="3">
         <f t="shared" si="26"/>
@@ -1322,7 +1322,7 @@
         <v>20</v>
       </c>
       <c r="U9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="V9">
         <v>1508497</v>
@@ -1334,7 +1334,7 @@
         <v>58790.011311030401</v>
       </c>
       <c r="Y9">
-        <v>117580.02262206</v>
+        <v>58790.011311030401</v>
       </c>
       <c r="Z9">
         <v>-2563.8673259979701</v>
@@ -1352,7 +1352,7 @@
         <v>1.3331798452802599</v>
       </c>
       <c r="AE9">
-        <v>1.3331798452802599</v>
+        <v>1.16658992264013</v>
       </c>
       <c r="AF9">
         <v>1.17664365882528</v>
@@ -1368,11 +1368,11 @@
       <c r="A10" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="15" t="str">
+      <c r="B10" s="13" t="str">
         <f>T10</f>
         <v>[85,90)</v>
       </c>
-      <c r="C10" s="17">
+      <c r="C10" s="12">
         <f>V10/1000</f>
         <v>940.56899999999996</v>
       </c>
@@ -1390,11 +1390,11 @@
       </c>
       <c r="G10" s="9">
         <f t="shared" si="30"/>
-        <v>93.505172410066507</v>
+        <v>46.752586205033197</v>
       </c>
       <c r="H10" s="5">
         <f t="shared" si="31"/>
-        <v>1.4092509556325299</v>
+        <v>1.2046254778162599</v>
       </c>
       <c r="I10" s="9">
         <f t="shared" si="32"/>
@@ -1422,11 +1422,11 @@
       </c>
       <c r="O10" s="7">
         <f>((SUM($K$3:$K$5)+ SUM($K$8:K10)) * 20 + (SUM($M$3:$M$5) + SUM($M$8:M10)) * 1000) /(SUM($G$3:$G$5) + SUM($G$8:G10))</f>
-        <v>84.033120014104398</v>
+        <v>98.307529489860457</v>
       </c>
       <c r="P10" s="7">
         <f t="shared" si="38"/>
-        <v>41.193774377112675</v>
+        <v>82.387548754225449</v>
       </c>
       <c r="Q10" s="3">
         <f t="shared" si="26"/>
@@ -1439,7 +1439,7 @@
         <v>23</v>
       </c>
       <c r="U10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="V10">
         <v>940569</v>
@@ -1451,7 +1451,7 @@
         <v>46752.5862050332</v>
       </c>
       <c r="Y10">
-        <v>93505.172410066501</v>
+        <v>46752.5862050332</v>
       </c>
       <c r="Z10">
         <v>-1774.83334438626</v>
@@ -1469,7 +1469,7 @@
         <v>1.4092509556325299</v>
       </c>
       <c r="AE10">
-        <v>1.4092509556325299</v>
+        <v>1.2046254778162599</v>
       </c>
       <c r="AF10">
         <v>1.2156802812985901</v>
@@ -1485,8 +1485,8 @@
       <c r="A11" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="15"/>
-      <c r="C11" s="17"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="12"/>
       <c r="D11" s="9">
         <f t="shared" si="27"/>
         <v>596.15128272620996</v>
@@ -1501,11 +1501,11 @@
       </c>
       <c r="G11" s="9">
         <f t="shared" si="30"/>
-        <v>161.84773801716</v>
+        <v>80.923869008580112</v>
       </c>
       <c r="H11" s="5">
         <f t="shared" si="31"/>
-        <v>1.54092214367092</v>
+        <v>1.2704610718354601</v>
       </c>
       <c r="I11" s="9">
         <f t="shared" si="32"/>
@@ -1533,11 +1533,11 @@
       </c>
       <c r="O11" s="7">
         <f>((SUM($K$3:$K$5)+ SUM($K$8:K11)) * 20 + (SUM($M$3:$M$5) + SUM($M$8:M11)) * 1000) /(SUM($G$3:$G$5) + SUM($G$8:G11))</f>
-        <v>81.881382235730811</v>
+        <v>99.312633687497438</v>
       </c>
       <c r="P11" s="7">
         <f t="shared" si="38"/>
-        <v>58.85175391978197</v>
+        <v>117.70350783956377</v>
       </c>
       <c r="Q11" s="3">
         <f t="shared" si="26"/>
@@ -1550,7 +1550,7 @@
         <v>23</v>
       </c>
       <c r="U11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="V11">
         <v>940569</v>
@@ -1562,7 +1562,7 @@
         <v>80923.869008580106</v>
       </c>
       <c r="Y11">
-        <v>161847.73801716001</v>
+        <v>80923.869008580106</v>
       </c>
       <c r="Z11">
         <v>-2719.1285037150701</v>
@@ -1580,7 +1580,7 @@
         <v>1.54092214367092</v>
       </c>
       <c r="AE11">
-        <v>1.54092214367092</v>
+        <v>1.2704610718354601</v>
       </c>
       <c r="AF11">
         <v>1.2754862305115999</v>
@@ -1618,11 +1618,11 @@
       </c>
       <c r="G12" s="9">
         <f t="shared" si="30"/>
-        <v>113.247834395767</v>
+        <v>56.6239171978836</v>
       </c>
       <c r="H12" s="5">
         <f t="shared" si="31"/>
-        <v>1.63305489189682</v>
+        <v>1.31652744594841</v>
       </c>
       <c r="I12" s="9">
         <f t="shared" si="32"/>
@@ -1650,11 +1650,11 @@
       </c>
       <c r="O12" s="7">
         <f>((SUM($K$3:$K$5)+ SUM($K$8:K12)) * 20 + (SUM($M$3:$M$5) + SUM($M$8:M12)) * 1000) /(SUM($G$3:$G$5) + SUM($G$8:G12))</f>
-        <v>79.793282360622712</v>
+        <v>98.977663170286334</v>
       </c>
       <c r="P12" s="7">
         <f t="shared" si="38"/>
-        <v>44.869768217079098</v>
+        <v>89.73953643415804</v>
       </c>
       <c r="Q12" s="3">
         <f t="shared" si="26"/>
@@ -1667,7 +1667,7 @@
         <v>25</v>
       </c>
       <c r="U12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="V12">
         <v>417138</v>
@@ -1679,7 +1679,7 @@
         <v>56623.917197883602</v>
       </c>
       <c r="Y12">
-        <v>113247.834395767</v>
+        <v>56623.917197883602</v>
       </c>
       <c r="Z12">
         <v>-1398.2286690972801</v>
@@ -1697,7 +1697,7 @@
         <v>1.63305489189682</v>
       </c>
       <c r="AE12">
-        <v>1.63305489189682</v>
+        <v>1.31652744594841</v>
       </c>
       <c r="AF12">
         <v>1.3062396107427801</v>
@@ -1714,23 +1714,23 @@
       <c r="Q13" s="3"/>
     </row>
     <row r="14" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A14" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="12"/>
-      <c r="L14" s="12"/>
-      <c r="M14" s="12"/>
-      <c r="N14" s="12"/>
-      <c r="O14" s="12"/>
+      <c r="A14" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="14"/>
+      <c r="N14" s="14"/>
+      <c r="O14" s="14"/>
       <c r="P14" s="7"/>
       <c r="Q14" s="3"/>
     </row>
@@ -1738,10 +1738,10 @@
       <c r="A15" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="17">
+      <c r="C15" s="12">
         <v>1508.4970000000001</v>
       </c>
       <c r="D15" s="9">
@@ -1758,11 +1758,11 @@
       </c>
       <c r="G15" s="9">
         <f t="shared" ref="G15:G19" si="42">Y15 / 1000</f>
-        <v>513.32357896639303</v>
+        <v>256.661789483196</v>
       </c>
       <c r="H15" s="5">
         <f t="shared" ref="H15:H19" si="43">AE15</f>
-        <v>1.4176142732588399</v>
+        <v>1.20880713662942</v>
       </c>
       <c r="I15" s="9">
         <f t="shared" ref="I15:I19" si="44">-Z15</f>
@@ -1790,11 +1790,11 @@
       </c>
       <c r="O15" s="7">
         <f>((SUM($K$3:$K$5)+ SUM($K$15:K15)) * 20 + (SUM($M$3:$M$5) + SUM($M$15:M15)) * 1000) /(SUM($G$3:$G$5) + SUM($G$15:G15))</f>
-        <v>82.815127872061908</v>
+        <v>97.120461780647219</v>
       </c>
       <c r="P15" s="7">
         <f>(K15 * 20 + M15 * 1000) /G15</f>
-        <v>47.665820507082259</v>
+        <v>95.331641014164703</v>
       </c>
       <c r="Q15" s="3">
         <f t="shared" ref="Q15:Q19" si="50">E15/I15*1000</f>
@@ -1807,7 +1807,7 @@
         <v>20</v>
       </c>
       <c r="U15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="V15">
         <v>1508497</v>
@@ -1819,7 +1819,7 @@
         <v>256661.78948319599</v>
       </c>
       <c r="Y15">
-        <v>513323.57896639302</v>
+        <v>256661.78948319599</v>
       </c>
       <c r="Z15">
         <v>-9869.6693576464895</v>
@@ -1837,7 +1837,7 @@
         <v>1.4176142732588399</v>
       </c>
       <c r="AE15">
-        <v>1.4176142732588399</v>
+        <v>1.20880713662942</v>
       </c>
       <c r="AF15">
         <v>1.2170787234020499</v>
@@ -1853,8 +1853,8 @@
       <c r="A16" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="15"/>
-      <c r="C16" s="17"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="12"/>
       <c r="D16" s="9">
         <f t="shared" si="39"/>
         <v>433.09521756606995</v>
@@ -1869,11 +1869,11 @@
       </c>
       <c r="G16" s="9">
         <f t="shared" si="42"/>
-        <v>153.41140535600599</v>
+        <v>76.705702678003306</v>
       </c>
       <c r="H16" s="5">
         <f t="shared" si="43"/>
-        <v>1.54242208490538</v>
+        <v>1.2712110424526899</v>
       </c>
       <c r="I16" s="9">
         <f t="shared" si="44"/>
@@ -1901,11 +1901,11 @@
       </c>
       <c r="O16" s="7">
         <f>((SUM($K$3:$K$5)+ SUM($K$15:K16)) * 20 + (SUM($M$3:$M$5) + SUM($M$15:M16)) * 1000) /(SUM($G$3:$G$5) + SUM($G$15:G16))</f>
-        <v>81.946562864145406</v>
+        <v>99.42974386052758</v>
       </c>
       <c r="P16" s="7">
         <f t="shared" ref="P16:P19" si="51">(K16 * 20 + M16 * 1000) /G16</f>
-        <v>72.081073386911271</v>
+        <v>144.16214677382195</v>
       </c>
       <c r="Q16" s="3">
         <f t="shared" si="50"/>
@@ -1918,7 +1918,7 @@
         <v>20</v>
       </c>
       <c r="U16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="V16">
         <v>1508497</v>
@@ -1930,7 +1930,7 @@
         <v>76705.702678003305</v>
       </c>
       <c r="Y16">
-        <v>153411.405356006</v>
+        <v>76705.702678003305</v>
       </c>
       <c r="Z16">
         <v>-3427.5937526859798</v>
@@ -1948,7 +1948,7 @@
         <v>1.54242208490538</v>
       </c>
       <c r="AE16">
-        <v>1.54242208490538</v>
+        <v>1.2712110424526899</v>
       </c>
       <c r="AF16">
         <v>1.29246703168387</v>
@@ -1964,11 +1964,11 @@
       <c r="A17" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="15" t="str">
-        <f t="shared" ref="B17" si="52">T15</f>
-        <v>[80,85)</v>
-      </c>
-      <c r="C17" s="17">
+      <c r="B17" s="13" t="str">
+        <f>T17</f>
+        <v>[85,90)</v>
+      </c>
+      <c r="C17" s="12">
         <v>940.56899999999996</v>
       </c>
       <c r="D17" s="9">
@@ -1985,11 +1985,11 @@
       </c>
       <c r="G17" s="9">
         <f t="shared" si="42"/>
-        <v>93.505172410066507</v>
+        <v>46.752586205033197</v>
       </c>
       <c r="H17" s="5">
         <f t="shared" si="43"/>
-        <v>1.61849319525765</v>
+        <v>1.3092465976288199</v>
       </c>
       <c r="I17" s="9">
         <f t="shared" si="44"/>
@@ -2017,11 +2017,11 @@
       </c>
       <c r="O17" s="7">
         <f>((SUM($K$3:$K$5)+ SUM($K$15:K17)) * 20 + (SUM($M$3:$M$5) + SUM($M$15:M17)) * 1000) /(SUM($G$3:$G$5) + SUM($G$15:G17))</f>
-        <v>80.03113320448216</v>
+        <v>98.934642820385761</v>
       </c>
       <c r="P17" s="7">
         <f t="shared" si="51"/>
-        <v>41.193774377112675</v>
+        <v>82.387548754225449</v>
       </c>
       <c r="Q17" s="3">
         <f t="shared" si="50"/>
@@ -2034,7 +2034,7 @@
         <v>23</v>
       </c>
       <c r="U17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="V17">
         <v>940569</v>
@@ -2046,7 +2046,7 @@
         <v>46752.5862050332</v>
       </c>
       <c r="Y17">
-        <v>93505.172410066501</v>
+        <v>46752.5862050332</v>
       </c>
       <c r="Z17">
         <v>-1774.83334438626</v>
@@ -2064,7 +2064,7 @@
         <v>1.61849319525765</v>
       </c>
       <c r="AE17">
-        <v>1.61849319525765</v>
+        <v>1.3092465976288199</v>
       </c>
       <c r="AF17">
         <v>1.3315036541571701</v>
@@ -2080,8 +2080,8 @@
       <c r="A18" t="s">
         <v>31</v>
       </c>
-      <c r="B18" s="15"/>
-      <c r="C18" s="17"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="12"/>
       <c r="D18" s="9">
         <f t="shared" si="39"/>
         <v>596.15128272620996</v>
@@ -2096,11 +2096,11 @@
       </c>
       <c r="G18" s="9">
         <f t="shared" si="42"/>
-        <v>161.84773801716</v>
+        <v>80.923869008580112</v>
       </c>
       <c r="H18" s="5">
         <f t="shared" si="43"/>
-        <v>1.7501643832960401</v>
+        <v>1.37508219164802</v>
       </c>
       <c r="I18" s="9">
         <f t="shared" si="44"/>
@@ -2128,11 +2128,11 @@
       </c>
       <c r="O18" s="7">
         <f>((SUM($K$3:$K$5)+ SUM($K$15:K18)) * 20 + (SUM($M$3:$M$5) + SUM($M$15:M18)) * 1000) /(SUM($G$3:$G$5) + SUM($G$15:G18))</f>
-        <v>78.437732002316082</v>
+        <v>99.833250470974832</v>
       </c>
       <c r="P18" s="7">
         <f t="shared" si="51"/>
-        <v>58.85175391978197</v>
+        <v>117.70350783956377</v>
       </c>
       <c r="Q18" s="3">
         <f t="shared" si="50"/>
@@ -2145,7 +2145,7 @@
         <v>23</v>
       </c>
       <c r="U18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="V18">
         <v>940569</v>
@@ -2157,7 +2157,7 @@
         <v>80923.869008580106</v>
       </c>
       <c r="Y18">
-        <v>161847.73801716001</v>
+        <v>80923.869008580106</v>
       </c>
       <c r="Z18">
         <v>-2719.1285037150701</v>
@@ -2175,7 +2175,7 @@
         <v>1.7501643832960401</v>
       </c>
       <c r="AE18">
-        <v>1.7501643832960401</v>
+        <v>1.37508219164802</v>
       </c>
       <c r="AF18">
         <v>1.3913096033701799</v>
@@ -2192,8 +2192,8 @@
         <v>31</v>
       </c>
       <c r="B19" s="10" t="str">
-        <f t="shared" ref="B19" si="53">T17</f>
-        <v>[85,90)</v>
+        <f>T19</f>
+        <v>[90,95)</v>
       </c>
       <c r="C19" s="11">
         <v>417.13799999999998</v>
@@ -2212,11 +2212,11 @@
       </c>
       <c r="G19" s="9">
         <f t="shared" si="42"/>
-        <v>113.247834395767</v>
+        <v>56.6239171978836</v>
       </c>
       <c r="H19" s="5">
         <f t="shared" si="43"/>
-        <v>1.8422971315219401</v>
+        <v>1.4211485657609699</v>
       </c>
       <c r="I19" s="9">
         <f t="shared" si="44"/>
@@ -2244,11 +2244,11 @@
       </c>
       <c r="O19" s="7">
         <f>((SUM($K$3:$K$5)+ SUM($K$15:K19)) * 20 + (SUM($M$3:$M$5) + SUM($M$15:M19)) * 1000) /(SUM($G$3:$G$5) + SUM($G$15:G19))</f>
-        <v>76.759007814472241</v>
+        <v>99.506063843051706</v>
       </c>
       <c r="P19" s="7">
         <f t="shared" si="51"/>
-        <v>44.869768217079098</v>
+        <v>89.73953643415804</v>
       </c>
       <c r="Q19" s="3">
         <f t="shared" si="50"/>
@@ -2261,7 +2261,7 @@
         <v>25</v>
       </c>
       <c r="U19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="V19">
         <v>417138</v>
@@ -2273,7 +2273,7 @@
         <v>56623.917197883602</v>
       </c>
       <c r="Y19">
-        <v>113247.834395767</v>
+        <v>56623.917197883602</v>
       </c>
       <c r="Z19">
         <v>-1398.2286690972801</v>
@@ -2291,7 +2291,7 @@
         <v>1.8422971315219401</v>
       </c>
       <c r="AE19">
-        <v>1.8422971315219401</v>
+        <v>1.4211485657609699</v>
       </c>
       <c r="AF19">
         <v>1.4220629836013701</v>
@@ -2337,12 +2337,12 @@
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="C8:C9"/>
+    <mergeCell ref="I1:J1"/>
     <mergeCell ref="C10:C11"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="A7:O7"/>
     <mergeCell ref="A4:A5"/>
-    <mergeCell ref="I1:J1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Enlarge the font size in the panel figures
</commit_message>
<xml_diff>
--- a/docs/tabs/Tab_ProgrammeProfile.xlsx
+++ b/docs/tabs/Tab_ProgrammeProfile.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\HPRU\Shingrix\HPRU_RZV\docs\tabs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1718D0B-2128-42EA-A6D9-A6AC582DBEA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32AA0869-788C-47AE-8EDC-C32930B52F0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="5265" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="64">
   <si>
     <t>Eligibility</t>
   </si>
@@ -225,6 +226,33 @@
       </rPr>
       <t>Those who reach age 80 years be called in on 80th birthday, keeping eligibility for higher ages to catch-up</t>
     </r>
+  </si>
+  <si>
+    <t>[95,100)</t>
+  </si>
+  <si>
+    <t>UV_100</t>
+  </si>
+  <si>
+    <t>Additional eligibility 1: Keeping 80+ eligible</t>
+  </si>
+  <si>
+    <t>Additional eligibility 2: Those who reach age 80 years be called in on 80th birthday, keeping eligibility for higher ages to catch-up</t>
+  </si>
+  <si>
+    <t>Current eligibility</t>
+  </si>
+  <si>
+    <t>Doses per uptake</t>
+  </si>
+  <si>
+    <t>Two</t>
+  </si>
+  <si>
+    <t>Single</t>
+  </si>
+  <si>
+    <t>cum. %</t>
   </si>
 </sst>
 </file>
@@ -271,7 +299,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -298,17 +326,14 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -318,6 +343,15 @@
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -599,10 +633,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AH22"/>
+  <dimension ref="A1:AH24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17:B19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -638,26 +672,26 @@
       <c r="D1" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="18"/>
-      <c r="G1" s="17" t="s">
+      <c r="F1" s="17"/>
+      <c r="G1" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17" t="s">
+      <c r="H1" s="16"/>
+      <c r="I1" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17" t="s">
+      <c r="J1" s="16"/>
+      <c r="K1" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="L1" s="17"/>
-      <c r="M1" s="16" t="s">
+      <c r="L1" s="16"/>
+      <c r="M1" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="N1" s="16"/>
+      <c r="N1" s="15"/>
       <c r="O1" s="6" t="s">
         <v>38</v>
       </c>
@@ -878,7 +912,7 @@
       </c>
     </row>
     <row r="4" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="18" t="s">
         <v>43</v>
       </c>
       <c r="B4" s="10" t="str">
@@ -995,7 +1029,7 @@
       </c>
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A5" s="15"/>
+      <c r="A5" s="18"/>
       <c r="B5" s="10" t="str">
         <f t="shared" si="1"/>
         <v>[75,80)</v>
@@ -1140,11 +1174,11 @@
       <c r="A8" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="13" t="str">
+      <c r="B8" s="12" t="str">
         <f>T8</f>
         <v>[80,85)</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C8" s="13">
         <f>V8/1000</f>
         <v>1508.4970000000001</v>
       </c>
@@ -1257,8 +1291,8 @@
       <c r="A9" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="12"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="13"/>
       <c r="D9" s="9">
         <f t="shared" ref="D9:D12" si="27">W9/1000</f>
         <v>433.09521756606995</v>
@@ -1368,11 +1402,11 @@
       <c r="A10" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="13" t="str">
+      <c r="B10" s="12" t="str">
         <f>T10</f>
         <v>[85,90)</v>
       </c>
-      <c r="C10" s="12">
+      <c r="C10" s="13">
         <f>V10/1000</f>
         <v>940.56899999999996</v>
       </c>
@@ -1485,8 +1519,8 @@
       <c r="A11" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="13"/>
-      <c r="C11" s="12"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="13"/>
       <c r="D11" s="9">
         <f t="shared" si="27"/>
         <v>596.15128272620996</v>
@@ -1710,641 +1744,1618 @@
       </c>
     </row>
     <row r="13" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="P13" s="7"/>
-      <c r="Q13" s="3"/>
+      <c r="A13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="10" t="str">
+        <f>T13</f>
+        <v>[95,100)</v>
+      </c>
+      <c r="C13" s="11">
+        <f>V13/1000</f>
+        <v>109.06399999999999</v>
+      </c>
+      <c r="D13" s="9">
+        <f t="shared" ref="D13" si="39">W13/1000</f>
+        <v>109.06399999999999</v>
+      </c>
+      <c r="E13" s="3">
+        <f t="shared" ref="E13" si="40">X13 / 1000</f>
+        <v>14.804767020194701</v>
+      </c>
+      <c r="F13" s="5">
+        <f t="shared" ref="F13" si="41">AD13</f>
+        <v>1.6571437211391999</v>
+      </c>
+      <c r="G13" s="9">
+        <f t="shared" ref="G13" si="42">Y13 / 1000</f>
+        <v>14.804767020194701</v>
+      </c>
+      <c r="H13" s="5">
+        <f t="shared" ref="H13" si="43">AE13</f>
+        <v>1.3285718605696</v>
+      </c>
+      <c r="I13" s="9">
+        <f t="shared" ref="I13" si="44">-Z13</f>
+        <v>234.88374918093501</v>
+      </c>
+      <c r="J13" s="5">
+        <f t="shared" ref="J13" si="45">AF13</f>
+        <v>1.3114057680447599</v>
+      </c>
+      <c r="K13" s="9">
+        <f t="shared" ref="K13" si="46">AB13</f>
+        <v>34.359355486366802</v>
+      </c>
+      <c r="L13" s="5">
+        <f t="shared" ref="L13" si="47">AG13</f>
+        <v>1.3229267891440299</v>
+      </c>
+      <c r="M13" s="7">
+        <f t="shared" ref="M13" si="48">-AA13/1000000</f>
+        <v>0.12997330756768199</v>
+      </c>
+      <c r="N13" s="5">
+        <f t="shared" ref="N13" si="49">AH13</f>
+        <v>1.6162034910869401</v>
+      </c>
+      <c r="O13" s="7">
+        <f>((SUM($K$3:$K$5)+ SUM($K$8:K13)) * 20 + (SUM($M$3:$M$5) + SUM($M$8:M13)) * 1000) /(SUM($G$3:$G$5) + SUM($G$8:G13))</f>
+        <v>98.58075023718358</v>
+      </c>
+      <c r="P13" s="7">
+        <f t="shared" ref="P13" si="50">(K13 * 20 + M13 * 1000) /G13</f>
+        <v>55.195763376779666</v>
+      </c>
+      <c r="Q13" s="3">
+        <f t="shared" ref="Q13" si="51">E13/I13*1000</f>
+        <v>63.03018864361848</v>
+      </c>
+      <c r="S13" t="s">
+        <v>56</v>
+      </c>
+      <c r="T13" t="s">
+        <v>55</v>
+      </c>
+      <c r="U13" t="s">
+        <v>52</v>
+      </c>
+      <c r="V13">
+        <v>109064</v>
+      </c>
+      <c r="W13">
+        <v>109064</v>
+      </c>
+      <c r="X13">
+        <v>14804.7670201947</v>
+      </c>
+      <c r="Y13">
+        <v>14804.7670201947</v>
+      </c>
+      <c r="Z13">
+        <v>-234.88374918093501</v>
+      </c>
+      <c r="AA13">
+        <v>-129973.307567682</v>
+      </c>
+      <c r="AB13">
+        <v>34.359355486366802</v>
+      </c>
+      <c r="AC13">
+        <v>98.580750237183594</v>
+      </c>
+      <c r="AD13">
+        <v>1.6571437211391999</v>
+      </c>
+      <c r="AE13">
+        <v>1.3285718605696</v>
+      </c>
+      <c r="AF13">
+        <v>1.3114057680447599</v>
+      </c>
+      <c r="AG13">
+        <v>1.3229267891440299</v>
+      </c>
+      <c r="AH13">
+        <v>1.6162034910869401</v>
+      </c>
     </row>
     <row r="14" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="14"/>
-      <c r="M14" s="14"/>
-      <c r="N14" s="14"/>
-      <c r="O14" s="14"/>
       <c r="P14" s="7"/>
       <c r="Q14" s="3"/>
     </row>
     <row r="15" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C15" s="12">
-        <v>1508.4970000000001</v>
-      </c>
-      <c r="D15" s="9">
-        <f t="shared" ref="D15:D19" si="39">W15/1000</f>
-        <v>1075.4017824339201</v>
-      </c>
-      <c r="E15" s="3">
-        <f t="shared" ref="E15:E19" si="40">X15 / 1000</f>
-        <v>256.661789483196</v>
-      </c>
-      <c r="F15" s="5">
-        <f t="shared" ref="F15:F19" si="41">AD15</f>
-        <v>1.4176142732588399</v>
-      </c>
-      <c r="G15" s="9">
-        <f t="shared" ref="G15:G19" si="42">Y15 / 1000</f>
-        <v>256.661789483196</v>
-      </c>
-      <c r="H15" s="5">
-        <f t="shared" ref="H15:H19" si="43">AE15</f>
-        <v>1.20880713662942</v>
-      </c>
-      <c r="I15" s="9">
-        <f t="shared" ref="I15:I19" si="44">-Z15</f>
-        <v>9869.6693576464895</v>
-      </c>
-      <c r="J15" s="5">
-        <f t="shared" ref="J15:J19" si="45">AF15</f>
-        <v>1.2170787234020499</v>
-      </c>
-      <c r="K15" s="9">
-        <f t="shared" ref="K15:K19" si="46">AB15</f>
-        <v>1093.2241011594599</v>
-      </c>
-      <c r="L15" s="5">
-        <f t="shared" ref="L15:L19" si="47">AG15</f>
-        <v>1.19612986147641</v>
-      </c>
-      <c r="M15" s="7">
-        <f t="shared" ref="M15:M19" si="48">-AA15/1000000</f>
-        <v>2.6035075538759598</v>
-      </c>
-      <c r="N15" s="5">
-        <f t="shared" ref="N15:N19" si="49">AH15</f>
-        <v>1.3114935881152701</v>
-      </c>
-      <c r="O15" s="7">
-        <f>((SUM($K$3:$K$5)+ SUM($K$15:K15)) * 20 + (SUM($M$3:$M$5) + SUM($M$15:M15)) * 1000) /(SUM($G$3:$G$5) + SUM($G$15:G15))</f>
-        <v>97.120461780647219</v>
-      </c>
-      <c r="P15" s="7">
-        <f>(K15 * 20 + M15 * 1000) /G15</f>
-        <v>95.331641014164703</v>
-      </c>
-      <c r="Q15" s="3">
-        <f t="shared" ref="Q15:Q19" si="50">E15/I15*1000</f>
-        <v>26.005105154241893</v>
-      </c>
-      <c r="S15" t="s">
-        <v>19</v>
-      </c>
-      <c r="T15" t="s">
-        <v>20</v>
-      </c>
-      <c r="U15" t="s">
-        <v>51</v>
-      </c>
-      <c r="V15">
-        <v>1508497</v>
-      </c>
-      <c r="W15">
-        <v>1075401.7824339201</v>
-      </c>
-      <c r="X15">
-        <v>256661.78948319599</v>
-      </c>
-      <c r="Y15">
-        <v>256661.78948319599</v>
-      </c>
-      <c r="Z15">
-        <v>-9869.6693576464895</v>
-      </c>
-      <c r="AA15">
-        <v>-2603507.5538759599</v>
-      </c>
-      <c r="AB15">
-        <v>1093.2241011594599</v>
-      </c>
-      <c r="AC15">
-        <v>97.120461780647304</v>
-      </c>
-      <c r="AD15">
-        <v>1.4176142732588399</v>
-      </c>
-      <c r="AE15">
-        <v>1.20880713662942</v>
-      </c>
-      <c r="AF15">
-        <v>1.2170787234020499</v>
-      </c>
-      <c r="AG15">
-        <v>1.19612986147641</v>
-      </c>
-      <c r="AH15">
-        <v>1.3114935881152701</v>
-      </c>
+      <c r="A15" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="14"/>
+      <c r="N15" s="14"/>
+      <c r="O15" s="14"/>
+      <c r="P15" s="7"/>
+      <c r="Q15" s="3"/>
     </row>
     <row r="16" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>31</v>
-      </c>
-      <c r="B16" s="13"/>
-      <c r="C16" s="12"/>
+        <v>30</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="13">
+        <v>1508.4970000000001</v>
+      </c>
       <c r="D16" s="9">
-        <f t="shared" si="39"/>
-        <v>433.09521756606995</v>
+        <f t="shared" ref="D16:D20" si="52">W16/1000</f>
+        <v>1075.4017824339201</v>
       </c>
       <c r="E16" s="3">
-        <f t="shared" si="40"/>
-        <v>76.705702678003306</v>
+        <f t="shared" ref="E16:E20" si="53">X16 / 1000</f>
+        <v>256.661789483196</v>
       </c>
       <c r="F16" s="5">
-        <f t="shared" si="41"/>
-        <v>1.54242208490538</v>
+        <f t="shared" ref="F16:F20" si="54">AD16</f>
+        <v>1.4176142732588399</v>
       </c>
       <c r="G16" s="9">
-        <f t="shared" si="42"/>
-        <v>76.705702678003306</v>
+        <f t="shared" ref="G16:G20" si="55">Y16 / 1000</f>
+        <v>256.661789483196</v>
       </c>
       <c r="H16" s="5">
-        <f t="shared" si="43"/>
-        <v>1.2712110424526899</v>
+        <f t="shared" ref="H16:H20" si="56">AE16</f>
+        <v>1.20880713662942</v>
       </c>
       <c r="I16" s="9">
-        <f t="shared" si="44"/>
-        <v>3427.5937526859798</v>
+        <f t="shared" ref="I16:I20" si="57">-Z16</f>
+        <v>9869.6693576464895</v>
       </c>
       <c r="J16" s="5">
-        <f t="shared" si="45"/>
-        <v>1.29246703168387</v>
+        <f t="shared" ref="J16:J20" si="58">AF16</f>
+        <v>1.2170787234020499</v>
       </c>
       <c r="K16" s="9">
-        <f t="shared" si="46"/>
-        <v>490.93811708074998</v>
+        <f t="shared" ref="K16:K20" si="59">AB16</f>
+        <v>1093.2241011594599</v>
       </c>
       <c r="L16" s="5">
-        <f t="shared" si="47"/>
-        <v>1.28420661060261</v>
+        <f t="shared" ref="L16:L20" si="60">AG16</f>
+        <v>1.19612986147641</v>
       </c>
       <c r="M16" s="7">
-        <f t="shared" si="48"/>
-        <v>1.23929642624046</v>
+        <f t="shared" ref="M16:M20" si="61">-AA16/1000000</f>
+        <v>2.6035075538759598</v>
       </c>
       <c r="N16" s="5">
-        <f t="shared" si="49"/>
-        <v>1.45976774617307</v>
+        <f t="shared" ref="N16:N20" si="62">AH16</f>
+        <v>1.3114935881152701</v>
       </c>
       <c r="O16" s="7">
-        <f>((SUM($K$3:$K$5)+ SUM($K$15:K16)) * 20 + (SUM($M$3:$M$5) + SUM($M$15:M16)) * 1000) /(SUM($G$3:$G$5) + SUM($G$15:G16))</f>
-        <v>99.42974386052758</v>
+        <f>((SUM($K$3:$K$5)+ SUM($K$16:K16)) * 20 + (SUM($M$3:$M$5) + SUM($M$16:M16)) * 1000) /(SUM($G$3:$G$5) + SUM($G$16:G16))</f>
+        <v>97.120461780647219</v>
       </c>
       <c r="P16" s="7">
-        <f t="shared" ref="P16:P19" si="51">(K16 * 20 + M16 * 1000) /G16</f>
-        <v>144.16214677382195</v>
+        <f>(K16 * 20 + M16 * 1000) /G16</f>
+        <v>95.331641014164703</v>
       </c>
       <c r="Q16" s="3">
-        <f t="shared" si="50"/>
-        <v>22.378878073836518</v>
+        <f t="shared" ref="Q16:Q20" si="63">E16/I16*1000</f>
+        <v>26.005105154241893</v>
       </c>
       <c r="S16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="T16" t="s">
         <v>20</v>
       </c>
       <c r="U16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="V16">
         <v>1508497</v>
       </c>
       <c r="W16">
-        <v>433095.21756606997</v>
+        <v>1075401.7824339201</v>
       </c>
       <c r="X16">
-        <v>76705.702678003305</v>
+        <v>256661.78948319599</v>
       </c>
       <c r="Y16">
-        <v>76705.702678003305</v>
+        <v>256661.78948319599</v>
       </c>
       <c r="Z16">
-        <v>-3427.5937526859798</v>
+        <v>-9869.6693576464895</v>
       </c>
       <c r="AA16">
-        <v>-1239296.42624046</v>
+        <v>-2603507.5538759599</v>
       </c>
       <c r="AB16">
-        <v>490.93811708074998</v>
+        <v>1093.2241011594599</v>
       </c>
       <c r="AC16">
-        <v>99.429743860527694</v>
+        <v>97.120461780647304</v>
       </c>
       <c r="AD16">
-        <v>1.54242208490538</v>
+        <v>1.4176142732588399</v>
       </c>
       <c r="AE16">
-        <v>1.2712110424526899</v>
+        <v>1.20880713662942</v>
       </c>
       <c r="AF16">
-        <v>1.29246703168387</v>
+        <v>1.2170787234020499</v>
       </c>
       <c r="AG16">
-        <v>1.28420661060261</v>
+        <v>1.19612986147641</v>
       </c>
       <c r="AH16">
-        <v>1.45976774617307</v>
+        <v>1.3114935881152701</v>
       </c>
     </row>
     <row r="17" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" s="13" t="str">
-        <f>T17</f>
-        <v>[85,90)</v>
-      </c>
-      <c r="C17" s="12">
-        <v>940.56899999999996</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="B17" s="12"/>
+      <c r="C17" s="13"/>
       <c r="D17" s="9">
-        <f t="shared" si="39"/>
-        <v>344.41771727378898</v>
+        <f t="shared" si="52"/>
+        <v>433.09521756606995</v>
       </c>
       <c r="E17" s="3">
-        <f t="shared" si="40"/>
-        <v>46.752586205033197</v>
+        <f t="shared" si="53"/>
+        <v>76.705702678003306</v>
       </c>
       <c r="F17" s="5">
-        <f t="shared" si="41"/>
-        <v>1.61849319525765</v>
+        <f t="shared" si="54"/>
+        <v>1.54242208490538</v>
       </c>
       <c r="G17" s="9">
-        <f t="shared" si="42"/>
-        <v>46.752586205033197</v>
+        <f t="shared" si="55"/>
+        <v>76.705702678003306</v>
       </c>
       <c r="H17" s="5">
-        <f t="shared" si="43"/>
-        <v>1.3092465976288199</v>
+        <f t="shared" si="56"/>
+        <v>1.2712110424526899</v>
       </c>
       <c r="I17" s="9">
-        <f t="shared" si="44"/>
-        <v>1774.83334438626</v>
+        <f t="shared" si="57"/>
+        <v>3427.5937526859798</v>
       </c>
       <c r="J17" s="5">
-        <f t="shared" si="45"/>
-        <v>1.3315036541571701</v>
+        <f t="shared" si="58"/>
+        <v>1.29246703168387</v>
       </c>
       <c r="K17" s="9">
-        <f t="shared" si="46"/>
-        <v>167.63179439661999</v>
+        <f t="shared" si="59"/>
+        <v>490.93811708074998</v>
       </c>
       <c r="L17" s="5">
-        <f t="shared" si="47"/>
-        <v>1.3142805913895099</v>
+        <f t="shared" si="60"/>
+        <v>1.28420661060261</v>
       </c>
       <c r="M17" s="7">
-        <f t="shared" si="48"/>
-        <v>0.49919508742090102</v>
+        <f t="shared" si="61"/>
+        <v>1.23929642624046</v>
       </c>
       <c r="N17" s="5">
-        <f t="shared" si="49"/>
-        <v>1.5194933531599799</v>
+        <f t="shared" si="62"/>
+        <v>1.45976774617307</v>
       </c>
       <c r="O17" s="7">
-        <f>((SUM($K$3:$K$5)+ SUM($K$15:K17)) * 20 + (SUM($M$3:$M$5) + SUM($M$15:M17)) * 1000) /(SUM($G$3:$G$5) + SUM($G$15:G17))</f>
-        <v>98.934642820385761</v>
+        <f>((SUM($K$3:$K$5)+ SUM($K$16:K17)) * 20 + (SUM($M$3:$M$5) + SUM($M$16:M17)) * 1000) /(SUM($G$3:$G$5) + SUM($G$16:G17))</f>
+        <v>99.42974386052758</v>
       </c>
       <c r="P17" s="7">
-        <f t="shared" si="51"/>
-        <v>82.387548754225449</v>
+        <f t="shared" ref="P17:P20" si="64">(K17 * 20 + M17 * 1000) /G17</f>
+        <v>144.16214677382195</v>
       </c>
       <c r="Q17" s="3">
-        <f t="shared" si="50"/>
-        <v>26.341958445230986</v>
+        <f t="shared" si="63"/>
+        <v>22.378878073836518</v>
       </c>
       <c r="S17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="T17" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="U17" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="V17">
-        <v>940569</v>
+        <v>1508497</v>
       </c>
       <c r="W17">
-        <v>344417.71727378899</v>
+        <v>433095.21756606997</v>
       </c>
       <c r="X17">
-        <v>46752.5862050332</v>
+        <v>76705.702678003305</v>
       </c>
       <c r="Y17">
-        <v>46752.5862050332</v>
+        <v>76705.702678003305</v>
       </c>
       <c r="Z17">
-        <v>-1774.83334438626</v>
+        <v>-3427.5937526859798</v>
       </c>
       <c r="AA17">
-        <v>-499195.08742090099</v>
+        <v>-1239296.42624046</v>
       </c>
       <c r="AB17">
-        <v>167.63179439661999</v>
+        <v>490.93811708074998</v>
       </c>
       <c r="AC17">
-        <v>98.934642820385903</v>
+        <v>99.429743860527694</v>
       </c>
       <c r="AD17">
-        <v>1.61849319525765</v>
+        <v>1.54242208490538</v>
       </c>
       <c r="AE17">
-        <v>1.3092465976288199</v>
+        <v>1.2712110424526899</v>
       </c>
       <c r="AF17">
-        <v>1.3315036541571701</v>
+        <v>1.29246703168387</v>
       </c>
       <c r="AG17">
-        <v>1.3142805913895099</v>
+        <v>1.28420661060261</v>
       </c>
       <c r="AH17">
-        <v>1.5194933531599799</v>
+        <v>1.45976774617307</v>
       </c>
     </row>
     <row r="18" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>31</v>
-      </c>
-      <c r="B18" s="13"/>
-      <c r="C18" s="12"/>
+        <v>30</v>
+      </c>
+      <c r="B18" s="12" t="str">
+        <f>T18</f>
+        <v>[85,90)</v>
+      </c>
+      <c r="C18" s="13">
+        <v>940.56899999999996</v>
+      </c>
       <c r="D18" s="9">
-        <f t="shared" si="39"/>
-        <v>596.15128272620996</v>
+        <f t="shared" si="52"/>
+        <v>344.41771727378898</v>
       </c>
       <c r="E18" s="3">
-        <f t="shared" si="40"/>
-        <v>80.923869008580112</v>
+        <f t="shared" si="53"/>
+        <v>46.752586205033197</v>
       </c>
       <c r="F18" s="5">
-        <f t="shared" si="41"/>
-        <v>1.7501643832960401</v>
+        <f t="shared" si="54"/>
+        <v>1.61849319525765</v>
       </c>
       <c r="G18" s="9">
-        <f t="shared" si="42"/>
-        <v>80.923869008580112</v>
+        <f t="shared" si="55"/>
+        <v>46.752586205033197</v>
       </c>
       <c r="H18" s="5">
-        <f t="shared" si="43"/>
-        <v>1.37508219164802</v>
+        <f t="shared" si="56"/>
+        <v>1.3092465976288199</v>
       </c>
       <c r="I18" s="9">
-        <f t="shared" si="44"/>
-        <v>2719.1285037150701</v>
+        <f t="shared" si="57"/>
+        <v>1774.83334438626</v>
       </c>
       <c r="J18" s="5">
-        <f t="shared" si="45"/>
-        <v>1.3913096033701799</v>
+        <f t="shared" si="58"/>
+        <v>1.3315036541571701</v>
       </c>
       <c r="K18" s="9">
-        <f t="shared" si="46"/>
-        <v>411.530665807768</v>
+        <f t="shared" si="59"/>
+        <v>167.63179439661999</v>
       </c>
       <c r="L18" s="5">
-        <f t="shared" si="47"/>
-        <v>1.38811124732965</v>
+        <f t="shared" si="60"/>
+        <v>1.3142805913895099</v>
       </c>
       <c r="M18" s="7">
-        <f t="shared" si="48"/>
-        <v>1.2944099341038802</v>
+        <f t="shared" si="61"/>
+        <v>0.49919508742090102</v>
       </c>
       <c r="N18" s="5">
-        <f t="shared" si="49"/>
-        <v>1.6743615018103699</v>
+        <f t="shared" si="62"/>
+        <v>1.5194933531599799</v>
       </c>
       <c r="O18" s="7">
-        <f>((SUM($K$3:$K$5)+ SUM($K$15:K18)) * 20 + (SUM($M$3:$M$5) + SUM($M$15:M18)) * 1000) /(SUM($G$3:$G$5) + SUM($G$15:G18))</f>
-        <v>99.833250470974832</v>
+        <f>((SUM($K$3:$K$5)+ SUM($K$16:K18)) * 20 + (SUM($M$3:$M$5) + SUM($M$16:M18)) * 1000) /(SUM($G$3:$G$5) + SUM($G$16:G18))</f>
+        <v>98.934642820385761</v>
       </c>
       <c r="P18" s="7">
-        <f t="shared" si="51"/>
-        <v>117.70350783956377</v>
+        <f t="shared" si="64"/>
+        <v>82.387548754225449</v>
       </c>
       <c r="Q18" s="3">
-        <f t="shared" si="50"/>
-        <v>29.760957931195993</v>
+        <f t="shared" si="63"/>
+        <v>26.341958445230986</v>
       </c>
       <c r="S18" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="T18" t="s">
         <v>23</v>
       </c>
       <c r="U18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="V18">
         <v>940569</v>
       </c>
       <c r="W18">
-        <v>596151.28272620996</v>
+        <v>344417.71727378899</v>
       </c>
       <c r="X18">
-        <v>80923.869008580106</v>
+        <v>46752.5862050332</v>
       </c>
       <c r="Y18">
-        <v>80923.869008580106</v>
+        <v>46752.5862050332</v>
       </c>
       <c r="Z18">
-        <v>-2719.1285037150701</v>
+        <v>-1774.83334438626</v>
       </c>
       <c r="AA18">
-        <v>-1294409.9341038801</v>
+        <v>-499195.08742090099</v>
       </c>
       <c r="AB18">
-        <v>411.530665807768</v>
+        <v>167.63179439661999</v>
       </c>
       <c r="AC18">
-        <v>99.833250470974903</v>
+        <v>98.934642820385903</v>
       </c>
       <c r="AD18">
-        <v>1.7501643832960401</v>
+        <v>1.61849319525765</v>
       </c>
       <c r="AE18">
-        <v>1.37508219164802</v>
+        <v>1.3092465976288199</v>
       </c>
       <c r="AF18">
-        <v>1.3913096033701799</v>
+        <v>1.3315036541571701</v>
       </c>
       <c r="AG18">
-        <v>1.38811124732965</v>
+        <v>1.3142805913895099</v>
       </c>
       <c r="AH18">
-        <v>1.6743615018103699</v>
+        <v>1.5194933531599799</v>
       </c>
     </row>
     <row r="19" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="10" t="str">
-        <f>T19</f>
-        <v>[90,95)</v>
-      </c>
-      <c r="C19" s="11">
-        <v>417.13799999999998</v>
-      </c>
+      <c r="B19" s="12"/>
+      <c r="C19" s="13"/>
       <c r="D19" s="9">
-        <f t="shared" si="39"/>
-        <v>417.13799999999998</v>
+        <f t="shared" si="52"/>
+        <v>596.15128272620996</v>
       </c>
       <c r="E19" s="3">
-        <f t="shared" si="40"/>
-        <v>56.6239171978836</v>
+        <f t="shared" si="53"/>
+        <v>80.923869008580112</v>
       </c>
       <c r="F19" s="5">
-        <f t="shared" si="41"/>
-        <v>1.8422971315219401</v>
+        <f t="shared" si="54"/>
+        <v>1.7501643832960401</v>
       </c>
       <c r="G19" s="9">
-        <f t="shared" si="42"/>
-        <v>56.6239171978836</v>
+        <f t="shared" si="55"/>
+        <v>80.923869008580112</v>
       </c>
       <c r="H19" s="5">
-        <f t="shared" si="43"/>
-        <v>1.4211485657609699</v>
+        <f t="shared" si="56"/>
+        <v>1.37508219164802</v>
       </c>
       <c r="I19" s="9">
-        <f t="shared" si="44"/>
-        <v>1398.2286690972801</v>
+        <f t="shared" si="57"/>
+        <v>2719.1285037150701</v>
       </c>
       <c r="J19" s="5">
-        <f t="shared" si="45"/>
-        <v>1.4220629836013701</v>
+        <f t="shared" si="58"/>
+        <v>1.3913096033701799</v>
       </c>
       <c r="K19" s="9">
-        <f t="shared" si="46"/>
-        <v>215.06649113910299</v>
+        <f t="shared" si="59"/>
+        <v>411.530665807768</v>
       </c>
       <c r="L19" s="5">
-        <f t="shared" si="47"/>
-        <v>1.4266952495215099</v>
+        <f t="shared" si="60"/>
+        <v>1.38811124732965</v>
       </c>
       <c r="M19" s="7">
-        <f t="shared" si="48"/>
-        <v>0.78007425764216398</v>
+        <f t="shared" si="61"/>
+        <v>1.2944099341038802</v>
       </c>
       <c r="N19" s="5">
-        <f t="shared" si="49"/>
-        <v>1.76769256556994</v>
+        <f t="shared" si="62"/>
+        <v>1.6743615018103699</v>
       </c>
       <c r="O19" s="7">
-        <f>((SUM($K$3:$K$5)+ SUM($K$15:K19)) * 20 + (SUM($M$3:$M$5) + SUM($M$15:M19)) * 1000) /(SUM($G$3:$G$5) + SUM($G$15:G19))</f>
-        <v>99.506063843051706</v>
+        <f>((SUM($K$3:$K$5)+ SUM($K$16:K19)) * 20 + (SUM($M$3:$M$5) + SUM($M$16:M19)) * 1000) /(SUM($G$3:$G$5) + SUM($G$16:G19))</f>
+        <v>99.833250470974832</v>
       </c>
       <c r="P19" s="7">
-        <f t="shared" si="51"/>
-        <v>89.73953643415804</v>
+        <f t="shared" si="64"/>
+        <v>117.70350783956377</v>
       </c>
       <c r="Q19" s="3">
-        <f t="shared" si="50"/>
-        <v>40.496893283157291</v>
+        <f t="shared" si="63"/>
+        <v>29.760957931195993</v>
       </c>
       <c r="S19" t="s">
         <v>24</v>
       </c>
       <c r="T19" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="U19" t="s">
         <v>52</v>
       </c>
       <c r="V19">
+        <v>940569</v>
+      </c>
+      <c r="W19">
+        <v>596151.28272620996</v>
+      </c>
+      <c r="X19">
+        <v>80923.869008580106</v>
+      </c>
+      <c r="Y19">
+        <v>80923.869008580106</v>
+      </c>
+      <c r="Z19">
+        <v>-2719.1285037150701</v>
+      </c>
+      <c r="AA19">
+        <v>-1294409.9341038801</v>
+      </c>
+      <c r="AB19">
+        <v>411.530665807768</v>
+      </c>
+      <c r="AC19">
+        <v>99.833250470974903</v>
+      </c>
+      <c r="AD19">
+        <v>1.7501643832960401</v>
+      </c>
+      <c r="AE19">
+        <v>1.37508219164802</v>
+      </c>
+      <c r="AF19">
+        <v>1.3913096033701799</v>
+      </c>
+      <c r="AG19">
+        <v>1.38811124732965</v>
+      </c>
+      <c r="AH19">
+        <v>1.6743615018103699</v>
+      </c>
+    </row>
+    <row r="20" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="10" t="str">
+        <f>T20</f>
+        <v>[90,95)</v>
+      </c>
+      <c r="C20" s="11">
+        <v>417.13799999999998</v>
+      </c>
+      <c r="D20" s="9">
+        <f t="shared" si="52"/>
+        <v>417.13799999999998</v>
+      </c>
+      <c r="E20" s="3">
+        <f t="shared" si="53"/>
+        <v>56.6239171978836</v>
+      </c>
+      <c r="F20" s="5">
+        <f t="shared" si="54"/>
+        <v>1.8422971315219401</v>
+      </c>
+      <c r="G20" s="9">
+        <f t="shared" si="55"/>
+        <v>56.6239171978836</v>
+      </c>
+      <c r="H20" s="5">
+        <f t="shared" si="56"/>
+        <v>1.4211485657609699</v>
+      </c>
+      <c r="I20" s="9">
+        <f t="shared" si="57"/>
+        <v>1398.2286690972801</v>
+      </c>
+      <c r="J20" s="5">
+        <f t="shared" si="58"/>
+        <v>1.4220629836013701</v>
+      </c>
+      <c r="K20" s="9">
+        <f t="shared" si="59"/>
+        <v>215.06649113910299</v>
+      </c>
+      <c r="L20" s="5">
+        <f t="shared" si="60"/>
+        <v>1.4266952495215099</v>
+      </c>
+      <c r="M20" s="7">
+        <f t="shared" si="61"/>
+        <v>0.78007425764216398</v>
+      </c>
+      <c r="N20" s="5">
+        <f t="shared" si="62"/>
+        <v>1.76769256556994</v>
+      </c>
+      <c r="O20" s="7">
+        <f>((SUM($K$3:$K$5)+ SUM($K$16:K20)) * 20 + (SUM($M$3:$M$5) + SUM($M$16:M20)) * 1000) /(SUM($G$3:$G$5) + SUM($G$16:G20))</f>
+        <v>99.506063843051706</v>
+      </c>
+      <c r="P20" s="7">
+        <f t="shared" si="64"/>
+        <v>89.73953643415804</v>
+      </c>
+      <c r="Q20" s="3">
+        <f t="shared" si="63"/>
+        <v>40.496893283157291</v>
+      </c>
+      <c r="S20" t="s">
+        <v>24</v>
+      </c>
+      <c r="T20" t="s">
+        <v>25</v>
+      </c>
+      <c r="U20" t="s">
+        <v>52</v>
+      </c>
+      <c r="V20">
         <v>417138</v>
       </c>
-      <c r="W19">
+      <c r="W20">
         <v>417138</v>
       </c>
-      <c r="X19">
+      <c r="X20">
         <v>56623.917197883602</v>
       </c>
-      <c r="Y19">
+      <c r="Y20">
         <v>56623.917197883602</v>
       </c>
-      <c r="Z19">
+      <c r="Z20">
         <v>-1398.2286690972801</v>
       </c>
-      <c r="AA19">
+      <c r="AA20">
         <v>-780074.25764216401</v>
       </c>
-      <c r="AB19">
+      <c r="AB20">
         <v>215.06649113910299</v>
       </c>
-      <c r="AC19">
+      <c r="AC20">
         <v>99.506063843051805</v>
       </c>
-      <c r="AD19">
+      <c r="AD20">
         <v>1.8422971315219401</v>
       </c>
-      <c r="AE19">
+      <c r="AE20">
         <v>1.4211485657609699</v>
       </c>
-      <c r="AF19">
+      <c r="AF20">
         <v>1.4220629836013701</v>
       </c>
-      <c r="AG19">
+      <c r="AG20">
         <v>1.4266952495215099</v>
       </c>
-      <c r="AH19">
+      <c r="AH20">
         <v>1.76769256556994</v>
       </c>
     </row>
-    <row r="22" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="D22" s="9">
+    <row r="21" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="10" t="str">
+        <f>T21</f>
+        <v>[95,100)</v>
+      </c>
+      <c r="C21" s="11">
+        <v>418.13799999999998</v>
+      </c>
+      <c r="D21" s="9">
+        <f t="shared" ref="D21" si="65">W21/1000</f>
+        <v>109.06399999999999</v>
+      </c>
+      <c r="E21" s="3">
+        <f t="shared" ref="E21" si="66">X21 / 1000</f>
+        <v>14.804767020194701</v>
+      </c>
+      <c r="F21" s="5">
+        <f t="shared" ref="F21" si="67">AD21</f>
+        <v>1.8663859607643201</v>
+      </c>
+      <c r="G21" s="9">
+        <f t="shared" ref="G21" si="68">Y21 / 1000</f>
+        <v>14.804767020194701</v>
+      </c>
+      <c r="H21" s="5">
+        <f t="shared" ref="H21" si="69">AE21</f>
+        <v>1.4331929803821599</v>
+      </c>
+      <c r="I21" s="9">
+        <f t="shared" ref="I21" si="70">-Z21</f>
+        <v>234.88374918093501</v>
+      </c>
+      <c r="J21" s="5">
+        <f t="shared" ref="J21" si="71">AF21</f>
+        <v>1.42722914090335</v>
+      </c>
+      <c r="K21" s="9">
+        <f t="shared" ref="K21" si="72">AB21</f>
+        <v>34.359355486366802</v>
+      </c>
+      <c r="L21" s="5">
+        <f t="shared" ref="L21" si="73">AG21</f>
+        <v>1.43285948942879</v>
+      </c>
+      <c r="M21" s="7">
+        <f t="shared" ref="M21" si="74">-AA21/1000000</f>
+        <v>0.12997330756768199</v>
+      </c>
+      <c r="N21" s="5">
+        <f t="shared" ref="N21" si="75">AH21</f>
+        <v>1.78324306853398</v>
+      </c>
+      <c r="O21" s="7">
+        <f>((SUM($K$3:$K$5)+ SUM($K$16:K21)) * 20 + (SUM($M$3:$M$5) + SUM($M$16:M21)) * 1000) /(SUM($G$3:$G$5) + SUM($G$16:G21))</f>
+        <v>99.133684381171406</v>
+      </c>
+      <c r="P21" s="7">
+        <f t="shared" ref="P21" si="76">(K21 * 20 + M21 * 1000) /G21</f>
+        <v>55.195763376779666</v>
+      </c>
+      <c r="Q21" s="3">
+        <f t="shared" ref="Q21" si="77">E21/I21*1000</f>
+        <v>63.03018864361848</v>
+      </c>
+      <c r="S21" t="s">
+        <v>56</v>
+      </c>
+      <c r="T21" t="s">
+        <v>55</v>
+      </c>
+      <c r="U21" t="s">
+        <v>52</v>
+      </c>
+      <c r="V21">
+        <v>109064</v>
+      </c>
+      <c r="W21">
+        <v>109064</v>
+      </c>
+      <c r="X21">
+        <v>14804.7670201947</v>
+      </c>
+      <c r="Y21">
+        <v>14804.7670201947</v>
+      </c>
+      <c r="Z21">
+        <v>-234.88374918093501</v>
+      </c>
+      <c r="AA21">
+        <v>-129973.307567682</v>
+      </c>
+      <c r="AB21">
+        <v>34.359355486366802</v>
+      </c>
+      <c r="AC21">
+        <v>99.133684381171506</v>
+      </c>
+      <c r="AD21">
+        <v>1.8663859607643201</v>
+      </c>
+      <c r="AE21">
+        <v>1.4331929803821599</v>
+      </c>
+      <c r="AF21">
+        <v>1.42722914090335</v>
+      </c>
+      <c r="AG21">
+        <v>1.43285948942879</v>
+      </c>
+      <c r="AH21">
+        <v>1.78324306853398</v>
+      </c>
+    </row>
+    <row r="24" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="D24" s="9">
         <f>SUM(D3:D5)</f>
         <v>2168.6131270308952</v>
       </c>
-      <c r="E22" s="9">
+      <c r="E24" s="9">
         <f>SUM(E3:E5)</f>
         <v>614.59055860409251</v>
       </c>
-      <c r="G22" s="9">
+      <c r="G24" s="9">
         <f>SUM(G3:G5)</f>
         <v>1229.1811172081859</v>
       </c>
-      <c r="K22" s="9">
+      <c r="K24" s="9">
         <f>SUM(K3:K5)</f>
         <v>5573.9808967893359</v>
       </c>
-      <c r="M22" s="9">
+      <c r="M24" s="9">
         <f>SUM(M3:M5)</f>
         <v>8.3581417185142399</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="A14:O14"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="A7:O7"/>
+    <mergeCell ref="A4:A5"/>
     <mergeCell ref="M1:N1"/>
     <mergeCell ref="K1:L1"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="C8:C9"/>
     <mergeCell ref="I1:J1"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="A7:O7"/>
-    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="A15:O15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F782D18A-8F87-4860-9C5B-20DBEF4FE7B3}">
+  <dimension ref="A1:M21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.28515625" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" customWidth="1"/>
+    <col min="13" max="13" width="16.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="J1" s="16"/>
+      <c r="K1" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="L1" s="15"/>
+      <c r="M1" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" s="9">
+        <v>640.87300000000005</v>
+      </c>
+      <c r="E3" s="9">
+        <v>617.97544771172397</v>
+      </c>
+      <c r="F3" s="5">
+        <v>0.50275377571315005</v>
+      </c>
+      <c r="G3" s="9">
+        <v>23217.646533121999</v>
+      </c>
+      <c r="H3" s="5">
+        <v>0.51066118703414098</v>
+      </c>
+      <c r="I3" s="9">
+        <v>2746.9011358783</v>
+      </c>
+      <c r="J3" s="5">
+        <v>0.49280777719574498</v>
+      </c>
+      <c r="K3" s="7">
+        <v>3.5657284397508398</v>
+      </c>
+      <c r="L3" s="5">
+        <v>0.42661737020471202</v>
+      </c>
+      <c r="M3" s="7">
+        <v>94.670025118227699</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="19"/>
+      <c r="B4" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="20"/>
+      <c r="D4" s="9">
+        <v>1053.4762497747899</v>
+      </c>
+      <c r="E4" s="9">
+        <v>482.44886232139299</v>
+      </c>
+      <c r="F4" s="5">
+        <v>0.89524993072826198</v>
+      </c>
+      <c r="G4" s="9">
+        <v>17934.2966911322</v>
+      </c>
+      <c r="H4" s="5">
+        <v>0.90511758569844303</v>
+      </c>
+      <c r="I4" s="9">
+        <v>2252.21658121984</v>
+      </c>
+      <c r="J4" s="5">
+        <v>0.89686667566042</v>
+      </c>
+      <c r="K4" s="7">
+        <v>3.6212972172669802</v>
+      </c>
+      <c r="L4" s="5">
+        <v>0.85988320120221595</v>
+      </c>
+      <c r="M4" s="7">
+        <v>97.3891425533443</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="19"/>
+      <c r="B5" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="20"/>
+      <c r="D5" s="9">
+        <v>474.26387725610499</v>
+      </c>
+      <c r="E5" s="9">
+        <v>128.75680717506901</v>
+      </c>
+      <c r="F5" s="5">
+        <v>1</v>
+      </c>
+      <c r="G5" s="9">
+        <v>4313.9099140414901</v>
+      </c>
+      <c r="H5" s="5">
+        <v>1</v>
+      </c>
+      <c r="I5" s="9">
+        <v>574.86317969119602</v>
+      </c>
+      <c r="J5" s="5">
+        <v>1</v>
+      </c>
+      <c r="K5" s="7">
+        <v>1.17111606149642</v>
+      </c>
+      <c r="L5" s="5">
+        <v>1</v>
+      </c>
+      <c r="M5" s="7">
+        <v>97.493980322839803</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="7"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="14"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="D8" s="9">
+        <v>1075.4017824339201</v>
+      </c>
+      <c r="E8" s="9">
+        <v>145.979175915393</v>
+      </c>
+      <c r="F8" s="5">
+        <v>1.1187613231864</v>
+      </c>
+      <c r="G8" s="9">
+        <v>5467.3873239638797</v>
+      </c>
+      <c r="H8" s="5">
+        <v>1.1202526060015501</v>
+      </c>
+      <c r="I8" s="9">
+        <v>601.68272542949398</v>
+      </c>
+      <c r="J8" s="5">
+        <v>1.10794488473687</v>
+      </c>
+      <c r="K8" s="7">
+        <v>1.49042303305565</v>
+      </c>
+      <c r="L8" s="5">
+        <v>1.17831990450152</v>
+      </c>
+      <c r="M8" s="7">
+        <v>96.979121534279145</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="12"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="9">
+        <v>433.09521756606995</v>
+      </c>
+      <c r="E9" s="9">
+        <v>58.790011311030398</v>
+      </c>
+      <c r="F9" s="5">
+        <v>1.16658992264013</v>
+      </c>
+      <c r="G9" s="9">
+        <v>2563.8673259979701</v>
+      </c>
+      <c r="H9" s="5">
+        <v>1.17664365882528</v>
+      </c>
+      <c r="I9" s="9">
+        <v>369.71672149104398</v>
+      </c>
+      <c r="J9" s="5">
+        <v>1.1742739103178601</v>
+      </c>
+      <c r="K9" s="7">
+        <v>0.95624048615763502</v>
+      </c>
+      <c r="L9" s="5">
+        <v>1.2927281687260199</v>
+      </c>
+      <c r="M9" s="7">
+        <v>98.826585324238735</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="20"/>
+      <c r="D10" s="9">
+        <v>344.41771727378898</v>
+      </c>
+      <c r="E10" s="9">
+        <v>46.752586205033197</v>
+      </c>
+      <c r="F10" s="5">
+        <v>1.2046254778162599</v>
+      </c>
+      <c r="G10" s="9">
+        <v>1774.83334438626</v>
+      </c>
+      <c r="H10" s="5">
+        <v>1.2156802812985901</v>
+      </c>
+      <c r="I10" s="9">
+        <v>167.63179439661999</v>
+      </c>
+      <c r="J10" s="5">
+        <v>1.20434789110476</v>
+      </c>
+      <c r="K10" s="7">
+        <v>0.49919508742090102</v>
+      </c>
+      <c r="L10" s="5">
+        <v>1.35245377571294</v>
+      </c>
+      <c r="M10" s="7">
+        <v>98.307529489860457</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="12"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="9">
+        <v>596.15128272620996</v>
+      </c>
+      <c r="E11" s="9">
+        <v>80.923869008580112</v>
+      </c>
+      <c r="F11" s="5">
+        <v>1.2704610718354601</v>
+      </c>
+      <c r="G11" s="9">
+        <v>2719.1285037150701</v>
+      </c>
+      <c r="H11" s="5">
+        <v>1.2754862305115999</v>
+      </c>
+      <c r="I11" s="9">
+        <v>411.530665807768</v>
+      </c>
+      <c r="J11" s="5">
+        <v>1.2781785470449001</v>
+      </c>
+      <c r="K11" s="7">
+        <v>1.2944099341038802</v>
+      </c>
+      <c r="L11" s="5">
+        <v>1.50732192436332</v>
+      </c>
+      <c r="M11" s="7">
+        <v>99.312633687497438</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="20"/>
+      <c r="D12" s="9">
+        <v>417.13799999999998</v>
+      </c>
+      <c r="E12" s="9">
+        <v>56.6239171978836</v>
+      </c>
+      <c r="F12" s="5">
+        <v>1.31652744594841</v>
+      </c>
+      <c r="G12" s="9">
+        <v>1398.2286690972801</v>
+      </c>
+      <c r="H12" s="5">
+        <v>1.3062396107427801</v>
+      </c>
+      <c r="I12" s="9">
+        <v>215.06649113910299</v>
+      </c>
+      <c r="J12" s="5">
+        <v>1.3167625492367601</v>
+      </c>
+      <c r="K12" s="7">
+        <v>0.78007425764216398</v>
+      </c>
+      <c r="L12" s="5">
+        <v>1.6006529881228899</v>
+      </c>
+      <c r="M12" s="7">
+        <v>98.977663170286334</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" s="20"/>
+      <c r="D13" s="9">
+        <v>109.06399999999999</v>
+      </c>
+      <c r="E13" s="9">
+        <v>14.804767020194701</v>
+      </c>
+      <c r="F13" s="5">
+        <v>1.3285718605696</v>
+      </c>
+      <c r="G13" s="9">
+        <v>234.88374918093501</v>
+      </c>
+      <c r="H13" s="5">
+        <v>1.3114057680447599</v>
+      </c>
+      <c r="I13" s="9">
+        <v>34.359355486366802</v>
+      </c>
+      <c r="J13" s="5">
+        <v>1.3229267891440299</v>
+      </c>
+      <c r="K13" s="7">
+        <v>0.12997330756768199</v>
+      </c>
+      <c r="L13" s="5">
+        <v>1.6162034910869401</v>
+      </c>
+      <c r="M13" s="7">
+        <v>98.58075023718358</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="7"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="14"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="D16" s="9">
+        <v>1075.4017824339201</v>
+      </c>
+      <c r="E16" s="9">
+        <v>256.661789483196</v>
+      </c>
+      <c r="F16" s="5">
+        <v>1.20880713662942</v>
+      </c>
+      <c r="G16" s="9">
+        <v>9869.6693576464895</v>
+      </c>
+      <c r="H16" s="5">
+        <v>1.2170787234020499</v>
+      </c>
+      <c r="I16" s="9">
+        <v>1093.2241011594599</v>
+      </c>
+      <c r="J16" s="5">
+        <v>1.19612986147641</v>
+      </c>
+      <c r="K16" s="7">
+        <v>2.6035075538759598</v>
+      </c>
+      <c r="L16" s="5">
+        <v>1.3114935881152701</v>
+      </c>
+      <c r="M16" s="7">
+        <v>97.120461780647219</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="12"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="9">
+        <v>433.09521756606995</v>
+      </c>
+      <c r="E17" s="9">
+        <v>76.705702678003306</v>
+      </c>
+      <c r="F17" s="5">
+        <v>1.2712110424526899</v>
+      </c>
+      <c r="G17" s="9">
+        <v>3427.5937526859798</v>
+      </c>
+      <c r="H17" s="5">
+        <v>1.29246703168387</v>
+      </c>
+      <c r="I17" s="9">
+        <v>490.93811708074998</v>
+      </c>
+      <c r="J17" s="5">
+        <v>1.28420661060261</v>
+      </c>
+      <c r="K17" s="7">
+        <v>1.23929642624046</v>
+      </c>
+      <c r="L17" s="5">
+        <v>1.45976774617307</v>
+      </c>
+      <c r="M17" s="7">
+        <v>99.42974386052758</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="20"/>
+      <c r="D18" s="9">
+        <v>344.41771727378898</v>
+      </c>
+      <c r="E18" s="9">
+        <v>46.752586205033197</v>
+      </c>
+      <c r="F18" s="5">
+        <v>1.3092465976288199</v>
+      </c>
+      <c r="G18" s="9">
+        <v>1774.83334438626</v>
+      </c>
+      <c r="H18" s="5">
+        <v>1.3315036541571701</v>
+      </c>
+      <c r="I18" s="9">
+        <v>167.63179439661999</v>
+      </c>
+      <c r="J18" s="5">
+        <v>1.3142805913895099</v>
+      </c>
+      <c r="K18" s="7">
+        <v>0.49919508742090102</v>
+      </c>
+      <c r="L18" s="5">
+        <v>1.5194933531599799</v>
+      </c>
+      <c r="M18" s="7">
+        <v>98.934642820385761</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="12"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="9">
+        <v>596.15128272620996</v>
+      </c>
+      <c r="E19" s="9">
+        <v>80.923869008580112</v>
+      </c>
+      <c r="F19" s="5">
+        <v>1.37508219164802</v>
+      </c>
+      <c r="G19" s="9">
+        <v>2719.1285037150701</v>
+      </c>
+      <c r="H19" s="5">
+        <v>1.3913096033701799</v>
+      </c>
+      <c r="I19" s="9">
+        <v>411.530665807768</v>
+      </c>
+      <c r="J19" s="5">
+        <v>1.38811124732965</v>
+      </c>
+      <c r="K19" s="7">
+        <v>1.2944099341038802</v>
+      </c>
+      <c r="L19" s="5">
+        <v>1.6743615018103699</v>
+      </c>
+      <c r="M19" s="7">
+        <v>99.833250470974832</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="20"/>
+      <c r="D20" s="9">
+        <v>417.13799999999998</v>
+      </c>
+      <c r="E20" s="9">
+        <v>56.6239171978836</v>
+      </c>
+      <c r="F20" s="5">
+        <v>1.4211485657609699</v>
+      </c>
+      <c r="G20" s="9">
+        <v>1398.2286690972801</v>
+      </c>
+      <c r="H20" s="5">
+        <v>1.4220629836013701</v>
+      </c>
+      <c r="I20" s="9">
+        <v>215.06649113910299</v>
+      </c>
+      <c r="J20" s="5">
+        <v>1.4266952495215099</v>
+      </c>
+      <c r="K20" s="7">
+        <v>0.78007425764216398</v>
+      </c>
+      <c r="L20" s="5">
+        <v>1.76769256556994</v>
+      </c>
+      <c r="M20" s="7">
+        <v>99.506063843051706</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" s="20"/>
+      <c r="D21" s="9">
+        <v>109.06399999999999</v>
+      </c>
+      <c r="E21" s="9">
+        <v>14.804767020194701</v>
+      </c>
+      <c r="F21" s="5">
+        <v>1.4331929803821599</v>
+      </c>
+      <c r="G21" s="9">
+        <v>234.88374918093501</v>
+      </c>
+      <c r="H21" s="5">
+        <v>1.42722914090335</v>
+      </c>
+      <c r="I21" s="9">
+        <v>34.359355486366802</v>
+      </c>
+      <c r="J21" s="5">
+        <v>1.43285948942879</v>
+      </c>
+      <c r="K21" s="7">
+        <v>0.12997330756768199</v>
+      </c>
+      <c r="L21" s="5">
+        <v>1.78324306853398</v>
+      </c>
+      <c r="M21" s="7">
+        <v>99.133684381171406</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="C16:C21"/>
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="C8:C13"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="A7:M7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="A15:M15"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="K1:L1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Append 2 doses programme
</commit_message>
<xml_diff>
--- a/docs/tabs/Tab_ProgrammeProfile.xlsx
+++ b/docs/tabs/Tab_ProgrammeProfile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\HPRU\Shingrix\HPRU_RZV\docs\tabs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32AA0869-788C-47AE-8EDC-C32930B52F0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5636B00-725A-4EA7-AEF4-7A0D0D1F6C35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="67">
   <si>
     <t>Eligibility</t>
   </si>
@@ -253,6 +253,39 @@
   </si>
   <si>
     <t>cum. %</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Additional eligibility 3: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Keeping 80+ eligible</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Additional eligibility 4: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Those who reach age 80 years be called in on 80th birthday, keeping eligibility for higher ages to catch-up</t>
+    </r>
+  </si>
+  <si>
+    <t>ReVac_RZV_2d</t>
   </si>
 </sst>
 </file>
@@ -326,14 +359,17 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -345,13 +381,10 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -633,10 +666,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AH24"/>
+  <dimension ref="A1:AH37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S24" sqref="S24:AH29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -672,26 +705,26 @@
       <c r="D1" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="17"/>
-      <c r="G1" s="16" t="s">
+      <c r="F1" s="18"/>
+      <c r="G1" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16" t="s">
+      <c r="H1" s="17"/>
+      <c r="I1" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16" t="s">
+      <c r="J1" s="17"/>
+      <c r="K1" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="L1" s="16"/>
-      <c r="M1" s="15" t="s">
+      <c r="L1" s="17"/>
+      <c r="M1" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="N1" s="15"/>
+      <c r="N1" s="16"/>
       <c r="O1" s="6" t="s">
         <v>38</v>
       </c>
@@ -912,7 +945,7 @@
       </c>
     </row>
     <row r="4" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="15" t="s">
         <v>43</v>
       </c>
       <c r="B4" s="10" t="str">
@@ -1029,7 +1062,7 @@
       </c>
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A5" s="18"/>
+      <c r="A5" s="15"/>
       <c r="B5" s="10" t="str">
         <f t="shared" si="1"/>
         <v>[75,80)</v>
@@ -1174,11 +1207,11 @@
       <c r="A8" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="12" t="str">
+      <c r="B8" s="13" t="str">
         <f>T8</f>
         <v>[80,85)</v>
       </c>
-      <c r="C8" s="13">
+      <c r="C8" s="12">
         <f>V8/1000</f>
         <v>1508.4970000000001</v>
       </c>
@@ -1291,8 +1324,8 @@
       <c r="A9" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="12"/>
-      <c r="C9" s="13"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="12"/>
       <c r="D9" s="9">
         <f t="shared" ref="D9:D12" si="27">W9/1000</f>
         <v>433.09521756606995</v>
@@ -1402,11 +1435,11 @@
       <c r="A10" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="12" t="str">
+      <c r="B10" s="13" t="str">
         <f>T10</f>
         <v>[85,90)</v>
       </c>
-      <c r="C10" s="13">
+      <c r="C10" s="12">
         <f>V10/1000</f>
         <v>940.56899999999996</v>
       </c>
@@ -1519,8 +1552,8 @@
       <c r="A11" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="12"/>
-      <c r="C11" s="13"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="12"/>
       <c r="D11" s="9">
         <f t="shared" si="27"/>
         <v>596.15128272620996</v>
@@ -1889,10 +1922,10 @@
       <c r="A16" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="13">
+      <c r="C16" s="12">
         <v>1508.4970000000001</v>
       </c>
       <c r="D16" s="9">
@@ -2004,8 +2037,8 @@
       <c r="A17" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="12"/>
-      <c r="C17" s="13"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="12"/>
       <c r="D17" s="9">
         <f t="shared" si="52"/>
         <v>433.09521756606995</v>
@@ -2115,11 +2148,11 @@
       <c r="A18" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="12" t="str">
+      <c r="B18" s="13" t="str">
         <f>T18</f>
         <v>[85,90)</v>
       </c>
-      <c r="C18" s="13">
+      <c r="C18" s="12">
         <v>940.56899999999996</v>
       </c>
       <c r="D18" s="9">
@@ -2231,8 +2264,8 @@
       <c r="A19" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="12"/>
-      <c r="C19" s="13"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="12"/>
       <c r="D19" s="9">
         <f t="shared" si="52"/>
         <v>596.15128272620996</v>
@@ -2570,46 +2603,1456 @@
         <v>1.78324306853398</v>
       </c>
     </row>
+    <row r="23" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A23" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="B23" s="14"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="14"/>
+      <c r="J23" s="14"/>
+      <c r="K23" s="14"/>
+      <c r="L23" s="14"/>
+      <c r="M23" s="14"/>
+      <c r="N23" s="14"/>
+      <c r="O23" s="14"/>
+      <c r="P23" s="7"/>
+      <c r="Q23" s="3"/>
+    </row>
     <row r="24" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" s="13" t="str">
+        <f>T24</f>
+        <v>[80,85)</v>
+      </c>
+      <c r="C24" s="12">
+        <f>V24/1000</f>
+        <v>1508.4970000000001</v>
+      </c>
       <c r="D24" s="9">
-        <f>SUM(D3:D5)</f>
-        <v>2168.6131270308952</v>
-      </c>
-      <c r="E24" s="9">
-        <f>SUM(E3:E5)</f>
-        <v>614.59055860409251</v>
+        <f>W24/1000</f>
+        <v>1075.4017819999999</v>
+      </c>
+      <c r="E24" s="3">
+        <f t="shared" ref="E24:E29" si="78">X24 / 1000</f>
+        <v>145.9791759</v>
+      </c>
+      <c r="F24" s="5">
+        <f t="shared" ref="F24:F29" si="79">AD24</f>
+        <v>1.2375226459999999</v>
       </c>
       <c r="G24" s="9">
-        <f>SUM(G3:G5)</f>
-        <v>1229.1811172081859</v>
+        <f t="shared" ref="G24:G29" si="80">Y24 / 1000</f>
+        <v>291.9583518</v>
+      </c>
+      <c r="H24" s="5">
+        <f t="shared" ref="H24:H29" si="81">AE24</f>
+        <v>1.2375226459999999</v>
+      </c>
+      <c r="I24" s="9">
+        <f t="shared" ref="I24:I29" si="82">-Z24</f>
+        <v>5467.3873240000003</v>
+      </c>
+      <c r="J24" s="5">
+        <f t="shared" ref="J24:J29" si="83">AF24</f>
+        <v>1.120252606</v>
       </c>
       <c r="K24" s="9">
-        <f>SUM(K3:K5)</f>
-        <v>5573.9808967893359</v>
-      </c>
-      <c r="M24" s="9">
-        <f>SUM(M3:M5)</f>
-        <v>8.3581417185142399</v>
+        <f t="shared" ref="K24:K29" si="84">AB24</f>
+        <v>601.68272539999998</v>
+      </c>
+      <c r="L24" s="5">
+        <f t="shared" ref="L24:L29" si="85">AG24</f>
+        <v>1.107944885</v>
+      </c>
+      <c r="M24" s="7">
+        <f t="shared" ref="M24:M29" si="86">-AA24/1000000</f>
+        <v>1.4904230330000001</v>
+      </c>
+      <c r="N24" s="5">
+        <f t="shared" ref="N24:N29" si="87">AH24</f>
+        <v>1.1783199049999999</v>
+      </c>
+      <c r="O24" s="7">
+        <f>((SUM($K$3:$K$5)+ SUM($K$24:K24)) * 20 + (SUM($M$3:$M$5) + SUM($M$24:M24)) * 1000) /(SUM($G$3:$G$5) + SUM($G$24:G24))</f>
+        <v>87.672327168169275</v>
+      </c>
+      <c r="P24" s="7">
+        <f>(K24 * 20 + M24 * 1000) /G24</f>
+        <v>46.321940981035496</v>
+      </c>
+      <c r="Q24" s="3">
+        <f t="shared" ref="Q24:Q29" si="88">E24/I24*1000</f>
+        <v>26.699987992290261</v>
+      </c>
+      <c r="S24" t="s">
+        <v>19</v>
+      </c>
+      <c r="T24" t="s">
+        <v>20</v>
+      </c>
+      <c r="U24" t="s">
+        <v>66</v>
+      </c>
+      <c r="V24">
+        <v>1508497</v>
+      </c>
+      <c r="W24">
+        <v>1075401.7819999999</v>
+      </c>
+      <c r="X24">
+        <v>145979.1759</v>
+      </c>
+      <c r="Y24">
+        <v>291958.3518</v>
+      </c>
+      <c r="Z24">
+        <v>-5467.3873240000003</v>
+      </c>
+      <c r="AA24">
+        <v>-1490423.0330000001</v>
+      </c>
+      <c r="AB24">
+        <v>601.68272539999998</v>
+      </c>
+      <c r="AC24">
+        <v>96.97912153</v>
+      </c>
+      <c r="AD24">
+        <v>1.2375226459999999</v>
+      </c>
+      <c r="AE24">
+        <v>1.2375226459999999</v>
+      </c>
+      <c r="AF24">
+        <v>1.120252606</v>
+      </c>
+      <c r="AG24">
+        <v>1.107944885</v>
+      </c>
+      <c r="AH24">
+        <v>1.1783199049999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" s="13"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="9">
+        <f t="shared" ref="D25:D29" si="89">W25/1000</f>
+        <v>433.09521759999996</v>
+      </c>
+      <c r="E25" s="3">
+        <f t="shared" si="78"/>
+        <v>58.790011310000004</v>
+      </c>
+      <c r="F25" s="5">
+        <f t="shared" si="79"/>
+        <v>1.3331798450000001</v>
+      </c>
+      <c r="G25" s="9">
+        <f t="shared" si="80"/>
+        <v>117.58002259999999</v>
+      </c>
+      <c r="H25" s="5">
+        <f t="shared" si="81"/>
+        <v>1.3331798450000001</v>
+      </c>
+      <c r="I25" s="9">
+        <f t="shared" si="82"/>
+        <v>2563.867326</v>
+      </c>
+      <c r="J25" s="5">
+        <f t="shared" si="83"/>
+        <v>1.176643659</v>
+      </c>
+      <c r="K25" s="9">
+        <f t="shared" si="84"/>
+        <v>369.71672150000001</v>
+      </c>
+      <c r="L25" s="5">
+        <f t="shared" si="85"/>
+        <v>1.1742739099999999</v>
+      </c>
+      <c r="M25" s="7">
+        <f t="shared" si="86"/>
+        <v>0.95624048620000002</v>
+      </c>
+      <c r="N25" s="5">
+        <f t="shared" si="87"/>
+        <v>1.2927281690000001</v>
+      </c>
+      <c r="O25" s="7">
+        <f>((SUM($K$3:$K$5)+ SUM($K$24:K25)) * 20 + (SUM($M$3:$M$5) + SUM($M$24:M25)) * 1000) /(SUM($G$3:$G$5) + SUM($G$24:G25))</f>
+        <v>86.477528849326731</v>
+      </c>
+      <c r="P25" s="7">
+        <f t="shared" ref="P25:P29" si="90">(K25 * 20 + M25 * 1000) /G25</f>
+        <v>71.020354746895578</v>
+      </c>
+      <c r="Q25" s="3">
+        <f t="shared" si="88"/>
+        <v>22.930208093770919</v>
+      </c>
+      <c r="S25" t="s">
+        <v>21</v>
+      </c>
+      <c r="T25" t="s">
+        <v>20</v>
+      </c>
+      <c r="U25" t="s">
+        <v>50</v>
+      </c>
+      <c r="V25">
+        <v>1508497</v>
+      </c>
+      <c r="W25">
+        <v>433095.21759999997</v>
+      </c>
+      <c r="X25">
+        <v>58790.011310000002</v>
+      </c>
+      <c r="Y25">
+        <v>117580.0226</v>
+      </c>
+      <c r="Z25">
+        <v>-2563.867326</v>
+      </c>
+      <c r="AA25">
+        <v>-956240.48620000004</v>
+      </c>
+      <c r="AB25">
+        <v>369.71672150000001</v>
+      </c>
+      <c r="AC25">
+        <v>98.826585320000007</v>
+      </c>
+      <c r="AD25">
+        <v>1.3331798450000001</v>
+      </c>
+      <c r="AE25">
+        <v>1.3331798450000001</v>
+      </c>
+      <c r="AF25">
+        <v>1.176643659</v>
+      </c>
+      <c r="AG25">
+        <v>1.1742739099999999</v>
+      </c>
+      <c r="AH25">
+        <v>1.2927281690000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26" s="13" t="str">
+        <f>T26</f>
+        <v>[85,90)</v>
+      </c>
+      <c r="C26" s="12">
+        <f>V26/1000</f>
+        <v>940.56899999999996</v>
+      </c>
+      <c r="D26" s="9">
+        <f t="shared" si="89"/>
+        <v>344.41771729999999</v>
+      </c>
+      <c r="E26" s="3">
+        <f t="shared" si="78"/>
+        <v>46.752586210000004</v>
+      </c>
+      <c r="F26" s="5">
+        <f t="shared" si="79"/>
+        <v>1.4092509559999999</v>
+      </c>
+      <c r="G26" s="9">
+        <f t="shared" si="80"/>
+        <v>93.50517241</v>
+      </c>
+      <c r="H26" s="5">
+        <f t="shared" si="81"/>
+        <v>1.4092509559999999</v>
+      </c>
+      <c r="I26" s="9">
+        <f t="shared" si="82"/>
+        <v>1774.8333439999999</v>
+      </c>
+      <c r="J26" s="5">
+        <f t="shared" si="83"/>
+        <v>1.215680281</v>
+      </c>
+      <c r="K26" s="9">
+        <f t="shared" si="84"/>
+        <v>167.63179439999999</v>
+      </c>
+      <c r="L26" s="5">
+        <f t="shared" si="85"/>
+        <v>1.2043478910000001</v>
+      </c>
+      <c r="M26" s="7">
+        <f t="shared" si="86"/>
+        <v>0.49919508740000001</v>
+      </c>
+      <c r="N26" s="5">
+        <f t="shared" si="87"/>
+        <v>1.3524537759999999</v>
+      </c>
+      <c r="O26" s="7">
+        <f>((SUM($K$3:$K$5)+ SUM($K$24:K26)) * 20 + (SUM($M$3:$M$5) + SUM($M$24:M26)) * 1000) /(SUM($G$3:$G$5) + SUM($G$24:G26))</f>
+        <v>84.033120016453452</v>
+      </c>
+      <c r="P26" s="7">
+        <f t="shared" si="90"/>
+        <v>41.193774377641404</v>
+      </c>
+      <c r="Q26" s="3">
+        <f t="shared" si="88"/>
+        <v>26.341958453762299</v>
+      </c>
+      <c r="S26" t="s">
+        <v>22</v>
+      </c>
+      <c r="T26" t="s">
+        <v>23</v>
+      </c>
+      <c r="U26" t="s">
+        <v>66</v>
+      </c>
+      <c r="V26">
+        <v>940569</v>
+      </c>
+      <c r="W26">
+        <v>344417.71730000002</v>
+      </c>
+      <c r="X26">
+        <v>46752.586210000001</v>
+      </c>
+      <c r="Y26">
+        <v>93505.172409999999</v>
+      </c>
+      <c r="Z26">
+        <v>-1774.8333439999999</v>
+      </c>
+      <c r="AA26">
+        <v>-499195.08740000002</v>
+      </c>
+      <c r="AB26">
+        <v>167.63179439999999</v>
+      </c>
+      <c r="AC26">
+        <v>98.307529489999993</v>
+      </c>
+      <c r="AD26">
+        <v>1.4092509559999999</v>
+      </c>
+      <c r="AE26">
+        <v>1.4092509559999999</v>
+      </c>
+      <c r="AF26">
+        <v>1.215680281</v>
+      </c>
+      <c r="AG26">
+        <v>1.2043478910000001</v>
+      </c>
+      <c r="AH26">
+        <v>1.3524537759999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27" s="13"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="9">
+        <f t="shared" si="89"/>
+        <v>596.15128270000002</v>
+      </c>
+      <c r="E27" s="3">
+        <f t="shared" si="78"/>
+        <v>80.92386900999999</v>
+      </c>
+      <c r="F27" s="5">
+        <f t="shared" si="79"/>
+        <v>1.540922144</v>
+      </c>
+      <c r="G27" s="9">
+        <f t="shared" si="80"/>
+        <v>161.84773800000002</v>
+      </c>
+      <c r="H27" s="5">
+        <f t="shared" si="81"/>
+        <v>1.540922144</v>
+      </c>
+      <c r="I27" s="9">
+        <f t="shared" si="82"/>
+        <v>2719.1285039999998</v>
+      </c>
+      <c r="J27" s="5">
+        <f t="shared" si="83"/>
+        <v>1.2754862309999999</v>
+      </c>
+      <c r="K27" s="9">
+        <f t="shared" si="84"/>
+        <v>411.53066580000001</v>
+      </c>
+      <c r="L27" s="5">
+        <f t="shared" si="85"/>
+        <v>1.278178547</v>
+      </c>
+      <c r="M27" s="7">
+        <f t="shared" si="86"/>
+        <v>1.2944099339999999</v>
+      </c>
+      <c r="N27" s="5">
+        <f t="shared" si="87"/>
+        <v>1.507321924</v>
+      </c>
+      <c r="O27" s="7">
+        <f>((SUM($K$3:$K$5)+ SUM($K$24:K27)) * 20 + (SUM($M$3:$M$5) + SUM($M$24:M27)) * 1000) /(SUM($G$3:$G$5) + SUM($G$24:G27))</f>
+        <v>81.881382238423981</v>
+      </c>
+      <c r="P27" s="7">
+        <f t="shared" si="90"/>
+        <v>58.851753924419995</v>
+      </c>
+      <c r="Q27" s="3">
+        <f t="shared" si="88"/>
+        <v>29.760957928599613</v>
+      </c>
+      <c r="S27" t="s">
+        <v>24</v>
+      </c>
+      <c r="T27" t="s">
+        <v>23</v>
+      </c>
+      <c r="U27" t="s">
+        <v>50</v>
+      </c>
+      <c r="V27">
+        <v>940569</v>
+      </c>
+      <c r="W27">
+        <v>596151.28269999998</v>
+      </c>
+      <c r="X27">
+        <v>80923.869009999995</v>
+      </c>
+      <c r="Y27">
+        <v>161847.73800000001</v>
+      </c>
+      <c r="Z27">
+        <v>-2719.1285039999998</v>
+      </c>
+      <c r="AA27">
+        <v>-1294409.9339999999</v>
+      </c>
+      <c r="AB27">
+        <v>411.53066580000001</v>
+      </c>
+      <c r="AC27">
+        <v>99.312633689999998</v>
+      </c>
+      <c r="AD27">
+        <v>1.540922144</v>
+      </c>
+      <c r="AE27">
+        <v>1.540922144</v>
+      </c>
+      <c r="AF27">
+        <v>1.2754862309999999</v>
+      </c>
+      <c r="AG27">
+        <v>1.278178547</v>
+      </c>
+      <c r="AH27">
+        <v>1.507321924</v>
+      </c>
+    </row>
+    <row r="28" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" s="10" t="str">
+        <f>T28</f>
+        <v>[90,95)</v>
+      </c>
+      <c r="C28" s="11">
+        <f>V28/1000</f>
+        <v>417.13799999999998</v>
+      </c>
+      <c r="D28" s="9">
+        <f t="shared" si="89"/>
+        <v>417.13799999999998</v>
+      </c>
+      <c r="E28" s="3">
+        <f t="shared" si="78"/>
+        <v>56.623917200000001</v>
+      </c>
+      <c r="F28" s="5">
+        <f t="shared" si="79"/>
+        <v>1.6330548920000001</v>
+      </c>
+      <c r="G28" s="9">
+        <f t="shared" si="80"/>
+        <v>113.2478344</v>
+      </c>
+      <c r="H28" s="5">
+        <f t="shared" si="81"/>
+        <v>1.6330548920000001</v>
+      </c>
+      <c r="I28" s="9">
+        <f t="shared" si="82"/>
+        <v>1398.2286690000001</v>
+      </c>
+      <c r="J28" s="5">
+        <f t="shared" si="83"/>
+        <v>1.3062396110000001</v>
+      </c>
+      <c r="K28" s="9">
+        <f t="shared" si="84"/>
+        <v>215.06649110000001</v>
+      </c>
+      <c r="L28" s="5">
+        <f t="shared" si="85"/>
+        <v>1.3167625489999999</v>
+      </c>
+      <c r="M28" s="7">
+        <f t="shared" si="86"/>
+        <v>0.78007425760000004</v>
+      </c>
+      <c r="N28" s="5">
+        <f t="shared" si="87"/>
+        <v>1.600652988</v>
+      </c>
+      <c r="O28" s="7">
+        <f>((SUM($K$3:$K$5)+ SUM($K$24:K28)) * 20 + (SUM($M$3:$M$5) + SUM($M$24:M28)) * 1000) /(SUM($G$3:$G$5) + SUM($G$24:G28))</f>
+        <v>79.793282362512144</v>
+      </c>
+      <c r="P28" s="7">
+        <f t="shared" si="90"/>
+        <v>44.869768208123894</v>
+      </c>
+      <c r="Q28" s="3">
+        <f t="shared" si="88"/>
+        <v>40.49689328748844</v>
+      </c>
+      <c r="S28" t="s">
+        <v>24</v>
+      </c>
+      <c r="T28" t="s">
+        <v>25</v>
+      </c>
+      <c r="U28" t="s">
+        <v>50</v>
+      </c>
+      <c r="V28">
+        <v>417138</v>
+      </c>
+      <c r="W28">
+        <v>417138</v>
+      </c>
+      <c r="X28">
+        <v>56623.917200000004</v>
+      </c>
+      <c r="Y28">
+        <v>113247.83440000001</v>
+      </c>
+      <c r="Z28">
+        <v>-1398.2286690000001</v>
+      </c>
+      <c r="AA28">
+        <v>-780074.25760000001</v>
+      </c>
+      <c r="AB28">
+        <v>215.06649110000001</v>
+      </c>
+      <c r="AC28">
+        <v>98.97766317</v>
+      </c>
+      <c r="AD28">
+        <v>1.6330548920000001</v>
+      </c>
+      <c r="AE28">
+        <v>1.6330548920000001</v>
+      </c>
+      <c r="AF28">
+        <v>1.3062396110000001</v>
+      </c>
+      <c r="AG28">
+        <v>1.3167625489999999</v>
+      </c>
+      <c r="AH28">
+        <v>1.600652988</v>
+      </c>
+    </row>
+    <row r="29" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29" s="10" t="str">
+        <f>T29</f>
+        <v>[95,100)</v>
+      </c>
+      <c r="C29" s="11">
+        <f>V29/1000</f>
+        <v>109.06399999999999</v>
+      </c>
+      <c r="D29" s="9">
+        <f t="shared" si="89"/>
+        <v>109.06399999999999</v>
+      </c>
+      <c r="E29" s="3">
+        <f t="shared" si="78"/>
+        <v>14.80476702</v>
+      </c>
+      <c r="F29" s="5">
+        <f t="shared" si="79"/>
+        <v>1.657143721</v>
+      </c>
+      <c r="G29" s="9">
+        <f t="shared" si="80"/>
+        <v>29.60953404</v>
+      </c>
+      <c r="H29" s="5">
+        <f t="shared" si="81"/>
+        <v>1.657143721</v>
+      </c>
+      <c r="I29" s="9">
+        <f t="shared" si="82"/>
+        <v>234.88374920000001</v>
+      </c>
+      <c r="J29" s="5">
+        <f t="shared" si="83"/>
+        <v>1.311405768</v>
+      </c>
+      <c r="K29" s="9">
+        <f t="shared" si="84"/>
+        <v>34.359355489999999</v>
+      </c>
+      <c r="L29" s="5">
+        <f t="shared" si="85"/>
+        <v>1.322926789</v>
+      </c>
+      <c r="M29" s="7">
+        <f t="shared" si="86"/>
+        <v>0.1299733076</v>
+      </c>
+      <c r="N29" s="5">
+        <f t="shared" si="87"/>
+        <v>1.616203491</v>
+      </c>
+      <c r="O29" s="7">
+        <f>((SUM($K$3:$K$5)+ SUM($K$24:K29)) * 20 + (SUM($M$3:$M$5) + SUM($M$24:M29)) * 1000) /(SUM($G$3:$G$5) + SUM($G$24:G29))</f>
+        <v>79.034551494472225</v>
+      </c>
+      <c r="P29" s="7">
+        <f t="shared" si="90"/>
+        <v>27.597881692298319</v>
+      </c>
+      <c r="Q29" s="3">
+        <f t="shared" si="88"/>
+        <v>63.030188637673525</v>
+      </c>
+      <c r="S29" t="s">
+        <v>56</v>
+      </c>
+      <c r="T29" t="s">
+        <v>55</v>
+      </c>
+      <c r="U29" t="s">
+        <v>50</v>
+      </c>
+      <c r="V29">
+        <v>109064</v>
+      </c>
+      <c r="W29">
+        <v>109064</v>
+      </c>
+      <c r="X29">
+        <v>14804.767019999999</v>
+      </c>
+      <c r="Y29">
+        <v>29609.534039999999</v>
+      </c>
+      <c r="Z29">
+        <v>-234.88374920000001</v>
+      </c>
+      <c r="AA29">
+        <v>-129973.3076</v>
+      </c>
+      <c r="AB29">
+        <v>34.359355489999999</v>
+      </c>
+      <c r="AC29">
+        <v>98.58075024</v>
+      </c>
+      <c r="AD29">
+        <v>1.657143721</v>
+      </c>
+      <c r="AE29">
+        <v>1.657143721</v>
+      </c>
+      <c r="AF29">
+        <v>1.311405768</v>
+      </c>
+      <c r="AG29">
+        <v>1.322926789</v>
+      </c>
+      <c r="AH29">
+        <v>1.616203491</v>
+      </c>
+    </row>
+    <row r="31" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A31" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="B31" s="14"/>
+      <c r="C31" s="14"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="14"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="14"/>
+      <c r="I31" s="14"/>
+      <c r="J31" s="14"/>
+      <c r="K31" s="14"/>
+      <c r="L31" s="14"/>
+      <c r="M31" s="14"/>
+      <c r="N31" s="14"/>
+      <c r="O31" s="14"/>
+      <c r="P31" s="7"/>
+      <c r="Q31" s="3"/>
+    </row>
+    <row r="32" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>30</v>
+      </c>
+      <c r="B32" s="13" t="str">
+        <f>T32</f>
+        <v>[80,85)</v>
+      </c>
+      <c r="C32" s="12">
+        <f>V32/1000</f>
+        <v>1508.4970000000001</v>
+      </c>
+      <c r="D32" s="9">
+        <f>W32/1000</f>
+        <v>1075.4017824339201</v>
+      </c>
+      <c r="E32" s="3">
+        <f t="shared" ref="E32:E37" si="91">X32 / 1000</f>
+        <v>256.661789483196</v>
+      </c>
+      <c r="F32" s="5">
+        <f t="shared" ref="F32:F37" si="92">AD32</f>
+        <v>1.4176142732588399</v>
+      </c>
+      <c r="G32" s="9">
+        <f t="shared" ref="G32:G37" si="93">Y32 / 1000</f>
+        <v>513.32357896639303</v>
+      </c>
+      <c r="H32" s="5">
+        <f t="shared" ref="H32:H37" si="94">AE32</f>
+        <v>1.4176142732588399</v>
+      </c>
+      <c r="I32" s="9">
+        <f t="shared" ref="I32:I37" si="95">-Z32</f>
+        <v>9869.6693576464895</v>
+      </c>
+      <c r="J32" s="5">
+        <f t="shared" ref="J32:J37" si="96">AF32</f>
+        <v>1.2170787234020499</v>
+      </c>
+      <c r="K32" s="9">
+        <f t="shared" ref="K32:K37" si="97">AB32</f>
+        <v>1093.2241011594599</v>
+      </c>
+      <c r="L32" s="5">
+        <f t="shared" ref="L32:L37" si="98">AG32</f>
+        <v>1.19612986147641</v>
+      </c>
+      <c r="M32" s="7">
+        <f t="shared" ref="M32:M37" si="99">-AA32/1000000</f>
+        <v>2.6035075538759598</v>
+      </c>
+      <c r="N32" s="5">
+        <f t="shared" ref="N32:N37" si="100">AH32</f>
+        <v>1.3114935881152701</v>
+      </c>
+      <c r="O32" s="7">
+        <f>((SUM($K$3:$K$5)+ SUM($K$32:K32)) * 20 + (SUM($M$3:$M$5) + SUM($M$32:M32)) * 1000) /(SUM($G$3:$G$5) + SUM($G$32:G32))</f>
+        <v>82.815127872061908</v>
+      </c>
+      <c r="P32" s="7">
+        <f>(K32 * 20 + M32 * 1000) /G32</f>
+        <v>47.665820507082259</v>
+      </c>
+      <c r="Q32" s="3">
+        <f t="shared" ref="Q32:Q37" si="101">E32/I32*1000</f>
+        <v>26.005105154241893</v>
+      </c>
+      <c r="S32" t="s">
+        <v>19</v>
+      </c>
+      <c r="T32" t="s">
+        <v>20</v>
+      </c>
+      <c r="U32" t="s">
+        <v>66</v>
+      </c>
+      <c r="V32">
+        <v>1508497</v>
+      </c>
+      <c r="W32">
+        <v>1075401.7824339201</v>
+      </c>
+      <c r="X32">
+        <v>256661.78948319599</v>
+      </c>
+      <c r="Y32">
+        <v>513323.57896639302</v>
+      </c>
+      <c r="Z32">
+        <v>-9869.6693576464895</v>
+      </c>
+      <c r="AA32">
+        <v>-2603507.5538759599</v>
+      </c>
+      <c r="AB32">
+        <v>1093.2241011594599</v>
+      </c>
+      <c r="AC32">
+        <v>97.120461780647304</v>
+      </c>
+      <c r="AD32">
+        <v>1.4176142732588399</v>
+      </c>
+      <c r="AE32">
+        <v>1.4176142732588399</v>
+      </c>
+      <c r="AF32">
+        <v>1.2170787234020499</v>
+      </c>
+      <c r="AG32">
+        <v>1.19612986147641</v>
+      </c>
+      <c r="AH32">
+        <v>1.3114935881152701</v>
+      </c>
+    </row>
+    <row r="33" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>31</v>
+      </c>
+      <c r="B33" s="13"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="9">
+        <f t="shared" ref="D33:D37" si="102">W33/1000</f>
+        <v>433.09521756606995</v>
+      </c>
+      <c r="E33" s="3">
+        <f t="shared" si="91"/>
+        <v>76.705702678003306</v>
+      </c>
+      <c r="F33" s="5">
+        <f t="shared" si="92"/>
+        <v>1.54242208490538</v>
+      </c>
+      <c r="G33" s="9">
+        <f t="shared" si="93"/>
+        <v>153.41140535600599</v>
+      </c>
+      <c r="H33" s="5">
+        <f t="shared" si="94"/>
+        <v>1.54242208490538</v>
+      </c>
+      <c r="I33" s="9">
+        <f t="shared" si="95"/>
+        <v>3427.5937526859798</v>
+      </c>
+      <c r="J33" s="5">
+        <f t="shared" si="96"/>
+        <v>1.29246703168387</v>
+      </c>
+      <c r="K33" s="9">
+        <f t="shared" si="97"/>
+        <v>490.93811708074998</v>
+      </c>
+      <c r="L33" s="5">
+        <f t="shared" si="98"/>
+        <v>1.28420661060261</v>
+      </c>
+      <c r="M33" s="7">
+        <f t="shared" si="99"/>
+        <v>1.23929642624046</v>
+      </c>
+      <c r="N33" s="5">
+        <f t="shared" si="100"/>
+        <v>1.45976774617307</v>
+      </c>
+      <c r="O33" s="7">
+        <f>((SUM($K$3:$K$5)+ SUM($K$32:K33)) * 20 + (SUM($M$3:$M$5) + SUM($M$32:M33)) * 1000) /(SUM($G$3:$G$5) + SUM($G$32:G33))</f>
+        <v>81.946562864145406</v>
+      </c>
+      <c r="P33" s="7">
+        <f t="shared" ref="P33:P37" si="103">(K33 * 20 + M33 * 1000) /G33</f>
+        <v>72.081073386911271</v>
+      </c>
+      <c r="Q33" s="3">
+        <f t="shared" si="101"/>
+        <v>22.378878073836518</v>
+      </c>
+      <c r="S33" t="s">
+        <v>21</v>
+      </c>
+      <c r="T33" t="s">
+        <v>20</v>
+      </c>
+      <c r="U33" t="s">
+        <v>50</v>
+      </c>
+      <c r="V33">
+        <v>1508497</v>
+      </c>
+      <c r="W33">
+        <v>433095.21756606997</v>
+      </c>
+      <c r="X33">
+        <v>76705.702678003305</v>
+      </c>
+      <c r="Y33">
+        <v>153411.405356006</v>
+      </c>
+      <c r="Z33">
+        <v>-3427.5937526859798</v>
+      </c>
+      <c r="AA33">
+        <v>-1239296.42624046</v>
+      </c>
+      <c r="AB33">
+        <v>490.93811708074998</v>
+      </c>
+      <c r="AC33">
+        <v>99.429743860527694</v>
+      </c>
+      <c r="AD33">
+        <v>1.54242208490538</v>
+      </c>
+      <c r="AE33">
+        <v>1.54242208490538</v>
+      </c>
+      <c r="AF33">
+        <v>1.29246703168387</v>
+      </c>
+      <c r="AG33">
+        <v>1.28420661060261</v>
+      </c>
+      <c r="AH33">
+        <v>1.45976774617307</v>
+      </c>
+    </row>
+    <row r="34" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>30</v>
+      </c>
+      <c r="B34" s="13" t="str">
+        <f>T34</f>
+        <v>[85,90)</v>
+      </c>
+      <c r="C34" s="12">
+        <f>V34/1000</f>
+        <v>940.56899999999996</v>
+      </c>
+      <c r="D34" s="9">
+        <f t="shared" si="102"/>
+        <v>344.41771727378898</v>
+      </c>
+      <c r="E34" s="3">
+        <f t="shared" si="91"/>
+        <v>46.752586205033197</v>
+      </c>
+      <c r="F34" s="5">
+        <f t="shared" si="92"/>
+        <v>1.61849319525765</v>
+      </c>
+      <c r="G34" s="9">
+        <f t="shared" si="93"/>
+        <v>93.505172410066507</v>
+      </c>
+      <c r="H34" s="5">
+        <f t="shared" si="94"/>
+        <v>1.61849319525765</v>
+      </c>
+      <c r="I34" s="9">
+        <f t="shared" si="95"/>
+        <v>1774.83334438626</v>
+      </c>
+      <c r="J34" s="5">
+        <f t="shared" si="96"/>
+        <v>1.3315036541571701</v>
+      </c>
+      <c r="K34" s="9">
+        <f t="shared" si="97"/>
+        <v>167.63179439661999</v>
+      </c>
+      <c r="L34" s="5">
+        <f t="shared" si="98"/>
+        <v>1.3142805913895099</v>
+      </c>
+      <c r="M34" s="7">
+        <f t="shared" si="99"/>
+        <v>0.49919508742090102</v>
+      </c>
+      <c r="N34" s="5">
+        <f t="shared" si="100"/>
+        <v>1.5194933531599799</v>
+      </c>
+      <c r="O34" s="7">
+        <f>((SUM($K$3:$K$5)+ SUM($K$32:K34)) * 20 + (SUM($M$3:$M$5) + SUM($M$32:M34)) * 1000) /(SUM($G$3:$G$5) + SUM($G$32:G34))</f>
+        <v>80.03113320448216</v>
+      </c>
+      <c r="P34" s="7">
+        <f t="shared" si="103"/>
+        <v>41.193774377112675</v>
+      </c>
+      <c r="Q34" s="3">
+        <f t="shared" si="101"/>
+        <v>26.341958445230986</v>
+      </c>
+      <c r="S34" t="s">
+        <v>22</v>
+      </c>
+      <c r="T34" t="s">
+        <v>23</v>
+      </c>
+      <c r="U34" t="s">
+        <v>66</v>
+      </c>
+      <c r="V34">
+        <v>940569</v>
+      </c>
+      <c r="W34">
+        <v>344417.71727378899</v>
+      </c>
+      <c r="X34">
+        <v>46752.5862050332</v>
+      </c>
+      <c r="Y34">
+        <v>93505.172410066501</v>
+      </c>
+      <c r="Z34">
+        <v>-1774.83334438626</v>
+      </c>
+      <c r="AA34">
+        <v>-499195.08742090099</v>
+      </c>
+      <c r="AB34">
+        <v>167.63179439661999</v>
+      </c>
+      <c r="AC34">
+        <v>98.934642820385903</v>
+      </c>
+      <c r="AD34">
+        <v>1.61849319525765</v>
+      </c>
+      <c r="AE34">
+        <v>1.61849319525765</v>
+      </c>
+      <c r="AF34">
+        <v>1.3315036541571701</v>
+      </c>
+      <c r="AG34">
+        <v>1.3142805913895099</v>
+      </c>
+      <c r="AH34">
+        <v>1.5194933531599799</v>
+      </c>
+    </row>
+    <row r="35" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>31</v>
+      </c>
+      <c r="B35" s="13"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="9">
+        <f t="shared" si="102"/>
+        <v>596.15128272620996</v>
+      </c>
+      <c r="E35" s="3">
+        <f t="shared" si="91"/>
+        <v>80.923869008580112</v>
+      </c>
+      <c r="F35" s="5">
+        <f t="shared" si="92"/>
+        <v>1.7501643832960401</v>
+      </c>
+      <c r="G35" s="9">
+        <f t="shared" si="93"/>
+        <v>161.84773801716</v>
+      </c>
+      <c r="H35" s="5">
+        <f t="shared" si="94"/>
+        <v>1.7501643832960401</v>
+      </c>
+      <c r="I35" s="9">
+        <f t="shared" si="95"/>
+        <v>2719.1285037150701</v>
+      </c>
+      <c r="J35" s="5">
+        <f t="shared" si="96"/>
+        <v>1.3913096033701799</v>
+      </c>
+      <c r="K35" s="9">
+        <f t="shared" si="97"/>
+        <v>411.530665807768</v>
+      </c>
+      <c r="L35" s="5">
+        <f t="shared" si="98"/>
+        <v>1.38811124732965</v>
+      </c>
+      <c r="M35" s="7">
+        <f t="shared" si="99"/>
+        <v>1.2944099341038802</v>
+      </c>
+      <c r="N35" s="5">
+        <f t="shared" si="100"/>
+        <v>1.6743615018103699</v>
+      </c>
+      <c r="O35" s="7">
+        <f>((SUM($K$3:$K$5)+ SUM($K$32:K35)) * 20 + (SUM($M$3:$M$5) + SUM($M$32:M35)) * 1000) /(SUM($G$3:$G$5) + SUM($G$32:G35))</f>
+        <v>78.437732002316082</v>
+      </c>
+      <c r="P35" s="7">
+        <f t="shared" si="103"/>
+        <v>58.85175391978197</v>
+      </c>
+      <c r="Q35" s="3">
+        <f t="shared" si="101"/>
+        <v>29.760957931195993</v>
+      </c>
+      <c r="S35" t="s">
+        <v>24</v>
+      </c>
+      <c r="T35" t="s">
+        <v>23</v>
+      </c>
+      <c r="U35" t="s">
+        <v>50</v>
+      </c>
+      <c r="V35">
+        <v>940569</v>
+      </c>
+      <c r="W35">
+        <v>596151.28272620996</v>
+      </c>
+      <c r="X35">
+        <v>80923.869008580106</v>
+      </c>
+      <c r="Y35">
+        <v>161847.73801716001</v>
+      </c>
+      <c r="Z35">
+        <v>-2719.1285037150701</v>
+      </c>
+      <c r="AA35">
+        <v>-1294409.9341038801</v>
+      </c>
+      <c r="AB35">
+        <v>411.530665807768</v>
+      </c>
+      <c r="AC35">
+        <v>99.833250470974903</v>
+      </c>
+      <c r="AD35">
+        <v>1.7501643832960401</v>
+      </c>
+      <c r="AE35">
+        <v>1.7501643832960401</v>
+      </c>
+      <c r="AF35">
+        <v>1.3913096033701799</v>
+      </c>
+      <c r="AG35">
+        <v>1.38811124732965</v>
+      </c>
+      <c r="AH35">
+        <v>1.6743615018103699</v>
+      </c>
+    </row>
+    <row r="36" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>31</v>
+      </c>
+      <c r="B36" s="10" t="str">
+        <f>T36</f>
+        <v>[90,95)</v>
+      </c>
+      <c r="C36" s="11">
+        <f>V36/1000</f>
+        <v>417.13799999999998</v>
+      </c>
+      <c r="D36" s="9">
+        <f t="shared" si="102"/>
+        <v>417.13799999999998</v>
+      </c>
+      <c r="E36" s="3">
+        <f t="shared" si="91"/>
+        <v>56.6239171978836</v>
+      </c>
+      <c r="F36" s="5">
+        <f t="shared" si="92"/>
+        <v>1.8422971315219401</v>
+      </c>
+      <c r="G36" s="9">
+        <f t="shared" si="93"/>
+        <v>113.247834395767</v>
+      </c>
+      <c r="H36" s="5">
+        <f t="shared" si="94"/>
+        <v>1.8422971315219401</v>
+      </c>
+      <c r="I36" s="9">
+        <f t="shared" si="95"/>
+        <v>1398.2286690972801</v>
+      </c>
+      <c r="J36" s="5">
+        <f t="shared" si="96"/>
+        <v>1.4220629836013701</v>
+      </c>
+      <c r="K36" s="9">
+        <f t="shared" si="97"/>
+        <v>215.06649113910299</v>
+      </c>
+      <c r="L36" s="5">
+        <f t="shared" si="98"/>
+        <v>1.4266952495215099</v>
+      </c>
+      <c r="M36" s="7">
+        <f t="shared" si="99"/>
+        <v>0.78007425764216398</v>
+      </c>
+      <c r="N36" s="5">
+        <f t="shared" si="100"/>
+        <v>1.76769256556994</v>
+      </c>
+      <c r="O36" s="7">
+        <f>((SUM($K$3:$K$5)+ SUM($K$32:K36)) * 20 + (SUM($M$3:$M$5) + SUM($M$32:M36)) * 1000) /(SUM($G$3:$G$5) + SUM($G$32:G36))</f>
+        <v>76.759007814472241</v>
+      </c>
+      <c r="P36" s="7">
+        <f t="shared" si="103"/>
+        <v>44.869768217079098</v>
+      </c>
+      <c r="Q36" s="3">
+        <f t="shared" si="101"/>
+        <v>40.496893283157291</v>
+      </c>
+      <c r="S36" t="s">
+        <v>24</v>
+      </c>
+      <c r="T36" t="s">
+        <v>25</v>
+      </c>
+      <c r="U36" t="s">
+        <v>50</v>
+      </c>
+      <c r="V36">
+        <v>417138</v>
+      </c>
+      <c r="W36">
+        <v>417138</v>
+      </c>
+      <c r="X36">
+        <v>56623.917197883602</v>
+      </c>
+      <c r="Y36">
+        <v>113247.834395767</v>
+      </c>
+      <c r="Z36">
+        <v>-1398.2286690972801</v>
+      </c>
+      <c r="AA36">
+        <v>-780074.25764216401</v>
+      </c>
+      <c r="AB36">
+        <v>215.06649113910299</v>
+      </c>
+      <c r="AC36">
+        <v>99.506063843051805</v>
+      </c>
+      <c r="AD36">
+        <v>1.8422971315219401</v>
+      </c>
+      <c r="AE36">
+        <v>1.8422971315219401</v>
+      </c>
+      <c r="AF36">
+        <v>1.4220629836013701</v>
+      </c>
+      <c r="AG36">
+        <v>1.4266952495215099</v>
+      </c>
+      <c r="AH36">
+        <v>1.76769256556994</v>
+      </c>
+    </row>
+    <row r="37" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>31</v>
+      </c>
+      <c r="B37" s="10" t="str">
+        <f>T37</f>
+        <v>[95,100)</v>
+      </c>
+      <c r="C37" s="11">
+        <f>V37/1000</f>
+        <v>109.06399999999999</v>
+      </c>
+      <c r="D37" s="9">
+        <f t="shared" si="102"/>
+        <v>109.06399999999999</v>
+      </c>
+      <c r="E37" s="3">
+        <f t="shared" si="91"/>
+        <v>14.804767020194701</v>
+      </c>
+      <c r="F37" s="5">
+        <f t="shared" si="92"/>
+        <v>1.8663859607643201</v>
+      </c>
+      <c r="G37" s="9">
+        <f t="shared" si="93"/>
+        <v>29.609534040389402</v>
+      </c>
+      <c r="H37" s="5">
+        <f t="shared" si="94"/>
+        <v>1.8663859607643201</v>
+      </c>
+      <c r="I37" s="9">
+        <f t="shared" si="95"/>
+        <v>234.88374918093501</v>
+      </c>
+      <c r="J37" s="5">
+        <f t="shared" si="96"/>
+        <v>1.42722914090335</v>
+      </c>
+      <c r="K37" s="9">
+        <f t="shared" si="97"/>
+        <v>34.359355486366802</v>
+      </c>
+      <c r="L37" s="5">
+        <f t="shared" si="98"/>
+        <v>1.43285948942879</v>
+      </c>
+      <c r="M37" s="7">
+        <f t="shared" si="99"/>
+        <v>0.12997330756768199</v>
+      </c>
+      <c r="N37" s="5">
+        <f t="shared" si="100"/>
+        <v>1.78324306853398</v>
+      </c>
+      <c r="O37" s="7">
+        <f>((SUM($K$3:$K$5)+ SUM($K$32:K37)) * 20 + (SUM($M$3:$M$5) + SUM($M$32:M37)) * 1000) /(SUM($G$3:$G$5) + SUM($G$32:G37))</f>
+        <v>76.124501341797369</v>
+      </c>
+      <c r="P37" s="7">
+        <f t="shared" si="103"/>
+        <v>27.597881688389833</v>
+      </c>
+      <c r="Q37" s="3">
+        <f t="shared" si="101"/>
+        <v>63.03018864361848</v>
+      </c>
+      <c r="S37" t="s">
+        <v>56</v>
+      </c>
+      <c r="T37" t="s">
+        <v>55</v>
+      </c>
+      <c r="U37" t="s">
+        <v>50</v>
+      </c>
+      <c r="V37">
+        <v>109064</v>
+      </c>
+      <c r="W37">
+        <v>109064</v>
+      </c>
+      <c r="X37">
+        <v>14804.7670201947</v>
+      </c>
+      <c r="Y37">
+        <v>29609.534040389401</v>
+      </c>
+      <c r="Z37">
+        <v>-234.88374918093501</v>
+      </c>
+      <c r="AA37">
+        <v>-129973.307567682</v>
+      </c>
+      <c r="AB37">
+        <v>34.359355486366802</v>
+      </c>
+      <c r="AC37">
+        <v>99.133684381171506</v>
+      </c>
+      <c r="AD37">
+        <v>1.8663859607643201</v>
+      </c>
+      <c r="AE37">
+        <v>1.8663859607643201</v>
+      </c>
+      <c r="AF37">
+        <v>1.42722914090335</v>
+      </c>
+      <c r="AG37">
+        <v>1.43285948942879</v>
+      </c>
+      <c r="AH37">
+        <v>1.78324306853398</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="A7:O7"/>
-    <mergeCell ref="A4:A5"/>
+  <mergeCells count="26">
+    <mergeCell ref="A31:O31"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="A23:O23"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="A15:O15"/>
     <mergeCell ref="M1:N1"/>
     <mergeCell ref="K1:L1"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="C8:C9"/>
     <mergeCell ref="I1:J1"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="A15:O15"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="A7:O7"/>
+    <mergeCell ref="A4:A5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2620,7 +4063,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F782D18A-8F87-4860-9C5B-20DBEF4FE7B3}">
   <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
@@ -2645,22 +4088,22 @@
       <c r="D1" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16" t="s">
+      <c r="F1" s="17"/>
+      <c r="G1" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16" t="s">
+      <c r="H1" s="17"/>
+      <c r="I1" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="J1" s="16"/>
-      <c r="K1" s="15" t="s">
+      <c r="J1" s="17"/>
+      <c r="K1" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="L1" s="15"/>
+      <c r="L1" s="16"/>
       <c r="M1" s="6" t="s">
         <v>38</v>
       </c>
@@ -2701,13 +4144,13 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="20" t="s">
         <v>59</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="19" t="s">
         <v>61</v>
       </c>
       <c r="D3" s="9">
@@ -2742,11 +4185,11 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="19"/>
+      <c r="A4" s="20"/>
       <c r="B4" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="20"/>
+      <c r="C4" s="19"/>
       <c r="D4" s="9">
         <v>1053.4762497747899</v>
       </c>
@@ -2779,11 +4222,11 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="19"/>
+      <c r="A5" s="20"/>
       <c r="B5" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="20"/>
+      <c r="C5" s="19"/>
       <c r="D5" s="9">
         <v>474.26387725610499</v>
       </c>
@@ -2850,10 +4293,10 @@
       <c r="A8" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="20" t="s">
+      <c r="C8" s="19" t="s">
         <v>62</v>
       </c>
       <c r="D8" s="9">
@@ -2891,8 +4334,8 @@
       <c r="A9" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="12"/>
-      <c r="C9" s="20"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="19"/>
       <c r="D9" s="9">
         <v>433.09521756606995</v>
       </c>
@@ -2928,10 +4371,10 @@
       <c r="A10" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="20"/>
+      <c r="C10" s="19"/>
       <c r="D10" s="9">
         <v>344.41771727378898</v>
       </c>
@@ -2967,8 +4410,8 @@
       <c r="A11" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="12"/>
-      <c r="C11" s="20"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="19"/>
       <c r="D11" s="9">
         <v>596.15128272620996</v>
       </c>
@@ -3007,7 +4450,7 @@
       <c r="B12" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="20"/>
+      <c r="C12" s="19"/>
       <c r="D12" s="9">
         <v>417.13799999999998</v>
       </c>
@@ -3046,7 +4489,7 @@
       <c r="B13" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="C13" s="20"/>
+      <c r="C13" s="19"/>
       <c r="D13" s="9">
         <v>109.06399999999999</v>
       </c>
@@ -3111,10 +4554,10 @@
       <c r="A16" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="20" t="s">
+      <c r="C16" s="19" t="s">
         <v>62</v>
       </c>
       <c r="D16" s="9">
@@ -3152,8 +4595,8 @@
       <c r="A17" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="12"/>
-      <c r="C17" s="20"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="19"/>
       <c r="D17" s="9">
         <v>433.09521756606995</v>
       </c>
@@ -3189,10 +4632,10 @@
       <c r="A18" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="12" t="s">
+      <c r="B18" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="20"/>
+      <c r="C18" s="19"/>
       <c r="D18" s="9">
         <v>344.41771727378898</v>
       </c>
@@ -3228,8 +4671,8 @@
       <c r="A19" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="12"/>
-      <c r="C19" s="20"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="19"/>
       <c r="D19" s="9">
         <v>596.15128272620996</v>
       </c>
@@ -3268,7 +4711,7 @@
       <c r="B20" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C20" s="20"/>
+      <c r="C20" s="19"/>
       <c r="D20" s="9">
         <v>417.13799999999998</v>
       </c>
@@ -3307,7 +4750,7 @@
       <c r="B21" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="C21" s="20"/>
+      <c r="C21" s="19"/>
       <c r="D21" s="9">
         <v>109.06399999999999</v>
       </c>
@@ -3341,6 +4784,10 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="K1:L1"/>
     <mergeCell ref="C16:C21"/>
     <mergeCell ref="C3:C5"/>
     <mergeCell ref="A3:A5"/>
@@ -3351,10 +4798,6 @@
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="A15:M15"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="K1:L1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>